<commit_message>
models updated to latest version
</commit_message>
<xml_diff>
--- a/models/ard-arm-cardiac/source/ard-arm-cardiac.xlsx
+++ b/models/ard-arm-cardiac/source/ard-arm-cardiac.xlsx
@@ -11,8 +11,9 @@
     <sheet state="visible" name="nodes" sheetId="6" r:id="rId9"/>
     <sheet state="visible" name="groups" sheetId="7" r:id="rId10"/>
     <sheet state="visible" name="publications" sheetId="8" r:id="rId11"/>
-    <sheet state="visible" name="localConventions" sheetId="9" r:id="rId12"/>
-    <sheet state="visible" name="neurons" sheetId="10" r:id="rId13"/>
+    <sheet state="visible" name="contributors" sheetId="9" r:id="rId12"/>
+    <sheet state="visible" name="localConventions" sheetId="10" r:id="rId13"/>
+    <sheet state="visible" name="neurons" sheetId="11" r:id="rId14"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -50,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2330" uniqueCount="1345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2345" uniqueCount="1357">
   <si>
     <t>id</t>
   </si>
@@ -3889,6 +3890,42 @@
   </si>
   <si>
     <t>Review of Neurocardiology: Structure-Based Function</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>Jeffrey Ardell</t>
+  </si>
+  <si>
+    <t>Still awaiting permission</t>
+  </si>
+  <si>
+    <t>Drew Armor</t>
+  </si>
+  <si>
+    <t>need to send email for permission</t>
+  </si>
+  <si>
+    <t>Peter Hunter</t>
+  </si>
+  <si>
+    <t>https://orcid.org/0000-0003-0638-5274</t>
+  </si>
+  <si>
+    <t>Bernard de Bono</t>
+  </si>
+  <si>
+    <t>https://orcid.org/0000-0002-2308-8813</t>
+  </si>
+  <si>
+    <t>Monique Surles-Zeigler</t>
+  </si>
+  <si>
+    <t>https://orcid.org/0000-0002-7509-4801</t>
+  </si>
+  <si>
+    <t>Thomas H Gillespie</t>
   </si>
   <si>
     <t>prefix</t>
@@ -4093,7 +4130,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="30">
+  <fonts count="31">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -4174,10 +4211,6 @@
       <name val="Arial"/>
     </font>
     <font>
-      <name val="Arial"/>
-    </font>
-    <font/>
-    <font>
       <b/>
       <sz val="9.0"/>
       <color rgb="FF008000"/>
@@ -4191,6 +4224,15 @@
     <font>
       <color theme="1"/>
       <name val="Droid Sans Mono"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
+    </font>
+    <font/>
+    <font>
+      <sz val="10.0"/>
+      <color rgb="FF000000"/>
     </font>
     <font>
       <u/>
@@ -4309,7 +4351,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="161">
+  <cellXfs count="158">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -4687,9 +4729,6 @@
     <xf borderId="0" fillId="8" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="16" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
     <xf borderId="0" fillId="8" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
@@ -4702,23 +4741,8 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
     <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="16" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
@@ -4732,7 +4756,7 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -4744,35 +4768,44 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="24" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="25" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="25" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="26" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="26" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="27" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="27" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="28" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -4781,10 +4814,10 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="28" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="30" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4800,6 +4833,10 @@
 </file>
 
 <file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -5082,19 +5119,164 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="2" max="2" width="39.29"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>1291</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1292</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="147" t="s">
+        <v>1293</v>
+      </c>
+      <c r="B2" s="148" t="s">
+        <v>1294</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="147" t="s">
+        <v>1295</v>
+      </c>
+      <c r="B3" s="149" t="s">
+        <v>1296</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="147" t="s">
+        <v>1297</v>
+      </c>
+      <c r="B4" s="150" t="s">
+        <v>1298</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="147" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B5" s="150" t="s">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="147" t="s">
+        <v>1301</v>
+      </c>
+      <c r="B6" s="150" t="s">
+        <v>1302</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="147" t="s">
+        <v>1303</v>
+      </c>
+      <c r="B7" s="150" t="s">
+        <v>1304</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="147" t="s">
+        <v>1305</v>
+      </c>
+      <c r="B8" s="150" t="s">
+        <v>1306</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="147" t="s">
+        <v>1307</v>
+      </c>
+      <c r="B9" s="150" t="s">
+        <v>1308</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="147" t="s">
+        <v>1309</v>
+      </c>
+      <c r="B10" s="150" t="s">
+        <v>1310</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="147" t="s">
+        <v>1311</v>
+      </c>
+      <c r="B11" s="150" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="5" t="s">
+        <v>1313</v>
+      </c>
+      <c r="B12" s="151" t="s">
+        <v>1314</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="26" t="s">
+        <v>1315</v>
+      </c>
+      <c r="B13" s="152" t="s">
+        <v>1316</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="26" t="s">
+        <v>1317</v>
+      </c>
+      <c r="B14" s="153" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="B2"/>
+    <hyperlink r:id="rId2" ref="B3"/>
+    <hyperlink r:id="rId3" ref="B4"/>
+    <hyperlink r:id="rId4" ref="B5"/>
+    <hyperlink r:id="rId5" ref="B6"/>
+    <hyperlink r:id="rId6" ref="B7"/>
+    <hyperlink r:id="rId7" ref="B8"/>
+    <hyperlink r:id="rId8" ref="B9"/>
+    <hyperlink r:id="rId9" ref="B10"/>
+    <hyperlink r:id="rId10" ref="B11"/>
+    <hyperlink r:id="rId11" ref="B12"/>
+    <hyperlink r:id="rId12" ref="B13"/>
+    <hyperlink r:id="rId13" ref="B14"/>
+  </hyperlinks>
+  <drawing r:id="rId14"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
       <c r="A1" s="17" t="s">
-        <v>1307</v>
+        <v>1319</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>1308</v>
+        <v>1320</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>1309</v>
+        <v>1321</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>1310</v>
+        <v>1322</v>
       </c>
       <c r="E1" s="17"/>
       <c r="F1" s="17"/>
@@ -5110,13 +5292,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>1311</v>
+        <v>1323</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>1312</v>
+        <v>1324</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>1313</v>
+        <v>1325</v>
       </c>
       <c r="E2" s="17"/>
       <c r="F2" s="17"/>
@@ -5157,13 +5339,13 @@
     </row>
     <row r="5">
       <c r="A5" s="17" t="s">
-        <v>1314</v>
+        <v>1326</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>1315</v>
+        <v>1327</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>1316</v>
+        <v>1328</v>
       </c>
       <c r="D5" s="17"/>
       <c r="E5" s="17"/>
@@ -5180,10 +5362,10 @@
         <v>0</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>1317</v>
+        <v>1329</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>1318</v>
+        <v>1330</v>
       </c>
       <c r="D6" s="17"/>
       <c r="E6" s="17"/>
@@ -5198,10 +5380,10 @@
     <row r="7">
       <c r="A7" s="17"/>
       <c r="B7" s="17" t="s">
-        <v>1319</v>
+        <v>1331</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>1318</v>
+        <v>1330</v>
       </c>
       <c r="D7" s="17"/>
       <c r="E7" s="17"/>
@@ -5216,10 +5398,10 @@
     <row r="8">
       <c r="A8" s="17"/>
       <c r="B8" s="17" t="s">
-        <v>1320</v>
+        <v>1332</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>1318</v>
+        <v>1330</v>
       </c>
       <c r="D8" s="17"/>
       <c r="E8" s="17"/>
@@ -5234,10 +5416,10 @@
     <row r="9">
       <c r="A9" s="17"/>
       <c r="B9" s="17" t="s">
-        <v>1321</v>
+        <v>1333</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>1318</v>
+        <v>1330</v>
       </c>
       <c r="D9" s="17"/>
       <c r="E9" s="17"/>
@@ -5265,10 +5447,10 @@
     </row>
     <row r="11">
       <c r="A11" s="17" t="s">
-        <v>1322</v>
+        <v>1334</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>1323</v>
+        <v>1335</v>
       </c>
       <c r="C11" s="17"/>
       <c r="D11" s="17"/>
@@ -5283,10 +5465,10 @@
     </row>
     <row r="12">
       <c r="A12" s="17" t="s">
-        <v>1324</v>
-      </c>
-      <c r="B12" s="157" t="s">
-        <v>1325</v>
+        <v>1336</v>
+      </c>
+      <c r="B12" s="154" t="s">
+        <v>1337</v>
       </c>
       <c r="C12" s="17"/>
       <c r="D12" s="17"/>
@@ -5301,10 +5483,10 @@
     </row>
     <row r="13">
       <c r="A13" s="17" t="s">
-        <v>1326</v>
-      </c>
-      <c r="B13" s="157" t="s">
-        <v>1327</v>
+        <v>1338</v>
+      </c>
+      <c r="B13" s="154" t="s">
+        <v>1339</v>
       </c>
       <c r="C13" s="17"/>
       <c r="D13" s="17"/>
@@ -5319,10 +5501,10 @@
     </row>
     <row r="14">
       <c r="A14" s="17" t="s">
-        <v>1328</v>
-      </c>
-      <c r="B14" s="157" t="s">
-        <v>1329</v>
+        <v>1340</v>
+      </c>
+      <c r="B14" s="154" t="s">
+        <v>1341</v>
       </c>
       <c r="C14" s="17"/>
       <c r="D14" s="17"/>
@@ -5337,10 +5519,10 @@
     </row>
     <row r="15">
       <c r="A15" s="17" t="s">
-        <v>1330</v>
-      </c>
-      <c r="B15" s="157" t="s">
-        <v>1331</v>
+        <v>1342</v>
+      </c>
+      <c r="B15" s="154" t="s">
+        <v>1343</v>
       </c>
       <c r="C15" s="17"/>
       <c r="D15" s="17"/>
@@ -5369,10 +5551,10 @@
     </row>
     <row r="17">
       <c r="A17" s="17" t="s">
-        <v>1332</v>
+        <v>1344</v>
       </c>
       <c r="B17" s="49" t="s">
-        <v>1333</v>
+        <v>1345</v>
       </c>
       <c r="C17" s="17"/>
       <c r="D17" s="17"/>
@@ -5387,28 +5569,28 @@
     </row>
     <row r="18">
       <c r="A18" s="17" t="s">
-        <v>1334</v>
+        <v>1346</v>
       </c>
       <c r="B18" s="92" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="158"/>
-      <c r="D18" s="158"/>
-      <c r="E18" s="158"/>
-      <c r="F18" s="158"/>
-      <c r="G18" s="158"/>
-      <c r="H18" s="158"/>
-      <c r="I18" s="158"/>
-      <c r="J18" s="158"/>
-      <c r="K18" s="158"/>
+      <c r="C18" s="155"/>
+      <c r="D18" s="155"/>
+      <c r="E18" s="155"/>
+      <c r="F18" s="155"/>
+      <c r="G18" s="155"/>
+      <c r="H18" s="155"/>
+      <c r="I18" s="155"/>
+      <c r="J18" s="155"/>
+      <c r="K18" s="155"/>
       <c r="L18" s="17"/>
     </row>
     <row r="19">
       <c r="A19" s="17" t="s">
-        <v>1335</v>
+        <v>1347</v>
       </c>
       <c r="B19" s="92" t="s">
-        <v>1336</v>
+        <v>1348</v>
       </c>
       <c r="L19" s="17"/>
     </row>
@@ -5437,65 +5619,65 @@
       <c r="L25" s="17"/>
     </row>
     <row r="26">
-      <c r="A26" s="158" t="s">
-        <v>1337</v>
-      </c>
-      <c r="B26" s="159" t="s">
-        <v>1338</v>
+      <c r="A26" s="155" t="s">
+        <v>1349</v>
+      </c>
+      <c r="B26" s="156" t="s">
+        <v>1350</v>
       </c>
       <c r="L26" s="17"/>
     </row>
     <row r="27">
-      <c r="A27" s="158" t="s">
-        <v>1339</v>
-      </c>
-      <c r="B27" s="160" t="s">
-        <v>1340</v>
+      <c r="A27" s="155" t="s">
+        <v>1351</v>
+      </c>
+      <c r="B27" s="157" t="s">
+        <v>1352</v>
       </c>
       <c r="L27" s="17"/>
     </row>
     <row r="28">
-      <c r="A28" s="158" t="s">
-        <v>1341</v>
-      </c>
-      <c r="B28" s="154" t="s">
-        <v>1342</v>
-      </c>
-      <c r="C28" s="159"/>
-      <c r="D28" s="159"/>
-      <c r="E28" s="159"/>
-      <c r="F28" s="159"/>
-      <c r="G28" s="159"/>
-      <c r="H28" s="159"/>
-      <c r="I28" s="159"/>
-      <c r="J28" s="159"/>
-      <c r="K28" s="159"/>
+      <c r="A28" s="155" t="s">
+        <v>1353</v>
+      </c>
+      <c r="B28" s="151" t="s">
+        <v>1354</v>
+      </c>
+      <c r="C28" s="156"/>
+      <c r="D28" s="156"/>
+      <c r="E28" s="156"/>
+      <c r="F28" s="156"/>
+      <c r="G28" s="156"/>
+      <c r="H28" s="156"/>
+      <c r="I28" s="156"/>
+      <c r="J28" s="156"/>
+      <c r="K28" s="156"/>
       <c r="L28" s="17"/>
     </row>
     <row r="29" hidden="1">
       <c r="A29" s="17" t="s">
-        <v>1343</v>
+        <v>1355</v>
       </c>
       <c r="L29" s="17"/>
     </row>
     <row r="30" hidden="1">
       <c r="A30" s="17" t="s">
-        <v>1344</v>
+        <v>1356</v>
       </c>
       <c r="L30" s="17"/>
     </row>
     <row r="31">
       <c r="A31" s="17"/>
-      <c r="B31" s="158"/>
-      <c r="C31" s="158"/>
-      <c r="D31" s="158"/>
-      <c r="E31" s="158"/>
-      <c r="F31" s="158"/>
-      <c r="G31" s="158"/>
-      <c r="H31" s="158"/>
-      <c r="I31" s="158"/>
-      <c r="J31" s="158"/>
-      <c r="K31" s="158"/>
+      <c r="B31" s="155"/>
+      <c r="C31" s="155"/>
+      <c r="D31" s="155"/>
+      <c r="E31" s="155"/>
+      <c r="F31" s="155"/>
+      <c r="G31" s="155"/>
+      <c r="H31" s="155"/>
+      <c r="I31" s="155"/>
+      <c r="J31" s="155"/>
+      <c r="K31" s="155"/>
       <c r="L31" s="17"/>
     </row>
   </sheetData>
@@ -15998,7 +16180,7 @@
         <v>742</v>
       </c>
       <c r="D110" s="26"/>
-      <c r="E110" s="127" t="s">
+      <c r="E110" s="25" t="s">
         <v>350</v>
       </c>
       <c r="F110" s="14" t="s">
@@ -16029,7 +16211,7 @@
         <v>742</v>
       </c>
       <c r="D111" s="122"/>
-      <c r="E111" s="128" t="s">
+      <c r="E111" s="127" t="s">
         <v>350</v>
       </c>
       <c r="F111" s="123" t="s">
@@ -16041,7 +16223,7 @@
       <c r="H111" s="124"/>
       <c r="I111" s="125"/>
       <c r="J111" s="125"/>
-      <c r="K111" s="129" t="s">
+      <c r="K111" s="128" t="s">
         <v>920</v>
       </c>
       <c r="L111" s="126" t="s">
@@ -16060,7 +16242,7 @@
         <v>742</v>
       </c>
       <c r="D112" s="122"/>
-      <c r="E112" s="128" t="s">
+      <c r="E112" s="127" t="s">
         <v>350</v>
       </c>
       <c r="F112" s="123" t="s">
@@ -16072,7 +16254,7 @@
       <c r="H112" s="124"/>
       <c r="I112" s="125"/>
       <c r="J112" s="125"/>
-      <c r="K112" s="129" t="s">
+      <c r="K112" s="128" t="s">
         <v>925</v>
       </c>
       <c r="L112" s="126" t="s">
@@ -16091,7 +16273,7 @@
         <v>742</v>
       </c>
       <c r="D113" s="122"/>
-      <c r="E113" s="128" t="s">
+      <c r="E113" s="127" t="s">
         <v>350</v>
       </c>
       <c r="F113" s="123" t="s">
@@ -16103,7 +16285,7 @@
       <c r="H113" s="124"/>
       <c r="I113" s="125"/>
       <c r="J113" s="125"/>
-      <c r="K113" s="129" t="s">
+      <c r="K113" s="128" t="s">
         <v>920</v>
       </c>
       <c r="L113" s="126" t="s">
@@ -16199,7 +16381,7 @@
       <c r="K116" s="93">
         <v>0.0</v>
       </c>
-      <c r="L116" s="130" t="s">
+      <c r="L116" s="129" t="s">
         <v>287</v>
       </c>
       <c r="M116" s="17"/>
@@ -16739,7 +16921,7 @@
         <v>742</v>
       </c>
       <c r="D134" s="26"/>
-      <c r="E134" s="127" t="s">
+      <c r="E134" s="25" t="s">
         <v>350</v>
       </c>
       <c r="F134" s="14" t="s">
@@ -16801,7 +16983,7 @@
         <v>742</v>
       </c>
       <c r="D136" s="26"/>
-      <c r="E136" s="127" t="s">
+      <c r="E136" s="25" t="s">
         <v>350</v>
       </c>
       <c r="F136" s="5" t="s">
@@ -16894,7 +17076,7 @@
         <v>739</v>
       </c>
       <c r="D139" s="26"/>
-      <c r="E139" s="127" t="s">
+      <c r="E139" s="25" t="s">
         <v>360</v>
       </c>
       <c r="F139" s="14" t="s">
@@ -16924,7 +17106,7 @@
       <c r="C140" s="106" t="s">
         <v>742</v>
       </c>
-      <c r="D140" s="131"/>
+      <c r="D140" s="130"/>
       <c r="E140" s="25" t="s">
         <v>350</v>
       </c>
@@ -16955,8 +17137,8 @@
       <c r="C141" s="106" t="s">
         <v>739</v>
       </c>
-      <c r="D141" s="131"/>
-      <c r="E141" s="127" t="s">
+      <c r="D141" s="130"/>
+      <c r="E141" s="25" t="s">
         <v>360</v>
       </c>
       <c r="F141" s="14" t="s">
@@ -16986,7 +17168,7 @@
       <c r="C142" s="106" t="s">
         <v>742</v>
       </c>
-      <c r="D142" s="131"/>
+      <c r="D142" s="130"/>
       <c r="E142" s="25" t="s">
         <v>350</v>
       </c>
@@ -17011,14 +17193,14 @@
       <c r="A143" s="25" t="s">
         <v>1175</v>
       </c>
-      <c r="B143" s="132" t="s">
+      <c r="B143" s="14" t="s">
         <v>1176</v>
       </c>
       <c r="C143" s="106" t="s">
         <v>739</v>
       </c>
-      <c r="D143" s="131"/>
-      <c r="E143" s="127" t="s">
+      <c r="D143" s="130"/>
+      <c r="E143" s="25" t="s">
         <v>360</v>
       </c>
       <c r="F143" s="14" t="s">
@@ -17042,13 +17224,13 @@
       <c r="A144" s="25" t="s">
         <v>1177</v>
       </c>
-      <c r="B144" s="132" t="s">
+      <c r="B144" s="14" t="s">
         <v>1178</v>
       </c>
       <c r="C144" s="106" t="s">
         <v>742</v>
       </c>
-      <c r="D144" s="131"/>
+      <c r="D144" s="130"/>
       <c r="E144" s="25" t="s">
         <v>350</v>
       </c>
@@ -17073,14 +17255,14 @@
       <c r="A145" s="25" t="s">
         <v>1181</v>
       </c>
-      <c r="B145" s="132" t="s">
+      <c r="B145" s="14" t="s">
         <v>1182</v>
       </c>
       <c r="C145" s="106" t="s">
         <v>739</v>
       </c>
-      <c r="D145" s="131"/>
-      <c r="E145" s="127" t="s">
+      <c r="D145" s="130"/>
+      <c r="E145" s="25" t="s">
         <v>360</v>
       </c>
       <c r="F145" s="14" t="s">
@@ -17104,13 +17286,13 @@
       <c r="A146" s="42" t="s">
         <v>1183</v>
       </c>
-      <c r="B146" s="133" t="s">
+      <c r="B146" s="37" t="s">
         <v>1184</v>
       </c>
       <c r="C146" s="104" t="s">
         <v>742</v>
       </c>
-      <c r="D146" s="134"/>
+      <c r="D146" s="131"/>
       <c r="E146" s="42" t="s">
         <v>350</v>
       </c>
@@ -17135,14 +17317,14 @@
       <c r="A147" s="25" t="s">
         <v>1187</v>
       </c>
-      <c r="B147" s="132" t="s">
+      <c r="B147" s="14" t="s">
         <v>1188</v>
       </c>
       <c r="C147" s="106" t="s">
         <v>739</v>
       </c>
-      <c r="D147" s="131"/>
-      <c r="E147" s="127" t="s">
+      <c r="D147" s="130"/>
+      <c r="E147" s="25" t="s">
         <v>360</v>
       </c>
       <c r="F147" s="14" t="s">
@@ -17166,13 +17348,13 @@
       <c r="A148" s="42" t="s">
         <v>1189</v>
       </c>
-      <c r="B148" s="133" t="s">
+      <c r="B148" s="37" t="s">
         <v>1190</v>
       </c>
       <c r="C148" s="104" t="s">
         <v>742</v>
       </c>
-      <c r="D148" s="134"/>
+      <c r="D148" s="131"/>
       <c r="E148" s="42" t="s">
         <v>350</v>
       </c>
@@ -17203,8 +17385,8 @@
       <c r="C149" s="106" t="s">
         <v>739</v>
       </c>
-      <c r="D149" s="131"/>
-      <c r="E149" s="127" t="s">
+      <c r="D149" s="130"/>
+      <c r="E149" s="25" t="s">
         <v>360</v>
       </c>
       <c r="F149" s="14" t="s">
@@ -17228,20 +17410,20 @@
       <c r="A150" s="42" t="s">
         <v>1195</v>
       </c>
-      <c r="B150" s="133" t="s">
+      <c r="B150" s="37" t="s">
         <v>1196</v>
       </c>
       <c r="C150" s="104" t="s">
         <v>742</v>
       </c>
-      <c r="D150" s="134"/>
+      <c r="D150" s="131"/>
       <c r="E150" s="42" t="s">
         <v>350</v>
       </c>
       <c r="F150" s="37" t="s">
         <v>713</v>
       </c>
-      <c r="G150" s="135" t="s">
+      <c r="G150" s="98" t="s">
         <v>1197</v>
       </c>
       <c r="H150" s="44"/>
@@ -17259,20 +17441,20 @@
       <c r="A151" s="25" t="s">
         <v>1199</v>
       </c>
-      <c r="B151" s="132" t="s">
+      <c r="B151" s="14" t="s">
         <v>1200</v>
       </c>
       <c r="C151" s="106" t="s">
         <v>739</v>
       </c>
-      <c r="D151" s="131"/>
-      <c r="E151" s="127" t="s">
+      <c r="D151" s="130"/>
+      <c r="E151" s="25" t="s">
         <v>360</v>
       </c>
       <c r="F151" s="14" t="s">
         <v>715</v>
       </c>
-      <c r="G151" s="136" t="s">
+      <c r="G151" s="5" t="s">
         <v>1163</v>
       </c>
       <c r="H151" s="13"/>
@@ -17290,20 +17472,20 @@
       <c r="A152" s="42" t="s">
         <v>1201</v>
       </c>
-      <c r="B152" s="133" t="s">
+      <c r="B152" s="37" t="s">
         <v>1202</v>
       </c>
       <c r="C152" s="104" t="s">
         <v>742</v>
       </c>
-      <c r="D152" s="134"/>
+      <c r="D152" s="131"/>
       <c r="E152" s="42" t="s">
         <v>350</v>
       </c>
       <c r="F152" s="37" t="s">
         <v>716</v>
       </c>
-      <c r="G152" s="135" t="s">
+      <c r="G152" s="98" t="s">
         <v>1203</v>
       </c>
       <c r="H152" s="44"/>
@@ -17321,14 +17503,14 @@
       <c r="A153" s="25" t="s">
         <v>1205</v>
       </c>
-      <c r="B153" s="132" t="s">
+      <c r="B153" s="14" t="s">
         <v>1206</v>
       </c>
       <c r="C153" s="106" t="s">
         <v>739</v>
       </c>
-      <c r="D153" s="131"/>
-      <c r="E153" s="127" t="s">
+      <c r="D153" s="130"/>
+      <c r="E153" s="25" t="s">
         <v>360</v>
       </c>
       <c r="F153" s="14" t="s">
@@ -17352,20 +17534,20 @@
       <c r="A154" s="42" t="s">
         <v>1207</v>
       </c>
-      <c r="B154" s="133" t="s">
+      <c r="B154" s="37" t="s">
         <v>1208</v>
       </c>
       <c r="C154" s="104" t="s">
         <v>742</v>
       </c>
-      <c r="D154" s="134"/>
+      <c r="D154" s="131"/>
       <c r="E154" s="42" t="s">
         <v>350</v>
       </c>
       <c r="F154" s="37" t="s">
         <v>719</v>
       </c>
-      <c r="G154" s="135" t="s">
+      <c r="G154" s="98" t="s">
         <v>1209</v>
       </c>
       <c r="H154" s="44"/>
@@ -17383,14 +17565,14 @@
       <c r="A155" s="25" t="s">
         <v>1211</v>
       </c>
-      <c r="B155" s="132" t="s">
+      <c r="B155" s="14" t="s">
         <v>1212</v>
       </c>
       <c r="C155" s="106" t="s">
         <v>739</v>
       </c>
-      <c r="D155" s="131"/>
-      <c r="E155" s="127" t="s">
+      <c r="D155" s="130"/>
+      <c r="E155" s="25" t="s">
         <v>360</v>
       </c>
       <c r="F155" s="14" t="s">
@@ -17414,20 +17596,20 @@
       <c r="A156" s="42" t="s">
         <v>1213</v>
       </c>
-      <c r="B156" s="133" t="s">
+      <c r="B156" s="37" t="s">
         <v>1214</v>
       </c>
       <c r="C156" s="104" t="s">
         <v>742</v>
       </c>
-      <c r="D156" s="134"/>
+      <c r="D156" s="131"/>
       <c r="E156" s="42" t="s">
         <v>350</v>
       </c>
       <c r="F156" s="37" t="s">
         <v>722</v>
       </c>
-      <c r="G156" s="135" t="s">
+      <c r="G156" s="98" t="s">
         <v>1215</v>
       </c>
       <c r="H156" s="44"/>
@@ -17442,7 +17624,7 @@
       <c r="M156" s="54"/>
     </row>
     <row r="157">
-      <c r="A157" s="137" t="s">
+      <c r="A157" s="42" t="s">
         <v>1217</v>
       </c>
       <c r="B157" s="37" t="s">
@@ -17451,14 +17633,14 @@
       <c r="C157" s="104" t="s">
         <v>739</v>
       </c>
-      <c r="D157" s="134"/>
+      <c r="D157" s="131"/>
       <c r="E157" s="40" t="s">
         <v>360</v>
       </c>
-      <c r="F157" s="135" t="s">
+      <c r="F157" s="98" t="s">
         <v>1163</v>
       </c>
-      <c r="G157" s="138" t="s">
+      <c r="G157" s="132" t="s">
         <v>701</v>
       </c>
       <c r="H157" s="44"/>
@@ -17473,7 +17655,7 @@
       <c r="M157" s="54"/>
     </row>
     <row r="158">
-      <c r="A158" s="137" t="s">
+      <c r="A158" s="42" t="s">
         <v>1219</v>
       </c>
       <c r="B158" s="37" t="s">
@@ -17482,7 +17664,7 @@
       <c r="C158" s="104" t="s">
         <v>739</v>
       </c>
-      <c r="D158" s="134"/>
+      <c r="D158" s="131"/>
       <c r="E158" s="55" t="s">
         <v>357</v>
       </c>
@@ -17504,7 +17686,7 @@
       <c r="M158" s="54"/>
     </row>
     <row r="159">
-      <c r="A159" s="137" t="s">
+      <c r="A159" s="42" t="s">
         <v>1221</v>
       </c>
       <c r="B159" s="37" t="s">
@@ -17513,7 +17695,7 @@
       <c r="C159" s="104" t="s">
         <v>739</v>
       </c>
-      <c r="D159" s="134"/>
+      <c r="D159" s="131"/>
       <c r="E159" s="55" t="s">
         <v>357</v>
       </c>
@@ -17566,7 +17748,7 @@
       <c r="M160" s="54"/>
     </row>
     <row r="161">
-      <c r="A161" s="139" t="s">
+      <c r="A161" s="133" t="s">
         <v>1225</v>
       </c>
       <c r="B161" s="37" t="s">
@@ -17597,7 +17779,7 @@
       <c r="M161" s="54"/>
     </row>
     <row r="162">
-      <c r="A162" s="139" t="s">
+      <c r="A162" s="133" t="s">
         <v>1227</v>
       </c>
       <c r="B162" s="37" t="s">
@@ -17716,7 +17898,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="140" t="s">
+      <c r="A1" s="134" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -17725,19 +17907,19 @@
       <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="140" t="s">
+      <c r="D1" s="134" t="s">
         <v>723</v>
       </c>
-      <c r="E1" s="140" t="s">
+      <c r="E1" s="134" t="s">
         <v>1233</v>
       </c>
-      <c r="F1" s="140" t="s">
+      <c r="F1" s="134" t="s">
         <v>1234</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>1235</v>
       </c>
-      <c r="H1" s="141" t="s">
+      <c r="H1" s="135" t="s">
         <v>599</v>
       </c>
       <c r="I1" s="5" t="s">
@@ -17754,9 +17936,9 @@
       <c r="C2" s="5" t="s">
         <v>1238</v>
       </c>
-      <c r="D2" s="142"/>
-      <c r="F2" s="141"/>
-      <c r="H2" s="143"/>
+      <c r="D2" s="136"/>
+      <c r="F2" s="135"/>
+      <c r="H2" s="137"/>
     </row>
     <row r="3">
       <c r="A3" s="5" t="s">
@@ -17768,10 +17950,10 @@
       <c r="C3" s="5" t="s">
         <v>1240</v>
       </c>
-      <c r="D3" s="143"/>
-      <c r="E3" s="141"/>
-      <c r="F3" s="141"/>
-      <c r="H3" s="141"/>
+      <c r="D3" s="137"/>
+      <c r="E3" s="135"/>
+      <c r="F3" s="135"/>
+      <c r="H3" s="135"/>
     </row>
     <row r="4">
       <c r="A4" s="5" t="s">
@@ -17783,10 +17965,10 @@
       <c r="C4" s="5" t="s">
         <v>1242</v>
       </c>
-      <c r="D4" s="143"/>
-      <c r="E4" s="141"/>
-      <c r="F4" s="141"/>
-      <c r="H4" s="141"/>
+      <c r="D4" s="137"/>
+      <c r="E4" s="135"/>
+      <c r="F4" s="135"/>
+      <c r="H4" s="135"/>
     </row>
     <row r="5">
       <c r="A5" s="5" t="s">
@@ -17798,10 +17980,10 @@
       <c r="C5" s="5" t="s">
         <v>1244</v>
       </c>
-      <c r="D5" s="141"/>
-      <c r="E5" s="141"/>
-      <c r="F5" s="141"/>
-      <c r="H5" s="143"/>
+      <c r="D5" s="135"/>
+      <c r="E5" s="135"/>
+      <c r="F5" s="135"/>
+      <c r="H5" s="137"/>
     </row>
     <row r="6">
       <c r="A6" s="5" t="s">
@@ -17813,9 +17995,9 @@
       <c r="C6" s="5" t="s">
         <v>1246</v>
       </c>
-      <c r="D6" s="141"/>
+      <c r="D6" s="135"/>
       <c r="E6" s="92"/>
-      <c r="F6" s="144"/>
+      <c r="F6" s="138"/>
       <c r="H6" s="5" t="s">
         <v>1247</v>
       </c>
@@ -17830,10 +18012,10 @@
       <c r="C7" s="5" t="s">
         <v>1249</v>
       </c>
-      <c r="D7" s="141"/>
-      <c r="E7" s="141"/>
-      <c r="F7" s="141"/>
-      <c r="H7" s="141"/>
+      <c r="D7" s="135"/>
+      <c r="E7" s="135"/>
+      <c r="F7" s="135"/>
+      <c r="H7" s="135"/>
     </row>
     <row r="8">
       <c r="A8" s="5" t="s">
@@ -17845,11 +18027,11 @@
       <c r="C8" s="5" t="s">
         <v>1251</v>
       </c>
-      <c r="D8" s="141"/>
-      <c r="E8" s="141"/>
-      <c r="F8" s="141"/>
-      <c r="G8" s="141"/>
-      <c r="H8" s="141"/>
+      <c r="D8" s="135"/>
+      <c r="E8" s="135"/>
+      <c r="F8" s="135"/>
+      <c r="G8" s="135"/>
+      <c r="H8" s="135"/>
     </row>
     <row r="9">
       <c r="A9" s="5" t="s">
@@ -17861,10 +18043,10 @@
       <c r="C9" s="5" t="s">
         <v>1253</v>
       </c>
-      <c r="D9" s="141"/>
-      <c r="E9" s="141"/>
-      <c r="F9" s="141"/>
-      <c r="H9" s="141"/>
+      <c r="D9" s="135"/>
+      <c r="E9" s="135"/>
+      <c r="F9" s="135"/>
+      <c r="H9" s="135"/>
     </row>
     <row r="10">
       <c r="A10" s="5" t="s">
@@ -17876,10 +18058,10 @@
       <c r="C10" s="5" t="s">
         <v>1255</v>
       </c>
-      <c r="D10" s="141"/>
-      <c r="E10" s="141"/>
-      <c r="F10" s="141"/>
-      <c r="H10" s="143"/>
+      <c r="D10" s="135"/>
+      <c r="E10" s="135"/>
+      <c r="F10" s="135"/>
+      <c r="H10" s="137"/>
     </row>
     <row r="11">
       <c r="A11" s="5" t="s">
@@ -17891,17 +18073,17 @@
       <c r="C11" s="5" t="s">
         <v>1257</v>
       </c>
-      <c r="D11" s="141"/>
-      <c r="E11" s="141"/>
-      <c r="F11" s="141"/>
-      <c r="G11" s="141"/>
-      <c r="H11" s="141"/>
+      <c r="D11" s="135"/>
+      <c r="E11" s="135"/>
+      <c r="F11" s="135"/>
+      <c r="G11" s="135"/>
+      <c r="H11" s="135"/>
     </row>
     <row r="12">
-      <c r="D12" s="141"/>
-      <c r="E12" s="141"/>
-      <c r="F12" s="141"/>
-      <c r="H12" s="141"/>
+      <c r="D12" s="135"/>
+      <c r="E12" s="135"/>
+      <c r="F12" s="135"/>
+      <c r="H12" s="135"/>
     </row>
     <row r="13">
       <c r="A13" s="5" t="s">
@@ -17913,11 +18095,11 @@
       <c r="C13" s="5" t="s">
         <v>1259</v>
       </c>
-      <c r="D13" s="141"/>
-      <c r="E13" s="141"/>
-      <c r="F13" s="141"/>
-      <c r="G13" s="141"/>
-      <c r="H13" s="141"/>
+      <c r="D13" s="135"/>
+      <c r="E13" s="135"/>
+      <c r="F13" s="135"/>
+      <c r="G13" s="135"/>
+      <c r="H13" s="135"/>
     </row>
     <row r="14">
       <c r="A14" s="5" t="s">
@@ -17929,10 +18111,10 @@
       <c r="C14" s="5" t="s">
         <v>1261</v>
       </c>
-      <c r="D14" s="141"/>
-      <c r="E14" s="141"/>
-      <c r="F14" s="141"/>
-      <c r="H14" s="141"/>
+      <c r="D14" s="135"/>
+      <c r="E14" s="135"/>
+      <c r="F14" s="135"/>
+      <c r="H14" s="135"/>
     </row>
     <row r="15">
       <c r="A15" s="5" t="s">
@@ -17944,10 +18126,10 @@
       <c r="C15" s="5" t="s">
         <v>1263</v>
       </c>
-      <c r="D15" s="141"/>
-      <c r="E15" s="141"/>
-      <c r="F15" s="141"/>
-      <c r="H15" s="143"/>
+      <c r="D15" s="135"/>
+      <c r="E15" s="135"/>
+      <c r="F15" s="135"/>
+      <c r="H15" s="137"/>
     </row>
     <row r="16">
       <c r="A16" s="5" t="s">
@@ -17959,11 +18141,11 @@
       <c r="C16" s="5" t="s">
         <v>1265</v>
       </c>
-      <c r="D16" s="141"/>
-      <c r="E16" s="141"/>
-      <c r="F16" s="141"/>
-      <c r="G16" s="141"/>
-      <c r="H16" s="141"/>
+      <c r="D16" s="135"/>
+      <c r="E16" s="135"/>
+      <c r="F16" s="135"/>
+      <c r="G16" s="135"/>
+      <c r="H16" s="135"/>
     </row>
     <row r="17">
       <c r="A17" s="5" t="s">
@@ -17975,9 +18157,9 @@
       <c r="C17" s="5" t="s">
         <v>1267</v>
       </c>
-      <c r="D17" s="143"/>
-      <c r="E17" s="141"/>
-      <c r="F17" s="141"/>
+      <c r="D17" s="137"/>
+      <c r="E17" s="135"/>
+      <c r="F17" s="135"/>
       <c r="H17" s="5" t="s">
         <v>1247</v>
       </c>
@@ -17992,9 +18174,9 @@
       <c r="C18" s="5" t="s">
         <v>1269</v>
       </c>
-      <c r="E18" s="141"/>
-      <c r="F18" s="145"/>
-      <c r="H18" s="141"/>
+      <c r="E18" s="135"/>
+      <c r="F18" s="139"/>
+      <c r="H18" s="135"/>
     </row>
     <row r="19">
       <c r="A19" s="5" t="s">
@@ -18006,8 +18188,8 @@
       <c r="C19" s="5" t="s">
         <v>1271</v>
       </c>
-      <c r="E19" s="141"/>
-      <c r="F19" s="145"/>
+      <c r="E19" s="135"/>
+      <c r="F19" s="139"/>
       <c r="H19" s="5" t="s">
         <v>1247</v>
       </c>
@@ -18032,7 +18214,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="146" t="s">
+      <c r="A1" s="140" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -18044,19 +18226,19 @@
       <c r="D1" s="1" t="s">
         <v>1273</v>
       </c>
-      <c r="E1" s="147" t="s">
+      <c r="E1" s="141" t="s">
         <v>1274</v>
       </c>
-      <c r="F1" s="147" t="s">
+      <c r="F1" s="141" t="s">
         <v>1275</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="148" t="s">
+      <c r="A2" s="142" t="s">
         <v>1247</v>
       </c>
       <c r="B2" s="5"/>
-      <c r="C2" s="149" t="s">
+      <c r="C2" s="143" t="s">
         <v>1276</v>
       </c>
       <c r="D2" s="5"/>
@@ -18084,138 +18266,74 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
-  <cols>
-    <col customWidth="1" min="2" max="2" width="39.29"/>
-  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>1279</v>
       </c>
-      <c r="B1" s="1" t="s">
+    </row>
+    <row r="2">
+      <c r="B2" s="144" t="s">
         <v>1280</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="150" t="s">
+      <c r="C2" s="5" t="s">
         <v>1281</v>
       </c>
-      <c r="B2" s="151" t="s">
+    </row>
+    <row r="3">
+      <c r="A3" s="5"/>
+      <c r="B3" s="145" t="s">
         <v>1282</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="150" t="s">
+      <c r="C3" s="5" t="s">
         <v>1283</v>
       </c>
-      <c r="B3" s="152" t="s">
+    </row>
+    <row r="4">
+      <c r="A4" s="5"/>
+      <c r="B4" s="145" t="s">
         <v>1284</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="150" t="s">
+      <c r="C4" s="5" t="s">
+        <v>1283</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="146" t="s">
         <v>1285</v>
       </c>
-      <c r="B4" s="153" t="s">
+      <c r="B5" s="5" t="s">
         <v>1286</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="150" t="s">
+    <row r="6">
+      <c r="A6" s="146" t="s">
         <v>1287</v>
       </c>
-      <c r="B5" s="153" t="s">
+      <c r="B6" s="5" t="s">
         <v>1288</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="150" t="s">
+    <row r="7">
+      <c r="A7" s="146" t="s">
         <v>1289</v>
       </c>
-      <c r="B6" s="153" t="s">
+      <c r="B7" s="5" t="s">
         <v>1290</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="150" t="s">
-        <v>1291</v>
-      </c>
-      <c r="B7" s="153" t="s">
-        <v>1292</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="150" t="s">
-        <v>1293</v>
-      </c>
-      <c r="B8" s="153" t="s">
-        <v>1294</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="150" t="s">
-        <v>1295</v>
-      </c>
-      <c r="B9" s="153" t="s">
-        <v>1296</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="150" t="s">
-        <v>1297</v>
-      </c>
-      <c r="B10" s="153" t="s">
-        <v>1298</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="150" t="s">
-        <v>1299</v>
-      </c>
-      <c r="B11" s="153" t="s">
-        <v>1300</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="5" t="s">
-        <v>1301</v>
-      </c>
-      <c r="B12" s="154" t="s">
-        <v>1302</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="26" t="s">
-        <v>1303</v>
-      </c>
-      <c r="B13" s="155" t="s">
-        <v>1304</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="26" t="s">
-        <v>1305</v>
-      </c>
-      <c r="B14" s="156" t="s">
-        <v>1306</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="B2"/>
-    <hyperlink r:id="rId2" ref="B3"/>
-    <hyperlink r:id="rId3" ref="B4"/>
-    <hyperlink r:id="rId4" ref="B5"/>
-    <hyperlink r:id="rId5" ref="B6"/>
-    <hyperlink r:id="rId6" ref="B7"/>
-    <hyperlink r:id="rId7" ref="B8"/>
-    <hyperlink r:id="rId8" ref="B9"/>
-    <hyperlink r:id="rId9" ref="B10"/>
-    <hyperlink r:id="rId10" ref="B11"/>
-    <hyperlink r:id="rId11" ref="B12"/>
-    <hyperlink r:id="rId12" ref="B13"/>
-    <hyperlink r:id="rId13" ref="B14"/>
+    <hyperlink r:id="rId1" ref="A5"/>
+    <hyperlink r:id="rId2" ref="A6"/>
+    <hyperlink r:id="rId3" ref="A7"/>
   </hyperlinks>
-  <drawing r:id="rId14"/>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
aacar-9a fix axon terminal housing location
</commit_message>
<xml_diff>
--- a/models/ard-arm-cardiac/source/ard-arm-cardiac.xlsx
+++ b/models/ard-arm-cardiac/source/ard-arm-cardiac.xlsx
@@ -4428,7 +4428,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="23">
+  <fills count="24">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4539,6 +4539,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFCFE2F3"/>
+        <bgColor rgb="FFCFE2F3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor theme="8"/>
       </patternFill>
@@ -4591,7 +4597,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="271">
+  <cellXfs count="274">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -5155,6 +5161,15 @@
     <xf borderId="0" fillId="18" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="19" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="19" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="19" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="7" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
@@ -5197,7 +5212,7 @@
     <xf borderId="0" fillId="2" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="19" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="20" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -5209,7 +5224,7 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="20" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="21" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -5218,7 +5233,7 @@
     <xf borderId="0" fillId="9" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="21" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="22" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -5258,7 +5273,7 @@
     <xf borderId="0" fillId="0" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="22" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="23" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -5270,7 +5285,7 @@
     <xf borderId="0" fillId="0" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="22" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="23" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -5703,82 +5718,82 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="260" t="s">
+      <c r="A2" s="263" t="s">
         <v>1326</v>
       </c>
-      <c r="B2" s="261" t="s">
+      <c r="B2" s="264" t="s">
         <v>1327</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="260" t="s">
+      <c r="A3" s="263" t="s">
         <v>1328</v>
       </c>
-      <c r="B3" s="262" t="s">
+      <c r="B3" s="265" t="s">
         <v>1329</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="260" t="s">
+      <c r="A4" s="263" t="s">
         <v>1330</v>
       </c>
-      <c r="B4" s="263" t="s">
+      <c r="B4" s="266" t="s">
         <v>1331</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="260" t="s">
+      <c r="A5" s="263" t="s">
         <v>1332</v>
       </c>
-      <c r="B5" s="263" t="s">
+      <c r="B5" s="266" t="s">
         <v>1333</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="260" t="s">
+      <c r="A6" s="263" t="s">
         <v>1334</v>
       </c>
-      <c r="B6" s="263" t="s">
+      <c r="B6" s="266" t="s">
         <v>1335</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="260" t="s">
+      <c r="A7" s="263" t="s">
         <v>1336</v>
       </c>
-      <c r="B7" s="263" t="s">
+      <c r="B7" s="266" t="s">
         <v>1337</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="260" t="s">
+      <c r="A8" s="263" t="s">
         <v>1338</v>
       </c>
-      <c r="B8" s="263" t="s">
+      <c r="B8" s="266" t="s">
         <v>1339</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="260" t="s">
+      <c r="A9" s="263" t="s">
         <v>1340</v>
       </c>
-      <c r="B9" s="263" t="s">
+      <c r="B9" s="266" t="s">
         <v>1341</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="260" t="s">
+      <c r="A10" s="263" t="s">
         <v>1342</v>
       </c>
-      <c r="B10" s="263" t="s">
+      <c r="B10" s="266" t="s">
         <v>1343</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="260" t="s">
+      <c r="A11" s="263" t="s">
         <v>1344</v>
       </c>
-      <c r="B11" s="263" t="s">
+      <c r="B11" s="266" t="s">
         <v>1345</v>
       </c>
     </row>
@@ -5786,7 +5801,7 @@
       <c r="A12" s="5" t="s">
         <v>1346</v>
       </c>
-      <c r="B12" s="264" t="s">
+      <c r="B12" s="267" t="s">
         <v>1347</v>
       </c>
     </row>
@@ -5794,7 +5809,7 @@
       <c r="A13" s="25" t="s">
         <v>1348</v>
       </c>
-      <c r="B13" s="265" t="s">
+      <c r="B13" s="268" t="s">
         <v>1349</v>
       </c>
     </row>
@@ -5802,7 +5817,7 @@
       <c r="A14" s="25" t="s">
         <v>1350</v>
       </c>
-      <c r="B14" s="266" t="s">
+      <c r="B14" s="269" t="s">
         <v>1351</v>
       </c>
     </row>
@@ -6038,7 +6053,7 @@
       <c r="A12" s="16" t="s">
         <v>1369</v>
       </c>
-      <c r="B12" s="267" t="s">
+      <c r="B12" s="270" t="s">
         <v>1370</v>
       </c>
       <c r="C12" s="16"/>
@@ -6056,7 +6071,7 @@
       <c r="A13" s="16" t="s">
         <v>1371</v>
       </c>
-      <c r="B13" s="267" t="s">
+      <c r="B13" s="270" t="s">
         <v>1372</v>
       </c>
       <c r="C13" s="16"/>
@@ -6074,7 +6089,7 @@
       <c r="A14" s="16" t="s">
         <v>1373</v>
       </c>
-      <c r="B14" s="267" t="s">
+      <c r="B14" s="270" t="s">
         <v>1374</v>
       </c>
       <c r="C14" s="16"/>
@@ -6092,7 +6107,7 @@
       <c r="A15" s="16" t="s">
         <v>1375</v>
       </c>
-      <c r="B15" s="267" t="s">
+      <c r="B15" s="270" t="s">
         <v>1376</v>
       </c>
       <c r="C15" s="16"/>
@@ -6181,15 +6196,15 @@
       <c r="B20" s="116" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="268"/>
-      <c r="D20" s="268"/>
-      <c r="E20" s="268"/>
-      <c r="F20" s="268"/>
-      <c r="G20" s="268"/>
-      <c r="H20" s="268"/>
-      <c r="I20" s="268"/>
-      <c r="J20" s="268"/>
-      <c r="K20" s="268"/>
+      <c r="C20" s="271"/>
+      <c r="D20" s="271"/>
+      <c r="E20" s="271"/>
+      <c r="F20" s="271"/>
+      <c r="G20" s="271"/>
+      <c r="H20" s="271"/>
+      <c r="I20" s="271"/>
+      <c r="J20" s="271"/>
+      <c r="K20" s="271"/>
       <c r="L20" s="16"/>
     </row>
     <row r="21">
@@ -6226,39 +6241,39 @@
       <c r="L27" s="16"/>
     </row>
     <row r="28">
-      <c r="A28" s="268" t="s">
+      <c r="A28" s="271" t="s">
         <v>1385</v>
       </c>
-      <c r="B28" s="269" t="s">
+      <c r="B28" s="272" t="s">
         <v>1386</v>
       </c>
       <c r="L28" s="16"/>
     </row>
     <row r="29">
-      <c r="A29" s="268" t="s">
+      <c r="A29" s="271" t="s">
         <v>1387</v>
       </c>
-      <c r="B29" s="270" t="s">
+      <c r="B29" s="273" t="s">
         <v>1388</v>
       </c>
       <c r="L29" s="16"/>
     </row>
     <row r="30">
-      <c r="A30" s="268" t="s">
+      <c r="A30" s="271" t="s">
         <v>1389</v>
       </c>
-      <c r="B30" s="264" t="s">
+      <c r="B30" s="267" t="s">
         <v>1390</v>
       </c>
-      <c r="C30" s="269"/>
-      <c r="D30" s="269"/>
-      <c r="E30" s="269"/>
-      <c r="F30" s="269"/>
-      <c r="G30" s="269"/>
-      <c r="H30" s="269"/>
-      <c r="I30" s="269"/>
-      <c r="J30" s="269"/>
-      <c r="K30" s="269"/>
+      <c r="C30" s="272"/>
+      <c r="D30" s="272"/>
+      <c r="E30" s="272"/>
+      <c r="F30" s="272"/>
+      <c r="G30" s="272"/>
+      <c r="H30" s="272"/>
+      <c r="I30" s="272"/>
+      <c r="J30" s="272"/>
+      <c r="K30" s="272"/>
       <c r="L30" s="16"/>
     </row>
     <row r="31" hidden="1">
@@ -6275,16 +6290,16 @@
     </row>
     <row r="33">
       <c r="A33" s="16"/>
-      <c r="B33" s="268"/>
-      <c r="C33" s="268"/>
-      <c r="D33" s="268"/>
-      <c r="E33" s="268"/>
-      <c r="F33" s="268"/>
-      <c r="G33" s="268"/>
-      <c r="H33" s="268"/>
-      <c r="I33" s="268"/>
-      <c r="J33" s="268"/>
-      <c r="K33" s="268"/>
+      <c r="B33" s="271"/>
+      <c r="C33" s="271"/>
+      <c r="D33" s="271"/>
+      <c r="E33" s="271"/>
+      <c r="F33" s="271"/>
+      <c r="G33" s="271"/>
+      <c r="H33" s="271"/>
+      <c r="I33" s="271"/>
+      <c r="J33" s="271"/>
+      <c r="K33" s="271"/>
       <c r="L33" s="16"/>
     </row>
   </sheetData>
@@ -14094,13 +14109,13 @@
       <c r="N108" s="34"/>
     </row>
     <row r="109">
-      <c r="A109" s="137" t="s">
+      <c r="A109" s="191" t="s">
         <v>838</v>
       </c>
-      <c r="B109" s="121" t="s">
+      <c r="B109" s="192" t="s">
         <v>839</v>
       </c>
-      <c r="C109" s="145" t="s">
+      <c r="C109" s="193" t="s">
         <v>484</v>
       </c>
       <c r="D109" s="39"/>
@@ -14126,17 +14141,17 @@
       <c r="N109" s="34"/>
     </row>
     <row r="110">
-      <c r="A110" s="137" t="s">
+      <c r="A110" s="191" t="s">
         <v>842</v>
       </c>
-      <c r="B110" s="121" t="s">
+      <c r="B110" s="192" t="s">
         <v>843</v>
       </c>
-      <c r="C110" s="145" t="s">
+      <c r="C110" s="193" t="s">
         <v>484</v>
       </c>
       <c r="D110" s="39"/>
-      <c r="E110" s="191" t="s">
+      <c r="E110" s="194" t="s">
         <v>370</v>
       </c>
       <c r="F110" s="32" t="s">
@@ -14151,24 +14166,24 @@
       <c r="K110" s="117">
         <v>0.0</v>
       </c>
-      <c r="L110" s="192" t="s">
+      <c r="L110" s="195" t="s">
         <v>274</v>
       </c>
-      <c r="M110" s="192"/>
+      <c r="M110" s="195"/>
       <c r="N110" s="34"/>
     </row>
     <row r="111">
-      <c r="A111" s="137" t="s">
+      <c r="A111" s="191" t="s">
         <v>845</v>
       </c>
-      <c r="B111" s="121" t="s">
+      <c r="B111" s="192" t="s">
         <v>846</v>
       </c>
-      <c r="C111" s="145" t="s">
+      <c r="C111" s="193" t="s">
         <v>484</v>
       </c>
       <c r="D111" s="39"/>
-      <c r="E111" s="191" t="s">
+      <c r="E111" s="194" t="s">
         <v>370</v>
       </c>
       <c r="F111" s="32" t="s">
@@ -14184,23 +14199,23 @@
         <v>704</v>
       </c>
       <c r="L111" s="121" t="s">
-        <v>731</v>
+        <v>757</v>
       </c>
       <c r="M111" s="121"/>
       <c r="N111" s="34"/>
     </row>
     <row r="112">
-      <c r="A112" s="137" t="s">
+      <c r="A112" s="191" t="s">
         <v>848</v>
       </c>
-      <c r="B112" s="121" t="s">
+      <c r="B112" s="192" t="s">
         <v>849</v>
       </c>
-      <c r="C112" s="145" t="s">
+      <c r="C112" s="193" t="s">
         <v>484</v>
       </c>
       <c r="D112" s="39"/>
-      <c r="E112" s="191" t="s">
+      <c r="E112" s="194" t="s">
         <v>370</v>
       </c>
       <c r="F112" s="32" t="s">
@@ -14222,17 +14237,17 @@
       <c r="N112" s="34"/>
     </row>
     <row r="113">
-      <c r="A113" s="137" t="s">
+      <c r="A113" s="191" t="s">
         <v>852</v>
       </c>
-      <c r="B113" s="121" t="s">
+      <c r="B113" s="192" t="s">
         <v>853</v>
       </c>
-      <c r="C113" s="145" t="s">
+      <c r="C113" s="193" t="s">
         <v>484</v>
       </c>
       <c r="D113" s="39"/>
-      <c r="E113" s="191" t="s">
+      <c r="E113" s="194" t="s">
         <v>370</v>
       </c>
       <c r="F113" s="32" t="s">
@@ -14254,17 +14269,17 @@
       <c r="N113" s="34"/>
     </row>
     <row r="114">
-      <c r="A114" s="137" t="s">
+      <c r="A114" s="191" t="s">
         <v>855</v>
       </c>
-      <c r="B114" s="121" t="s">
+      <c r="B114" s="192" t="s">
         <v>856</v>
       </c>
-      <c r="C114" s="145" t="s">
+      <c r="C114" s="193" t="s">
         <v>484</v>
       </c>
       <c r="D114" s="39"/>
-      <c r="E114" s="191" t="s">
+      <c r="E114" s="194" t="s">
         <v>370</v>
       </c>
       <c r="F114" s="32" t="s">
@@ -14292,7 +14307,7 @@
       <c r="B115" s="157" t="s">
         <v>859</v>
       </c>
-      <c r="C115" s="193" t="s">
+      <c r="C115" s="196" t="s">
         <v>480</v>
       </c>
       <c r="D115" s="59"/>
@@ -14360,7 +14375,7 @@
         <v>484</v>
       </c>
       <c r="D117" s="39"/>
-      <c r="E117" s="191" t="s">
+      <c r="E117" s="194" t="s">
         <v>370</v>
       </c>
       <c r="F117" s="41" t="s">
@@ -14375,10 +14390,10 @@
       <c r="K117" s="117">
         <v>0.0</v>
       </c>
-      <c r="L117" s="192" t="s">
+      <c r="L117" s="195" t="s">
         <v>274</v>
       </c>
-      <c r="M117" s="192"/>
+      <c r="M117" s="195"/>
       <c r="N117" s="34"/>
     </row>
     <row r="118">
@@ -14388,11 +14403,11 @@
       <c r="B118" s="157" t="s">
         <v>870</v>
       </c>
-      <c r="C118" s="193" t="s">
+      <c r="C118" s="196" t="s">
         <v>484</v>
       </c>
       <c r="D118" s="59"/>
-      <c r="E118" s="191" t="s">
+      <c r="E118" s="194" t="s">
         <v>370</v>
       </c>
       <c r="F118" s="41" t="s">
@@ -14420,11 +14435,11 @@
       <c r="B119" s="157" t="s">
         <v>873</v>
       </c>
-      <c r="C119" s="193" t="s">
+      <c r="C119" s="196" t="s">
         <v>484</v>
       </c>
       <c r="D119" s="59"/>
-      <c r="E119" s="191" t="s">
+      <c r="E119" s="194" t="s">
         <v>370</v>
       </c>
       <c r="F119" s="41" t="s">
@@ -14452,11 +14467,11 @@
       <c r="B120" s="157" t="s">
         <v>876</v>
       </c>
-      <c r="C120" s="193" t="s">
+      <c r="C120" s="196" t="s">
         <v>484</v>
       </c>
       <c r="D120" s="59"/>
-      <c r="E120" s="191" t="s">
+      <c r="E120" s="194" t="s">
         <v>370</v>
       </c>
       <c r="F120" s="41" t="s">
@@ -14488,7 +14503,7 @@
         <v>484</v>
       </c>
       <c r="D121" s="129"/>
-      <c r="E121" s="191" t="s">
+      <c r="E121" s="194" t="s">
         <v>370</v>
       </c>
       <c r="F121" s="41" t="s">
@@ -14516,7 +14531,7 @@
       <c r="B122" s="123" t="s">
         <v>882</v>
       </c>
-      <c r="C122" s="194" t="s">
+      <c r="C122" s="197" t="s">
         <v>480</v>
       </c>
       <c r="D122" s="25"/>
@@ -14548,7 +14563,7 @@
       <c r="B123" s="123" t="s">
         <v>886</v>
       </c>
-      <c r="C123" s="194" t="s">
+      <c r="C123" s="197" t="s">
         <v>484</v>
       </c>
       <c r="D123" s="25"/>
@@ -14567,10 +14582,10 @@
       <c r="K123" s="115">
         <v>0.0</v>
       </c>
-      <c r="L123" s="195" t="s">
+      <c r="L123" s="198" t="s">
         <v>297</v>
       </c>
-      <c r="M123" s="195"/>
+      <c r="M123" s="198"/>
       <c r="N123" s="16"/>
     </row>
     <row r="124">
@@ -14580,7 +14595,7 @@
       <c r="B124" s="123" t="s">
         <v>890</v>
       </c>
-      <c r="C124" s="194" t="s">
+      <c r="C124" s="197" t="s">
         <v>480</v>
       </c>
       <c r="D124" s="25"/>
@@ -14610,7 +14625,7 @@
       <c r="B125" s="123" t="s">
         <v>893</v>
       </c>
-      <c r="C125" s="194" t="s">
+      <c r="C125" s="197" t="s">
         <v>484</v>
       </c>
       <c r="D125" s="25"/>
@@ -14754,7 +14769,7 @@
       <c r="H129" s="36"/>
       <c r="I129" s="34"/>
       <c r="J129" s="34"/>
-      <c r="K129" s="196" t="s">
+      <c r="K129" s="199" t="s">
         <v>704</v>
       </c>
       <c r="L129" s="147" t="s">
@@ -14786,7 +14801,7 @@
       <c r="H130" s="36"/>
       <c r="I130" s="34"/>
       <c r="J130" s="34"/>
-      <c r="K130" s="196" t="s">
+      <c r="K130" s="199" t="s">
         <v>709</v>
       </c>
       <c r="L130" s="147" t="s">
@@ -14882,7 +14897,7 @@
       <c r="H133" s="36"/>
       <c r="I133" s="34"/>
       <c r="J133" s="34"/>
-      <c r="K133" s="196" t="s">
+      <c r="K133" s="199" t="s">
         <v>704</v>
       </c>
       <c r="L133" s="147" t="s">
@@ -14914,7 +14929,7 @@
       <c r="H134" s="36"/>
       <c r="I134" s="34"/>
       <c r="J134" s="34"/>
-      <c r="K134" s="196" t="s">
+      <c r="K134" s="199" t="s">
         <v>709</v>
       </c>
       <c r="L134" s="147" t="s">
@@ -15084,17 +15099,17 @@
       <c r="N139" s="34"/>
     </row>
     <row r="140">
-      <c r="A140" s="197" t="s">
+      <c r="A140" s="200" t="s">
         <v>947</v>
       </c>
-      <c r="B140" s="198" t="s">
+      <c r="B140" s="201" t="s">
         <v>948</v>
       </c>
-      <c r="C140" s="199" t="s">
+      <c r="C140" s="202" t="s">
         <v>480</v>
       </c>
-      <c r="D140" s="199"/>
-      <c r="E140" s="200" t="s">
+      <c r="D140" s="202"/>
+      <c r="E140" s="203" t="s">
         <v>370</v>
       </c>
       <c r="F140" s="32" t="s">
@@ -15103,17 +15118,17 @@
       <c r="G140" s="143" t="s">
         <v>949</v>
       </c>
-      <c r="H140" s="201"/>
-      <c r="I140" s="202"/>
-      <c r="J140" s="202"/>
-      <c r="K140" s="203" t="s">
+      <c r="H140" s="204"/>
+      <c r="I140" s="205"/>
+      <c r="J140" s="205"/>
+      <c r="K140" s="206" t="s">
         <v>945</v>
       </c>
-      <c r="L140" s="204" t="s">
+      <c r="L140" s="207" t="s">
         <v>950</v>
       </c>
-      <c r="M140" s="204"/>
-      <c r="N140" s="202"/>
+      <c r="M140" s="207"/>
+      <c r="N140" s="205"/>
     </row>
     <row r="141">
       <c r="A141" s="24" t="s">
@@ -15122,7 +15137,7 @@
       <c r="B141" s="115" t="s">
         <v>952</v>
       </c>
-      <c r="C141" s="194" t="s">
+      <c r="C141" s="197" t="s">
         <v>480</v>
       </c>
       <c r="D141" s="25"/>
@@ -15132,7 +15147,7 @@
       <c r="F141" s="14" t="s">
         <v>953</v>
       </c>
-      <c r="G141" s="205" t="s">
+      <c r="G141" s="208" t="s">
         <v>954</v>
       </c>
       <c r="H141" s="13"/>
@@ -15141,10 +15156,10 @@
       <c r="K141" s="123">
         <v>0.0</v>
       </c>
-      <c r="L141" s="206" t="s">
+      <c r="L141" s="209" t="s">
         <v>230</v>
       </c>
-      <c r="M141" s="206"/>
+      <c r="M141" s="209"/>
       <c r="N141" s="16"/>
     </row>
     <row r="142">
@@ -15154,7 +15169,7 @@
       <c r="B142" s="115" t="s">
         <v>956</v>
       </c>
-      <c r="C142" s="194" t="s">
+      <c r="C142" s="197" t="s">
         <v>484</v>
       </c>
       <c r="D142" s="25"/>
@@ -15173,10 +15188,10 @@
       <c r="K142" s="123">
         <v>0.0</v>
       </c>
-      <c r="L142" s="206" t="s">
+      <c r="L142" s="209" t="s">
         <v>230</v>
       </c>
-      <c r="M142" s="206"/>
+      <c r="M142" s="209"/>
       <c r="N142" s="16"/>
     </row>
     <row r="143">
@@ -15186,7 +15201,7 @@
       <c r="B143" s="115" t="s">
         <v>960</v>
       </c>
-      <c r="C143" s="194" t="s">
+      <c r="C143" s="197" t="s">
         <v>480</v>
       </c>
       <c r="D143" s="25"/>
@@ -15196,7 +15211,7 @@
       <c r="F143" s="14" t="s">
         <v>961</v>
       </c>
-      <c r="G143" s="205" t="s">
+      <c r="G143" s="208" t="s">
         <v>954</v>
       </c>
       <c r="H143" s="13"/>
@@ -15205,10 +15220,10 @@
       <c r="K143" s="123">
         <v>0.0</v>
       </c>
-      <c r="L143" s="206" t="s">
+      <c r="L143" s="209" t="s">
         <v>225</v>
       </c>
-      <c r="M143" s="206"/>
+      <c r="M143" s="209"/>
       <c r="N143" s="16"/>
     </row>
     <row r="144">
@@ -15218,7 +15233,7 @@
       <c r="B144" s="115" t="s">
         <v>963</v>
       </c>
-      <c r="C144" s="194" t="s">
+      <c r="C144" s="197" t="s">
         <v>484</v>
       </c>
       <c r="D144" s="25"/>
@@ -15237,10 +15252,10 @@
       <c r="K144" s="123">
         <v>0.0</v>
       </c>
-      <c r="L144" s="206" t="s">
+      <c r="L144" s="209" t="s">
         <v>225</v>
       </c>
-      <c r="M144" s="206"/>
+      <c r="M144" s="209"/>
       <c r="N144" s="16"/>
     </row>
     <row r="145">
@@ -15250,14 +15265,14 @@
       <c r="B145" s="115" t="s">
         <v>967</v>
       </c>
-      <c r="C145" s="194" t="s">
+      <c r="C145" s="197" t="s">
         <v>480</v>
       </c>
       <c r="D145" s="25"/>
       <c r="E145" s="20" t="s">
         <v>370</v>
       </c>
-      <c r="F145" s="205" t="s">
+      <c r="F145" s="208" t="s">
         <v>954</v>
       </c>
       <c r="G145" s="5" t="s">
@@ -15269,10 +15284,10 @@
       <c r="K145" s="123">
         <v>3.0</v>
       </c>
-      <c r="L145" s="206" t="s">
+      <c r="L145" s="209" t="s">
         <v>346</v>
       </c>
-      <c r="M145" s="206"/>
+      <c r="M145" s="209"/>
       <c r="N145" s="16"/>
     </row>
     <row r="146">
@@ -15282,14 +15297,14 @@
       <c r="B146" s="115" t="s">
         <v>970</v>
       </c>
-      <c r="C146" s="194" t="s">
+      <c r="C146" s="197" t="s">
         <v>480</v>
       </c>
       <c r="D146" s="25"/>
       <c r="E146" s="20" t="s">
         <v>370</v>
       </c>
-      <c r="F146" s="205" t="s">
+      <c r="F146" s="208" t="s">
         <v>954</v>
       </c>
       <c r="G146" s="5" t="s">
@@ -15301,10 +15316,10 @@
       <c r="K146" s="123">
         <v>3.0</v>
       </c>
-      <c r="L146" s="206" t="s">
+      <c r="L146" s="209" t="s">
         <v>293</v>
       </c>
-      <c r="M146" s="206"/>
+      <c r="M146" s="209"/>
       <c r="N146" s="16"/>
     </row>
     <row r="147">
@@ -15349,7 +15364,7 @@
       <c r="C148" s="145" t="s">
         <v>484</v>
       </c>
-      <c r="D148" s="207"/>
+      <c r="D148" s="210"/>
       <c r="E148" s="137" t="s">
         <v>363</v>
       </c>
@@ -15362,7 +15377,7 @@
       <c r="H148" s="38"/>
       <c r="I148" s="34"/>
       <c r="J148" s="34"/>
-      <c r="K148" s="208" t="s">
+      <c r="K148" s="211" t="s">
         <v>981</v>
       </c>
       <c r="L148" s="5" t="s">
@@ -15381,7 +15396,7 @@
       <c r="C149" s="145" t="s">
         <v>480</v>
       </c>
-      <c r="D149" s="207"/>
+      <c r="D149" s="210"/>
       <c r="E149" s="137" t="s">
         <v>373</v>
       </c>
@@ -15397,10 +15412,10 @@
       <c r="K149" s="134" t="s">
         <v>512</v>
       </c>
-      <c r="L149" s="209" t="s">
+      <c r="L149" s="212" t="s">
         <v>986</v>
       </c>
-      <c r="M149" s="209"/>
+      <c r="M149" s="212"/>
       <c r="N149" s="34"/>
     </row>
     <row r="150">
@@ -15413,7 +15428,7 @@
       <c r="C150" s="145" t="s">
         <v>484</v>
       </c>
-      <c r="D150" s="207"/>
+      <c r="D150" s="210"/>
       <c r="E150" s="137" t="s">
         <v>363</v>
       </c>
@@ -15426,7 +15441,7 @@
       <c r="H150" s="36"/>
       <c r="I150" s="34"/>
       <c r="J150" s="34"/>
-      <c r="K150" s="208" t="s">
+      <c r="K150" s="211" t="s">
         <v>981</v>
       </c>
       <c r="L150" s="5" t="s">
@@ -15445,7 +15460,7 @@
       <c r="C151" s="145" t="s">
         <v>480</v>
       </c>
-      <c r="D151" s="207"/>
+      <c r="D151" s="210"/>
       <c r="E151" s="137" t="s">
         <v>373</v>
       </c>
@@ -15477,7 +15492,7 @@
       <c r="C152" s="145" t="s">
         <v>484</v>
       </c>
-      <c r="D152" s="207"/>
+      <c r="D152" s="210"/>
       <c r="E152" s="137" t="s">
         <v>363</v>
       </c>
@@ -15490,7 +15505,7 @@
       <c r="H152" s="36"/>
       <c r="I152" s="34"/>
       <c r="J152" s="34"/>
-      <c r="K152" s="208" t="s">
+      <c r="K152" s="211" t="s">
         <v>981</v>
       </c>
       <c r="L152" s="5" t="s">
@@ -15509,7 +15524,7 @@
       <c r="C153" s="145" t="s">
         <v>480</v>
       </c>
-      <c r="D153" s="207"/>
+      <c r="D153" s="210"/>
       <c r="E153" s="137" t="s">
         <v>373</v>
       </c>
@@ -15541,8 +15556,8 @@
       <c r="C154" s="156" t="s">
         <v>484</v>
       </c>
-      <c r="D154" s="210"/>
-      <c r="E154" s="211" t="s">
+      <c r="D154" s="213"/>
+      <c r="E154" s="214" t="s">
         <v>363</v>
       </c>
       <c r="F154" s="14" t="s">
@@ -15554,7 +15569,7 @@
       <c r="H154" s="13"/>
       <c r="I154" s="16"/>
       <c r="J154" s="16"/>
-      <c r="K154" s="208" t="s">
+      <c r="K154" s="211" t="s">
         <v>981</v>
       </c>
       <c r="L154" s="5" t="s">
@@ -15573,14 +15588,14 @@
       <c r="C155" s="156" t="s">
         <v>480</v>
       </c>
-      <c r="D155" s="210"/>
+      <c r="D155" s="213"/>
       <c r="E155" s="24" t="s">
         <v>373</v>
       </c>
       <c r="F155" s="14" t="s">
         <v>1012</v>
       </c>
-      <c r="G155" s="212" t="s">
+      <c r="G155" s="215" t="s">
         <v>975</v>
       </c>
       <c r="H155" s="13"/>
@@ -15589,10 +15604,10 @@
       <c r="K155" s="123" t="s">
         <v>512</v>
       </c>
-      <c r="L155" s="206" t="s">
+      <c r="L155" s="209" t="s">
         <v>1013</v>
       </c>
-      <c r="M155" s="206"/>
+      <c r="M155" s="209"/>
       <c r="N155" s="16"/>
     </row>
     <row r="156">
@@ -15605,8 +15620,8 @@
       <c r="C156" s="156" t="s">
         <v>484</v>
       </c>
-      <c r="D156" s="210"/>
-      <c r="E156" s="211" t="s">
+      <c r="D156" s="213"/>
+      <c r="E156" s="214" t="s">
         <v>363</v>
       </c>
       <c r="F156" s="14" t="s">
@@ -15618,7 +15633,7 @@
       <c r="H156" s="13"/>
       <c r="I156" s="16"/>
       <c r="J156" s="16"/>
-      <c r="K156" s="208" t="s">
+      <c r="K156" s="211" t="s">
         <v>981</v>
       </c>
       <c r="L156" s="5" t="s">
@@ -15637,14 +15652,14 @@
       <c r="C157" s="156" t="s">
         <v>480</v>
       </c>
-      <c r="D157" s="210"/>
+      <c r="D157" s="213"/>
       <c r="E157" s="24" t="s">
         <v>373</v>
       </c>
       <c r="F157" s="14" t="s">
         <v>1021</v>
       </c>
-      <c r="G157" s="212" t="s">
+      <c r="G157" s="215" t="s">
         <v>975</v>
       </c>
       <c r="H157" s="13"/>
@@ -15653,10 +15668,10 @@
       <c r="K157" s="123" t="s">
         <v>512</v>
       </c>
-      <c r="L157" s="206" t="s">
+      <c r="L157" s="209" t="s">
         <v>1022</v>
       </c>
-      <c r="M157" s="206"/>
+      <c r="M157" s="209"/>
       <c r="N157" s="16"/>
     </row>
     <row r="158">
@@ -15669,8 +15684,8 @@
       <c r="C158" s="156" t="s">
         <v>484</v>
       </c>
-      <c r="D158" s="210"/>
-      <c r="E158" s="211" t="s">
+      <c r="D158" s="213"/>
+      <c r="E158" s="214" t="s">
         <v>363</v>
       </c>
       <c r="F158" s="14" t="s">
@@ -15682,7 +15697,7 @@
       <c r="H158" s="13"/>
       <c r="I158" s="16"/>
       <c r="J158" s="16"/>
-      <c r="K158" s="208" t="s">
+      <c r="K158" s="211" t="s">
         <v>981</v>
       </c>
       <c r="L158" s="5" t="s">
@@ -15701,14 +15716,14 @@
       <c r="C159" s="156" t="s">
         <v>480</v>
       </c>
-      <c r="D159" s="210"/>
+      <c r="D159" s="213"/>
       <c r="E159" s="24" t="s">
         <v>373</v>
       </c>
       <c r="F159" s="14" t="s">
         <v>1030</v>
       </c>
-      <c r="G159" s="212" t="s">
+      <c r="G159" s="215" t="s">
         <v>975</v>
       </c>
       <c r="H159" s="13"/>
@@ -15717,10 +15732,10 @@
       <c r="K159" s="123" t="s">
         <v>512</v>
       </c>
-      <c r="L159" s="206" t="s">
+      <c r="L159" s="209" t="s">
         <v>1031</v>
       </c>
-      <c r="M159" s="206"/>
+      <c r="M159" s="209"/>
       <c r="N159" s="16"/>
     </row>
     <row r="160">
@@ -15733,8 +15748,8 @@
       <c r="C160" s="156" t="s">
         <v>484</v>
       </c>
-      <c r="D160" s="210"/>
-      <c r="E160" s="211" t="s">
+      <c r="D160" s="213"/>
+      <c r="E160" s="214" t="s">
         <v>363</v>
       </c>
       <c r="F160" s="14" t="s">
@@ -15746,7 +15761,7 @@
       <c r="H160" s="13"/>
       <c r="I160" s="16"/>
       <c r="J160" s="16"/>
-      <c r="K160" s="208" t="s">
+      <c r="K160" s="211" t="s">
         <v>981</v>
       </c>
       <c r="L160" s="5" t="s">
@@ -15765,14 +15780,14 @@
       <c r="C161" s="156" t="s">
         <v>480</v>
       </c>
-      <c r="D161" s="210"/>
+      <c r="D161" s="213"/>
       <c r="E161" s="24" t="s">
         <v>373</v>
       </c>
       <c r="F161" s="14" t="s">
         <v>1039</v>
       </c>
-      <c r="G161" s="212" t="s">
+      <c r="G161" s="215" t="s">
         <v>975</v>
       </c>
       <c r="H161" s="13"/>
@@ -15781,10 +15796,10 @@
       <c r="K161" s="123" t="s">
         <v>512</v>
       </c>
-      <c r="L161" s="206" t="s">
+      <c r="L161" s="209" t="s">
         <v>1040</v>
       </c>
-      <c r="M161" s="206"/>
+      <c r="M161" s="209"/>
       <c r="N161" s="16"/>
     </row>
     <row r="162">
@@ -15797,8 +15812,8 @@
       <c r="C162" s="156" t="s">
         <v>484</v>
       </c>
-      <c r="D162" s="210"/>
-      <c r="E162" s="211" t="s">
+      <c r="D162" s="213"/>
+      <c r="E162" s="214" t="s">
         <v>363</v>
       </c>
       <c r="F162" s="14" t="s">
@@ -15810,7 +15825,7 @@
       <c r="H162" s="13"/>
       <c r="I162" s="16"/>
       <c r="J162" s="16"/>
-      <c r="K162" s="208" t="s">
+      <c r="K162" s="211" t="s">
         <v>981</v>
       </c>
       <c r="L162" s="5" t="s">
@@ -15829,14 +15844,14 @@
       <c r="C163" s="156" t="s">
         <v>480</v>
       </c>
-      <c r="D163" s="210"/>
+      <c r="D163" s="213"/>
       <c r="E163" s="24" t="s">
         <v>373</v>
       </c>
       <c r="F163" s="14" t="s">
         <v>1048</v>
       </c>
-      <c r="G163" s="212" t="s">
+      <c r="G163" s="215" t="s">
         <v>975</v>
       </c>
       <c r="H163" s="13"/>
@@ -15845,10 +15860,10 @@
       <c r="K163" s="123" t="s">
         <v>512</v>
       </c>
-      <c r="L163" s="206" t="s">
+      <c r="L163" s="209" t="s">
         <v>1049</v>
       </c>
-      <c r="M163" s="206"/>
+      <c r="M163" s="209"/>
       <c r="N163" s="16"/>
     </row>
     <row r="164">
@@ -15861,8 +15876,8 @@
       <c r="C164" s="156" t="s">
         <v>484</v>
       </c>
-      <c r="D164" s="210"/>
-      <c r="E164" s="211" t="s">
+      <c r="D164" s="213"/>
+      <c r="E164" s="214" t="s">
         <v>363</v>
       </c>
       <c r="F164" s="14" t="s">
@@ -15874,7 +15889,7 @@
       <c r="H164" s="13"/>
       <c r="I164" s="16"/>
       <c r="J164" s="16"/>
-      <c r="K164" s="208" t="s">
+      <c r="K164" s="211" t="s">
         <v>981</v>
       </c>
       <c r="L164" s="5" t="s">
@@ -15893,11 +15908,11 @@
       <c r="C165" s="156" t="s">
         <v>480</v>
       </c>
-      <c r="D165" s="210"/>
+      <c r="D165" s="213"/>
       <c r="E165" s="20" t="s">
         <v>370</v>
       </c>
-      <c r="F165" s="212" t="s">
+      <c r="F165" s="215" t="s">
         <v>975</v>
       </c>
       <c r="G165" s="5"/>
@@ -15907,10 +15922,10 @@
       <c r="K165" s="123">
         <v>0.0</v>
       </c>
-      <c r="L165" s="206" t="s">
+      <c r="L165" s="209" t="s">
         <v>274</v>
       </c>
-      <c r="M165" s="206"/>
+      <c r="M165" s="209"/>
       <c r="N165" s="16"/>
     </row>
     <row r="166">
@@ -15923,11 +15938,11 @@
       <c r="C166" s="156" t="s">
         <v>480</v>
       </c>
-      <c r="D166" s="210"/>
+      <c r="D166" s="213"/>
       <c r="E166" s="20" t="s">
         <v>370</v>
       </c>
-      <c r="F166" s="212" t="s">
+      <c r="F166" s="215" t="s">
         <v>975</v>
       </c>
       <c r="G166" s="14"/>
@@ -15937,10 +15952,10 @@
       <c r="K166" s="123" t="s">
         <v>704</v>
       </c>
-      <c r="L166" s="206" t="s">
+      <c r="L166" s="209" t="s">
         <v>714</v>
       </c>
-      <c r="M166" s="206"/>
+      <c r="M166" s="209"/>
       <c r="N166" s="16"/>
     </row>
     <row r="167">
@@ -15957,7 +15972,7 @@
       <c r="E167" s="20" t="s">
         <v>370</v>
       </c>
-      <c r="F167" s="212" t="s">
+      <c r="F167" s="215" t="s">
         <v>975</v>
       </c>
       <c r="G167" s="14"/>
@@ -15967,10 +15982,10 @@
       <c r="K167" s="123" t="s">
         <v>709</v>
       </c>
-      <c r="L167" s="206" t="s">
+      <c r="L167" s="209" t="s">
         <v>785</v>
       </c>
-      <c r="M167" s="206"/>
+      <c r="M167" s="209"/>
       <c r="N167" s="16"/>
     </row>
     <row r="168">
@@ -15987,7 +16002,7 @@
       <c r="E168" s="20" t="s">
         <v>370</v>
       </c>
-      <c r="F168" s="212" t="s">
+      <c r="F168" s="215" t="s">
         <v>975</v>
       </c>
       <c r="G168" s="14"/>
@@ -15997,10 +16012,10 @@
       <c r="K168" s="123" t="s">
         <v>704</v>
       </c>
-      <c r="L168" s="206" t="s">
+      <c r="L168" s="209" t="s">
         <v>705</v>
       </c>
-      <c r="M168" s="206"/>
+      <c r="M168" s="209"/>
       <c r="N168" s="16"/>
     </row>
     <row r="169">
@@ -16017,7 +16032,7 @@
       <c r="E169" s="20" t="s">
         <v>370</v>
       </c>
-      <c r="F169" s="212" t="s">
+      <c r="F169" s="215" t="s">
         <v>975</v>
       </c>
       <c r="G169" s="14"/>
@@ -16027,10 +16042,10 @@
       <c r="K169" s="123" t="s">
         <v>709</v>
       </c>
-      <c r="L169" s="206" t="s">
+      <c r="L169" s="209" t="s">
         <v>710</v>
       </c>
-      <c r="M169" s="206"/>
+      <c r="M169" s="209"/>
       <c r="N169" s="16"/>
     </row>
   </sheetData>
@@ -16058,639 +16073,639 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="213" t="s">
+      <c r="A1" s="216" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="214" t="s">
+      <c r="B1" s="217" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="215" t="s">
+      <c r="C1" s="218" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="215" t="s">
+      <c r="D1" s="218" t="s">
         <v>1065</v>
       </c>
-      <c r="E1" s="213" t="s">
+      <c r="E1" s="216" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="216" t="s">
+      <c r="F1" s="219" t="s">
         <v>1066</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="217" t="s">
+      <c r="A2" s="220" t="s">
         <v>1067</v>
       </c>
-      <c r="B2" s="218" t="s">
+      <c r="B2" s="221" t="s">
         <v>1068</v>
       </c>
-      <c r="C2" s="219" t="s">
+      <c r="C2" s="222" t="s">
         <v>1069</v>
       </c>
-      <c r="D2" s="219"/>
-      <c r="E2" s="220"/>
-      <c r="F2" s="221"/>
+      <c r="D2" s="222"/>
+      <c r="E2" s="223"/>
+      <c r="F2" s="224"/>
     </row>
     <row r="3">
-      <c r="A3" s="217" t="s">
+      <c r="A3" s="220" t="s">
         <v>1070</v>
       </c>
-      <c r="B3" s="218" t="s">
+      <c r="B3" s="221" t="s">
         <v>1071</v>
       </c>
-      <c r="C3" s="218" t="s">
+      <c r="C3" s="221" t="s">
         <v>1072</v>
       </c>
-      <c r="D3" s="218"/>
-      <c r="E3" s="222"/>
-      <c r="F3" s="216" t="s">
+      <c r="D3" s="221"/>
+      <c r="E3" s="225"/>
+      <c r="F3" s="219" t="s">
         <v>1073</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="217" t="s">
+      <c r="A4" s="220" t="s">
         <v>1074</v>
       </c>
-      <c r="B4" s="218" t="s">
+      <c r="B4" s="221" t="s">
         <v>1075</v>
       </c>
-      <c r="C4" s="218" t="s">
+      <c r="C4" s="221" t="s">
         <v>1076</v>
       </c>
-      <c r="D4" s="218"/>
-      <c r="E4" s="223"/>
-      <c r="F4" s="221"/>
+      <c r="D4" s="221"/>
+      <c r="E4" s="226"/>
+      <c r="F4" s="224"/>
     </row>
     <row r="5">
-      <c r="A5" s="217" t="s">
+      <c r="A5" s="220" t="s">
         <v>1077</v>
       </c>
-      <c r="B5" s="218" t="s">
+      <c r="B5" s="221" t="s">
         <v>1078</v>
       </c>
-      <c r="C5" s="218" t="s">
+      <c r="C5" s="221" t="s">
         <v>1079</v>
       </c>
-      <c r="D5" s="218"/>
-      <c r="E5" s="223"/>
-      <c r="F5" s="221"/>
+      <c r="D5" s="221"/>
+      <c r="E5" s="226"/>
+      <c r="F5" s="224"/>
     </row>
     <row r="6">
-      <c r="A6" s="217" t="s">
+      <c r="A6" s="220" t="s">
         <v>1080</v>
       </c>
-      <c r="B6" s="224" t="s">
+      <c r="B6" s="227" t="s">
         <v>1081</v>
       </c>
-      <c r="C6" s="218" t="s">
+      <c r="C6" s="221" t="s">
         <v>1082</v>
       </c>
-      <c r="D6" s="218"/>
-      <c r="E6" s="222"/>
-      <c r="F6" s="221"/>
+      <c r="D6" s="221"/>
+      <c r="E6" s="225"/>
+      <c r="F6" s="224"/>
     </row>
     <row r="7">
-      <c r="A7" s="217" t="s">
+      <c r="A7" s="220" t="s">
         <v>1083</v>
       </c>
-      <c r="B7" s="225" t="s">
+      <c r="B7" s="228" t="s">
         <v>1084</v>
       </c>
-      <c r="C7" s="218" t="s">
+      <c r="C7" s="221" t="s">
         <v>1085</v>
       </c>
-      <c r="D7" s="218"/>
-      <c r="E7" s="216"/>
-      <c r="F7" s="221"/>
+      <c r="D7" s="221"/>
+      <c r="E7" s="219"/>
+      <c r="F7" s="224"/>
     </row>
     <row r="8">
-      <c r="A8" s="217" t="s">
+      <c r="A8" s="220" t="s">
         <v>1086</v>
       </c>
-      <c r="B8" s="225" t="s">
+      <c r="B8" s="228" t="s">
         <v>1087</v>
       </c>
-      <c r="C8" s="218" t="s">
+      <c r="C8" s="221" t="s">
         <v>1069</v>
       </c>
-      <c r="D8" s="218"/>
-      <c r="E8" s="216"/>
-      <c r="F8" s="221"/>
+      <c r="D8" s="221"/>
+      <c r="E8" s="219"/>
+      <c r="F8" s="224"/>
     </row>
     <row r="9">
-      <c r="A9" s="217" t="s">
+      <c r="A9" s="220" t="s">
         <v>1088</v>
       </c>
-      <c r="B9" s="225" t="s">
+      <c r="B9" s="228" t="s">
         <v>1089</v>
       </c>
-      <c r="C9" s="226" t="s">
+      <c r="C9" s="229" t="s">
         <v>1090</v>
       </c>
-      <c r="D9" s="226"/>
-      <c r="E9" s="227"/>
-      <c r="F9" s="221"/>
+      <c r="D9" s="229"/>
+      <c r="E9" s="230"/>
+      <c r="F9" s="224"/>
     </row>
     <row r="10">
-      <c r="A10" s="217" t="s">
+      <c r="A10" s="220" t="s">
         <v>1091</v>
       </c>
-      <c r="B10" s="225" t="s">
+      <c r="B10" s="228" t="s">
         <v>1092</v>
       </c>
-      <c r="C10" s="218" t="s">
+      <c r="C10" s="221" t="s">
         <v>1093</v>
       </c>
-      <c r="D10" s="218"/>
-      <c r="E10" s="216"/>
-      <c r="F10" s="221"/>
+      <c r="D10" s="221"/>
+      <c r="E10" s="219"/>
+      <c r="F10" s="224"/>
     </row>
     <row r="11">
-      <c r="A11" s="217" t="s">
+      <c r="A11" s="220" t="s">
         <v>1094</v>
       </c>
-      <c r="B11" s="218" t="s">
+      <c r="B11" s="221" t="s">
         <v>1095</v>
       </c>
-      <c r="C11" s="218" t="s">
+      <c r="C11" s="221" t="s">
         <v>1096</v>
       </c>
-      <c r="D11" s="218"/>
-      <c r="E11" s="221"/>
-      <c r="F11" s="221"/>
+      <c r="D11" s="221"/>
+      <c r="E11" s="224"/>
+      <c r="F11" s="224"/>
     </row>
     <row r="12">
-      <c r="A12" s="217" t="s">
+      <c r="A12" s="220" t="s">
         <v>1097</v>
       </c>
-      <c r="B12" s="228" t="s">
+      <c r="B12" s="231" t="s">
         <v>1098</v>
       </c>
-      <c r="C12" s="228" t="s">
+      <c r="C12" s="231" t="s">
         <v>1099</v>
       </c>
-      <c r="D12" s="228"/>
-      <c r="E12" s="221"/>
-      <c r="F12" s="221"/>
+      <c r="D12" s="231"/>
+      <c r="E12" s="224"/>
+      <c r="F12" s="224"/>
     </row>
     <row r="13">
-      <c r="A13" s="217" t="s">
+      <c r="A13" s="220" t="s">
         <v>1100</v>
       </c>
-      <c r="B13" s="229" t="s">
+      <c r="B13" s="232" t="s">
         <v>1101</v>
       </c>
-      <c r="C13" s="228" t="s">
+      <c r="C13" s="231" t="s">
         <v>1102</v>
       </c>
-      <c r="D13" s="228"/>
-      <c r="E13" s="221"/>
-      <c r="F13" s="221"/>
+      <c r="D13" s="231"/>
+      <c r="E13" s="224"/>
+      <c r="F13" s="224"/>
     </row>
     <row r="14">
-      <c r="A14" s="217" t="s">
+      <c r="A14" s="220" t="s">
         <v>1103</v>
       </c>
-      <c r="B14" s="229" t="s">
+      <c r="B14" s="232" t="s">
         <v>1104</v>
       </c>
-      <c r="C14" s="228" t="s">
+      <c r="C14" s="231" t="s">
         <v>1105</v>
       </c>
-      <c r="D14" s="228"/>
-      <c r="E14" s="221"/>
-      <c r="F14" s="221"/>
+      <c r="D14" s="231"/>
+      <c r="E14" s="224"/>
+      <c r="F14" s="224"/>
     </row>
     <row r="15">
-      <c r="A15" s="217" t="s">
+      <c r="A15" s="220" t="s">
         <v>1106</v>
       </c>
-      <c r="B15" s="229" t="s">
+      <c r="B15" s="232" t="s">
         <v>1107</v>
       </c>
-      <c r="C15" s="228" t="s">
+      <c r="C15" s="231" t="s">
         <v>1108</v>
       </c>
-      <c r="D15" s="228"/>
-      <c r="E15" s="221"/>
-      <c r="F15" s="221"/>
+      <c r="D15" s="231"/>
+      <c r="E15" s="224"/>
+      <c r="F15" s="224"/>
     </row>
     <row r="16">
-      <c r="A16" s="217" t="s">
+      <c r="A16" s="220" t="s">
         <v>1109</v>
       </c>
-      <c r="B16" s="229" t="s">
+      <c r="B16" s="232" t="s">
         <v>1110</v>
       </c>
-      <c r="C16" s="228" t="s">
+      <c r="C16" s="231" t="s">
         <v>1111</v>
       </c>
-      <c r="D16" s="228"/>
-      <c r="E16" s="221"/>
-      <c r="F16" s="221"/>
+      <c r="D16" s="231"/>
+      <c r="E16" s="224"/>
+      <c r="F16" s="224"/>
     </row>
     <row r="17">
-      <c r="A17" s="217" t="s">
+      <c r="A17" s="220" t="s">
         <v>1112</v>
       </c>
-      <c r="B17" s="229" t="s">
+      <c r="B17" s="232" t="s">
         <v>1113</v>
       </c>
-      <c r="C17" s="228" t="s">
+      <c r="C17" s="231" t="s">
         <v>1114</v>
       </c>
-      <c r="D17" s="228"/>
-      <c r="E17" s="221"/>
-      <c r="F17" s="221"/>
+      <c r="D17" s="231"/>
+      <c r="E17" s="224"/>
+      <c r="F17" s="224"/>
     </row>
     <row r="18">
-      <c r="A18" s="217" t="s">
+      <c r="A18" s="220" t="s">
         <v>1115</v>
       </c>
-      <c r="B18" s="229" t="s">
+      <c r="B18" s="232" t="s">
         <v>1116</v>
       </c>
-      <c r="C18" s="228" t="s">
+      <c r="C18" s="231" t="s">
         <v>1117</v>
       </c>
-      <c r="D18" s="228"/>
-      <c r="E18" s="221"/>
-      <c r="F18" s="221"/>
+      <c r="D18" s="231"/>
+      <c r="E18" s="224"/>
+      <c r="F18" s="224"/>
     </row>
     <row r="19">
-      <c r="A19" s="217" t="s">
+      <c r="A19" s="220" t="s">
         <v>1118</v>
       </c>
-      <c r="B19" s="229" t="s">
+      <c r="B19" s="232" t="s">
         <v>1119</v>
       </c>
-      <c r="C19" s="228" t="s">
+      <c r="C19" s="231" t="s">
         <v>1120</v>
       </c>
-      <c r="D19" s="228"/>
-      <c r="E19" s="221"/>
-      <c r="F19" s="221"/>
+      <c r="D19" s="231"/>
+      <c r="E19" s="224"/>
+      <c r="F19" s="224"/>
     </row>
     <row r="20">
-      <c r="A20" s="217" t="s">
+      <c r="A20" s="220" t="s">
         <v>1121</v>
       </c>
-      <c r="B20" s="229" t="s">
+      <c r="B20" s="232" t="s">
         <v>1122</v>
       </c>
-      <c r="C20" s="230" t="s">
+      <c r="C20" s="233" t="s">
         <v>1090</v>
       </c>
-      <c r="D20" s="230"/>
-      <c r="E20" s="221"/>
-      <c r="F20" s="221"/>
+      <c r="D20" s="233"/>
+      <c r="E20" s="224"/>
+      <c r="F20" s="224"/>
     </row>
     <row r="21">
-      <c r="A21" s="217" t="s">
+      <c r="A21" s="220" t="s">
         <v>1123</v>
       </c>
-      <c r="B21" s="231" t="s">
+      <c r="B21" s="234" t="s">
         <v>1124</v>
       </c>
-      <c r="C21" s="228" t="s">
+      <c r="C21" s="231" t="s">
         <v>1125</v>
       </c>
-      <c r="D21" s="228"/>
-      <c r="E21" s="221"/>
-      <c r="F21" s="221"/>
+      <c r="D21" s="231"/>
+      <c r="E21" s="224"/>
+      <c r="F21" s="224"/>
     </row>
     <row r="22">
-      <c r="A22" s="217" t="s">
+      <c r="A22" s="220" t="s">
         <v>1126</v>
       </c>
-      <c r="B22" s="229" t="s">
+      <c r="B22" s="232" t="s">
         <v>1127</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>1128</v>
       </c>
-      <c r="D22" s="232" t="s">
+      <c r="D22" s="235" t="s">
         <v>1129</v>
       </c>
-      <c r="E22" s="216"/>
-      <c r="F22" s="221"/>
+      <c r="E22" s="219"/>
+      <c r="F22" s="224"/>
     </row>
     <row r="23">
-      <c r="A23" s="217" t="s">
+      <c r="A23" s="220" t="s">
         <v>1130</v>
       </c>
-      <c r="B23" s="233" t="s">
+      <c r="B23" s="236" t="s">
         <v>1131</v>
       </c>
-      <c r="C23" s="234" t="s">
+      <c r="C23" s="237" t="s">
         <v>1132</v>
       </c>
-      <c r="D23" s="234"/>
-      <c r="E23" s="221"/>
-      <c r="F23" s="221"/>
+      <c r="D23" s="237"/>
+      <c r="E23" s="224"/>
+      <c r="F23" s="224"/>
     </row>
     <row r="24">
-      <c r="A24" s="217" t="s">
+      <c r="A24" s="220" t="s">
         <v>1133</v>
       </c>
-      <c r="B24" s="233" t="s">
+      <c r="B24" s="236" t="s">
         <v>1134</v>
       </c>
-      <c r="C24" s="234" t="s">
+      <c r="C24" s="237" t="s">
         <v>1135</v>
       </c>
-      <c r="D24" s="234"/>
-      <c r="E24" s="221"/>
-      <c r="F24" s="221"/>
+      <c r="D24" s="237"/>
+      <c r="E24" s="224"/>
+      <c r="F24" s="224"/>
     </row>
     <row r="25">
-      <c r="A25" s="217" t="s">
+      <c r="A25" s="220" t="s">
         <v>1136</v>
       </c>
-      <c r="B25" s="233" t="s">
+      <c r="B25" s="236" t="s">
         <v>1137</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>1128</v>
       </c>
-      <c r="D25" s="234" t="s">
+      <c r="D25" s="237" t="s">
         <v>453</v>
       </c>
-      <c r="E25" s="216"/>
-      <c r="F25" s="221"/>
+      <c r="E25" s="219"/>
+      <c r="F25" s="224"/>
     </row>
     <row r="26">
-      <c r="A26" s="217" t="s">
+      <c r="A26" s="220" t="s">
         <v>1138</v>
       </c>
-      <c r="B26" s="228" t="s">
+      <c r="B26" s="231" t="s">
         <v>1139</v>
       </c>
-      <c r="C26" s="228" t="s">
+      <c r="C26" s="231" t="s">
         <v>1140</v>
       </c>
-      <c r="D26" s="228"/>
-      <c r="E26" s="216"/>
-      <c r="F26" s="221"/>
+      <c r="D26" s="231"/>
+      <c r="E26" s="219"/>
+      <c r="F26" s="224"/>
     </row>
     <row r="27">
-      <c r="A27" s="217" t="s">
+      <c r="A27" s="220" t="s">
         <v>1141</v>
       </c>
-      <c r="B27" s="228" t="s">
+      <c r="B27" s="231" t="s">
         <v>1142</v>
       </c>
-      <c r="C27" s="228" t="s">
+      <c r="C27" s="231" t="s">
         <v>1143</v>
       </c>
-      <c r="D27" s="228"/>
-      <c r="E27" s="221"/>
-      <c r="F27" s="221"/>
+      <c r="D27" s="231"/>
+      <c r="E27" s="224"/>
+      <c r="F27" s="224"/>
     </row>
     <row r="28">
-      <c r="A28" s="217" t="s">
+      <c r="A28" s="220" t="s">
         <v>1144</v>
       </c>
-      <c r="B28" s="228" t="s">
+      <c r="B28" s="231" t="s">
         <v>1145</v>
       </c>
-      <c r="C28" s="228" t="s">
+      <c r="C28" s="231" t="s">
         <v>1146</v>
       </c>
-      <c r="D28" s="228"/>
-      <c r="E28" s="221"/>
-      <c r="F28" s="221"/>
+      <c r="D28" s="231"/>
+      <c r="E28" s="224"/>
+      <c r="F28" s="224"/>
     </row>
     <row r="29">
-      <c r="A29" s="217" t="s">
+      <c r="A29" s="220" t="s">
         <v>1147</v>
       </c>
-      <c r="B29" s="235" t="s">
+      <c r="B29" s="238" t="s">
         <v>1148</v>
       </c>
-      <c r="C29" s="225" t="s">
+      <c r="C29" s="228" t="s">
         <v>1149</v>
       </c>
-      <c r="D29" s="225"/>
-      <c r="E29" s="236"/>
+      <c r="D29" s="228"/>
+      <c r="E29" s="239"/>
     </row>
     <row r="30">
-      <c r="A30" s="217" t="s">
+      <c r="A30" s="220" t="s">
         <v>1150</v>
       </c>
-      <c r="B30" s="235" t="s">
+      <c r="B30" s="238" t="s">
         <v>1151</v>
       </c>
-      <c r="C30" s="225" t="s">
+      <c r="C30" s="228" t="s">
         <v>1152</v>
       </c>
-      <c r="D30" s="225"/>
-      <c r="E30" s="236"/>
+      <c r="D30" s="228"/>
+      <c r="E30" s="239"/>
     </row>
     <row r="31">
-      <c r="A31" s="217" t="s">
+      <c r="A31" s="220" t="s">
         <v>1153</v>
       </c>
-      <c r="B31" s="235" t="s">
+      <c r="B31" s="238" t="s">
         <v>1154</v>
       </c>
-      <c r="C31" s="225" t="s">
+      <c r="C31" s="228" t="s">
         <v>1155</v>
       </c>
-      <c r="D31" s="225"/>
-      <c r="E31" s="236"/>
+      <c r="D31" s="228"/>
+      <c r="E31" s="239"/>
     </row>
     <row r="32">
-      <c r="A32" s="217" t="s">
+      <c r="A32" s="220" t="s">
         <v>1156</v>
       </c>
-      <c r="B32" s="235" t="s">
+      <c r="B32" s="238" t="s">
         <v>1157</v>
       </c>
-      <c r="C32" s="225" t="s">
+      <c r="C32" s="228" t="s">
         <v>1158</v>
       </c>
-      <c r="D32" s="225"/>
-      <c r="E32" s="236"/>
+      <c r="D32" s="228"/>
+      <c r="E32" s="239"/>
     </row>
     <row r="33">
-      <c r="A33" s="217" t="s">
+      <c r="A33" s="220" t="s">
         <v>1159</v>
       </c>
-      <c r="B33" s="235" t="s">
+      <c r="B33" s="238" t="s">
         <v>1160</v>
       </c>
-      <c r="C33" s="225" t="s">
+      <c r="C33" s="228" t="s">
         <v>1161</v>
       </c>
-      <c r="D33" s="225"/>
-      <c r="E33" s="236"/>
+      <c r="D33" s="228"/>
+      <c r="E33" s="239"/>
     </row>
     <row r="34">
-      <c r="A34" s="217" t="s">
+      <c r="A34" s="220" t="s">
         <v>1162</v>
       </c>
-      <c r="B34" s="235" t="s">
+      <c r="B34" s="238" t="s">
         <v>1163</v>
       </c>
-      <c r="C34" s="225" t="s">
+      <c r="C34" s="228" t="s">
         <v>1164</v>
       </c>
-      <c r="D34" s="225"/>
-      <c r="E34" s="236"/>
+      <c r="D34" s="228"/>
+      <c r="E34" s="239"/>
     </row>
     <row r="35">
-      <c r="A35" s="217" t="s">
+      <c r="A35" s="220" t="s">
         <v>1165</v>
       </c>
-      <c r="B35" s="235" t="s">
+      <c r="B35" s="238" t="s">
         <v>1166</v>
       </c>
-      <c r="C35" s="225" t="s">
+      <c r="C35" s="228" t="s">
         <v>1167</v>
       </c>
-      <c r="D35" s="225"/>
-      <c r="E35" s="236"/>
+      <c r="D35" s="228"/>
+      <c r="E35" s="239"/>
     </row>
     <row r="36">
-      <c r="A36" s="217" t="s">
+      <c r="A36" s="220" t="s">
         <v>1168</v>
       </c>
-      <c r="B36" s="235" t="s">
+      <c r="B36" s="238" t="s">
         <v>1169</v>
       </c>
-      <c r="C36" s="225" t="s">
+      <c r="C36" s="228" t="s">
         <v>1170</v>
       </c>
-      <c r="D36" s="225"/>
-      <c r="E36" s="236"/>
+      <c r="D36" s="228"/>
+      <c r="E36" s="239"/>
     </row>
     <row r="37">
-      <c r="A37" s="217" t="s">
+      <c r="A37" s="220" t="s">
         <v>1171</v>
       </c>
-      <c r="B37" s="235" t="s">
+      <c r="B37" s="238" t="s">
         <v>1172</v>
       </c>
-      <c r="C37" s="225" t="s">
+      <c r="C37" s="228" t="s">
         <v>1173</v>
       </c>
-      <c r="D37" s="225"/>
-      <c r="E37" s="236"/>
+      <c r="D37" s="228"/>
+      <c r="E37" s="239"/>
     </row>
     <row r="38">
-      <c r="A38" s="217" t="s">
+      <c r="A38" s="220" t="s">
         <v>1174</v>
       </c>
-      <c r="B38" s="235" t="s">
+      <c r="B38" s="238" t="s">
         <v>1175</v>
       </c>
-      <c r="C38" s="225" t="s">
+      <c r="C38" s="228" t="s">
         <v>1176</v>
       </c>
-      <c r="D38" s="225"/>
-      <c r="E38" s="236"/>
+      <c r="D38" s="228"/>
+      <c r="E38" s="239"/>
     </row>
     <row r="39">
-      <c r="A39" s="217" t="s">
+      <c r="A39" s="220" t="s">
         <v>1177</v>
       </c>
-      <c r="B39" s="237" t="s">
+      <c r="B39" s="240" t="s">
         <v>1178</v>
       </c>
-      <c r="C39" s="233" t="s">
+      <c r="C39" s="236" t="s">
         <v>1179</v>
       </c>
-      <c r="D39" s="233"/>
-      <c r="E39" s="238"/>
-      <c r="F39" s="221"/>
+      <c r="D39" s="236"/>
+      <c r="E39" s="241"/>
+      <c r="F39" s="224"/>
     </row>
     <row r="40">
-      <c r="A40" s="217" t="s">
+      <c r="A40" s="220" t="s">
         <v>1180</v>
       </c>
-      <c r="B40" s="237" t="s">
+      <c r="B40" s="240" t="s">
         <v>1181</v>
       </c>
-      <c r="C40" s="233" t="s">
+      <c r="C40" s="236" t="s">
         <v>1182</v>
       </c>
-      <c r="D40" s="233"/>
-      <c r="E40" s="239"/>
-      <c r="F40" s="221"/>
+      <c r="D40" s="236"/>
+      <c r="E40" s="242"/>
+      <c r="F40" s="224"/>
     </row>
     <row r="41">
-      <c r="A41" s="217" t="s">
+      <c r="A41" s="220" t="s">
         <v>1183</v>
       </c>
-      <c r="B41" s="237" t="s">
+      <c r="B41" s="240" t="s">
         <v>1184</v>
       </c>
-      <c r="C41" s="233" t="s">
+      <c r="C41" s="236" t="s">
         <v>1185</v>
       </c>
-      <c r="D41" s="233"/>
-      <c r="E41" s="238"/>
-      <c r="F41" s="221"/>
+      <c r="D41" s="236"/>
+      <c r="E41" s="241"/>
+      <c r="F41" s="224"/>
     </row>
     <row r="42">
-      <c r="A42" s="217" t="s">
+      <c r="A42" s="220" t="s">
         <v>1186</v>
       </c>
-      <c r="B42" s="237" t="s">
+      <c r="B42" s="240" t="s">
         <v>1081</v>
       </c>
-      <c r="C42" s="240" t="s">
+      <c r="C42" s="243" t="s">
         <v>1187</v>
       </c>
-      <c r="D42" s="240"/>
-      <c r="E42" s="221"/>
-      <c r="F42" s="221"/>
+      <c r="D42" s="243"/>
+      <c r="E42" s="224"/>
+      <c r="F42" s="224"/>
     </row>
     <row r="43">
-      <c r="A43" s="217" t="s">
+      <c r="A43" s="220" t="s">
         <v>1188</v>
       </c>
-      <c r="B43" s="241" t="s">
+      <c r="B43" s="244" t="s">
         <v>1189</v>
       </c>
-      <c r="C43" s="240" t="s">
+      <c r="C43" s="243" t="s">
         <v>1190</v>
       </c>
-      <c r="D43" s="240"/>
-      <c r="E43" s="221"/>
-      <c r="F43" s="221"/>
+      <c r="D43" s="243"/>
+      <c r="E43" s="224"/>
+      <c r="F43" s="224"/>
     </row>
     <row r="44">
-      <c r="A44" s="217" t="s">
+      <c r="A44" s="220" t="s">
         <v>1191</v>
       </c>
-      <c r="B44" s="241" t="s">
+      <c r="B44" s="244" t="s">
         <v>1192</v>
       </c>
-      <c r="C44" s="242" t="s">
+      <c r="C44" s="245" t="s">
         <v>1193</v>
       </c>
-      <c r="D44" s="242"/>
-      <c r="E44" s="221"/>
-      <c r="F44" s="221"/>
+      <c r="D44" s="245"/>
+      <c r="E44" s="224"/>
+      <c r="F44" s="224"/>
     </row>
     <row r="45" ht="20.25" customHeight="1">
-      <c r="A45" s="217" t="s">
+      <c r="A45" s="220" t="s">
         <v>1194</v>
       </c>
       <c r="B45" s="14" t="s">
         <v>1195</v>
       </c>
-      <c r="C45" s="243" t="s">
+      <c r="C45" s="246" t="s">
         <v>308</v>
       </c>
-      <c r="D45" s="243"/>
+      <c r="D45" s="246"/>
       <c r="E45" s="16"/>
       <c r="F45" s="50"/>
     </row>
     <row r="46">
-      <c r="A46" s="217" t="s">
+      <c r="A46" s="220" t="s">
         <v>1196</v>
       </c>
       <c r="B46" s="14" t="s">
@@ -16704,35 +16719,35 @@
       <c r="F46" s="50"/>
     </row>
     <row r="47">
-      <c r="A47" s="217" t="s">
+      <c r="A47" s="220" t="s">
         <v>1198</v>
       </c>
       <c r="B47" s="14" t="s">
         <v>1199</v>
       </c>
-      <c r="C47" s="220" t="s">
+      <c r="C47" s="223" t="s">
         <v>315</v>
       </c>
-      <c r="D47" s="220"/>
+      <c r="D47" s="223"/>
       <c r="E47" s="16"/>
       <c r="F47" s="30"/>
     </row>
     <row r="48">
-      <c r="A48" s="217" t="s">
+      <c r="A48" s="220" t="s">
         <v>1200</v>
       </c>
       <c r="B48" s="14" t="s">
         <v>1201</v>
       </c>
-      <c r="C48" s="220" t="s">
+      <c r="C48" s="223" t="s">
         <v>318</v>
       </c>
-      <c r="D48" s="220"/>
+      <c r="D48" s="223"/>
       <c r="E48" s="16"/>
       <c r="F48" s="30"/>
     </row>
     <row r="49">
-      <c r="A49" s="217" t="s">
+      <c r="A49" s="220" t="s">
         <v>1202</v>
       </c>
       <c r="B49" s="14" t="s">
@@ -16746,7 +16761,7 @@
       <c r="F49" s="30"/>
     </row>
     <row r="50">
-      <c r="A50" s="217" t="s">
+      <c r="A50" s="220" t="s">
         <v>1204</v>
       </c>
       <c r="B50" s="14" t="s">
@@ -16760,21 +16775,21 @@
       <c r="F50" s="30"/>
     </row>
     <row r="51">
-      <c r="A51" s="217" t="s">
+      <c r="A51" s="220" t="s">
         <v>1206</v>
       </c>
       <c r="B51" s="14" t="s">
         <v>1207</v>
       </c>
-      <c r="C51" s="220" t="s">
+      <c r="C51" s="223" t="s">
         <v>327</v>
       </c>
-      <c r="D51" s="220"/>
+      <c r="D51" s="223"/>
       <c r="E51" s="16"/>
       <c r="F51" s="30"/>
     </row>
     <row r="52">
-      <c r="A52" s="217" t="s">
+      <c r="A52" s="220" t="s">
         <v>1208</v>
       </c>
       <c r="B52" s="14" t="s">
@@ -16788,35 +16803,35 @@
       <c r="F52" s="30"/>
     </row>
     <row r="53">
-      <c r="A53" s="217" t="s">
+      <c r="A53" s="220" t="s">
         <v>1210</v>
       </c>
       <c r="B53" s="14" t="s">
         <v>1211</v>
       </c>
-      <c r="C53" s="220" t="s">
+      <c r="C53" s="223" t="s">
         <v>333</v>
       </c>
-      <c r="D53" s="220"/>
+      <c r="D53" s="223"/>
       <c r="E53" s="16"/>
       <c r="F53" s="30"/>
     </row>
     <row r="54">
-      <c r="A54" s="244" t="s">
+      <c r="A54" s="247" t="s">
         <v>1212</v>
       </c>
-      <c r="B54" s="245" t="s">
+      <c r="B54" s="248" t="s">
         <v>1213</v>
       </c>
-      <c r="C54" s="246" t="s">
+      <c r="C54" s="249" t="s">
         <v>336</v>
       </c>
-      <c r="D54" s="246"/>
-      <c r="E54" s="247"/>
-      <c r="F54" s="248"/>
+      <c r="D54" s="249"/>
+      <c r="E54" s="250"/>
+      <c r="F54" s="251"/>
     </row>
     <row r="55">
-      <c r="A55" s="217" t="s">
+      <c r="A55" s="220" t="s">
         <v>1214</v>
       </c>
       <c r="B55" s="5" t="s">
@@ -16888,7 +16903,7 @@
         <v>269</v>
       </c>
       <c r="F2" s="27"/>
-      <c r="G2" s="249"/>
+      <c r="G2" s="252"/>
     </row>
     <row r="3">
       <c r="A3" s="24" t="s">
@@ -17659,7 +17674,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="250" t="s">
+      <c r="A1" s="253" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="108" t="s">
@@ -17668,19 +17683,19 @@
       <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="250" t="s">
+      <c r="D1" s="253" t="s">
         <v>462</v>
       </c>
-      <c r="E1" s="250" t="s">
+      <c r="E1" s="253" t="s">
         <v>1265</v>
       </c>
-      <c r="F1" s="250" t="s">
+      <c r="F1" s="253" t="s">
         <v>1266</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>1267</v>
       </c>
-      <c r="H1" s="251" t="s">
+      <c r="H1" s="254" t="s">
         <v>471</v>
       </c>
       <c r="I1" s="5" t="s">
@@ -17700,9 +17715,9 @@
       <c r="C2" s="5" t="s">
         <v>1271</v>
       </c>
-      <c r="D2" s="252"/>
-      <c r="F2" s="251"/>
-      <c r="H2" s="253"/>
+      <c r="D2" s="255"/>
+      <c r="F2" s="254"/>
+      <c r="H2" s="256"/>
       <c r="J2" s="5" t="s">
         <v>1272</v>
       </c>
@@ -17717,10 +17732,10 @@
       <c r="C3" s="5" t="s">
         <v>1274</v>
       </c>
-      <c r="D3" s="253"/>
-      <c r="E3" s="251"/>
-      <c r="F3" s="251"/>
-      <c r="H3" s="251"/>
+      <c r="D3" s="256"/>
+      <c r="E3" s="254"/>
+      <c r="F3" s="254"/>
+      <c r="H3" s="254"/>
       <c r="J3" s="5" t="s">
         <v>1275</v>
       </c>
@@ -17735,10 +17750,10 @@
       <c r="C4" s="5" t="s">
         <v>1277</v>
       </c>
-      <c r="D4" s="253"/>
-      <c r="E4" s="251"/>
-      <c r="F4" s="251"/>
-      <c r="H4" s="251"/>
+      <c r="D4" s="256"/>
+      <c r="E4" s="254"/>
+      <c r="F4" s="254"/>
+      <c r="H4" s="254"/>
       <c r="J4" s="5" t="s">
         <v>1275</v>
       </c>
@@ -17753,10 +17768,10 @@
       <c r="C5" s="5" t="s">
         <v>1279</v>
       </c>
-      <c r="D5" s="251"/>
-      <c r="E5" s="251"/>
-      <c r="F5" s="251"/>
-      <c r="H5" s="253"/>
+      <c r="D5" s="254"/>
+      <c r="E5" s="254"/>
+      <c r="F5" s="254"/>
+      <c r="H5" s="256"/>
       <c r="J5" s="5" t="s">
         <v>1280</v>
       </c>
@@ -17771,9 +17786,9 @@
       <c r="C6" s="5" t="s">
         <v>1282</v>
       </c>
-      <c r="D6" s="251"/>
+      <c r="D6" s="254"/>
       <c r="E6" s="116"/>
-      <c r="F6" s="254"/>
+      <c r="F6" s="257"/>
       <c r="H6" s="5" t="s">
         <v>458</v>
       </c>
@@ -17791,10 +17806,10 @@
       <c r="C7" s="5" t="s">
         <v>1285</v>
       </c>
-      <c r="D7" s="251"/>
-      <c r="E7" s="251"/>
-      <c r="F7" s="251"/>
-      <c r="H7" s="251"/>
+      <c r="D7" s="254"/>
+      <c r="E7" s="254"/>
+      <c r="F7" s="254"/>
+      <c r="H7" s="254"/>
       <c r="J7" s="5" t="s">
         <v>1286</v>
       </c>
@@ -17809,11 +17824,11 @@
       <c r="C8" s="5" t="s">
         <v>1288</v>
       </c>
-      <c r="D8" s="251"/>
-      <c r="E8" s="251"/>
-      <c r="F8" s="251"/>
-      <c r="G8" s="251"/>
-      <c r="H8" s="251"/>
+      <c r="D8" s="254"/>
+      <c r="E8" s="254"/>
+      <c r="F8" s="254"/>
+      <c r="G8" s="254"/>
+      <c r="H8" s="254"/>
       <c r="J8" s="5" t="s">
         <v>1289</v>
       </c>
@@ -17828,10 +17843,10 @@
       <c r="C9" s="5" t="s">
         <v>1291</v>
       </c>
-      <c r="D9" s="251"/>
-      <c r="E9" s="251"/>
-      <c r="F9" s="251"/>
-      <c r="H9" s="251"/>
+      <c r="D9" s="254"/>
+      <c r="E9" s="254"/>
+      <c r="F9" s="254"/>
+      <c r="H9" s="254"/>
       <c r="J9" s="5" t="s">
         <v>1286</v>
       </c>
@@ -17846,10 +17861,10 @@
       <c r="C10" s="5" t="s">
         <v>1293</v>
       </c>
-      <c r="D10" s="251"/>
-      <c r="E10" s="251"/>
-      <c r="F10" s="251"/>
-      <c r="H10" s="253"/>
+      <c r="D10" s="254"/>
+      <c r="E10" s="254"/>
+      <c r="F10" s="254"/>
+      <c r="H10" s="256"/>
       <c r="J10" s="5" t="s">
         <v>1294</v>
       </c>
@@ -17864,11 +17879,11 @@
       <c r="C11" s="5" t="s">
         <v>1296</v>
       </c>
-      <c r="D11" s="251"/>
-      <c r="E11" s="251"/>
-      <c r="F11" s="251"/>
-      <c r="G11" s="251"/>
-      <c r="H11" s="251"/>
+      <c r="D11" s="254"/>
+      <c r="E11" s="254"/>
+      <c r="F11" s="254"/>
+      <c r="G11" s="254"/>
+      <c r="H11" s="254"/>
       <c r="J11" s="14" t="s">
         <v>1275</v>
       </c>
@@ -17883,11 +17898,11 @@
       <c r="C12" s="5" t="s">
         <v>1298</v>
       </c>
-      <c r="D12" s="251"/>
-      <c r="E12" s="251"/>
-      <c r="F12" s="251"/>
-      <c r="G12" s="251"/>
-      <c r="H12" s="251"/>
+      <c r="D12" s="254"/>
+      <c r="E12" s="254"/>
+      <c r="F12" s="254"/>
+      <c r="G12" s="254"/>
+      <c r="H12" s="254"/>
       <c r="J12" s="5" t="s">
         <v>1289</v>
       </c>
@@ -17902,10 +17917,10 @@
       <c r="C13" s="5" t="s">
         <v>1300</v>
       </c>
-      <c r="D13" s="251"/>
-      <c r="E13" s="251"/>
-      <c r="F13" s="251"/>
-      <c r="H13" s="251"/>
+      <c r="D13" s="254"/>
+      <c r="E13" s="254"/>
+      <c r="F13" s="254"/>
+      <c r="H13" s="254"/>
       <c r="J13" s="5" t="s">
         <v>1286</v>
       </c>
@@ -17920,10 +17935,10 @@
       <c r="C14" s="5" t="s">
         <v>1302</v>
       </c>
-      <c r="D14" s="251"/>
-      <c r="E14" s="251"/>
-      <c r="F14" s="251"/>
-      <c r="H14" s="253"/>
+      <c r="D14" s="254"/>
+      <c r="E14" s="254"/>
+      <c r="F14" s="254"/>
+      <c r="H14" s="256"/>
       <c r="J14" s="5" t="s">
         <v>1294</v>
       </c>
@@ -17938,11 +17953,11 @@
       <c r="C15" s="5" t="s">
         <v>1304</v>
       </c>
-      <c r="D15" s="251"/>
-      <c r="E15" s="251"/>
-      <c r="F15" s="251"/>
-      <c r="G15" s="251"/>
-      <c r="H15" s="251"/>
+      <c r="D15" s="254"/>
+      <c r="E15" s="254"/>
+      <c r="F15" s="254"/>
+      <c r="G15" s="254"/>
+      <c r="H15" s="254"/>
       <c r="J15" s="14" t="s">
         <v>1275</v>
       </c>
@@ -17957,13 +17972,13 @@
       <c r="C16" s="5" t="s">
         <v>1306</v>
       </c>
-      <c r="D16" s="253"/>
-      <c r="E16" s="251"/>
-      <c r="F16" s="251"/>
+      <c r="D16" s="256"/>
+      <c r="E16" s="254"/>
+      <c r="F16" s="254"/>
       <c r="H16" s="5" t="s">
         <v>458</v>
       </c>
-      <c r="J16" s="255" t="s">
+      <c r="J16" s="258" t="s">
         <v>1294</v>
       </c>
     </row>
@@ -17977,12 +17992,12 @@
       <c r="C17" s="5" t="s">
         <v>1308</v>
       </c>
-      <c r="E17" s="251"/>
-      <c r="F17" s="256"/>
-      <c r="H17" s="257" t="s">
+      <c r="E17" s="254"/>
+      <c r="F17" s="259"/>
+      <c r="H17" s="260" t="s">
         <v>1309</v>
       </c>
-      <c r="J17" s="255" t="s">
+      <c r="J17" s="258" t="s">
         <v>1294</v>
       </c>
     </row>
@@ -17996,12 +18011,12 @@
       <c r="C18" s="5" t="s">
         <v>1311</v>
       </c>
-      <c r="E18" s="251"/>
-      <c r="F18" s="256"/>
+      <c r="E18" s="254"/>
+      <c r="F18" s="259"/>
       <c r="H18" s="5" t="s">
         <v>458</v>
       </c>
-      <c r="J18" s="255" t="s">
+      <c r="J18" s="258" t="s">
         <v>1294</v>
       </c>
     </row>
@@ -18032,7 +18047,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="258" t="s">
+      <c r="A2" s="261" t="s">
         <v>1313</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -18043,7 +18058,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="258" t="s">
+      <c r="A3" s="261" t="s">
         <v>1316</v>
       </c>
       <c r="B3" s="5" t="s">
@@ -18054,7 +18069,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="258" t="s">
+      <c r="A4" s="261" t="s">
         <v>1318</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -18074,7 +18089,7 @@
     </row>
     <row r="6">
       <c r="A6" s="5"/>
-      <c r="B6" s="259" t="s">
+      <c r="B6" s="262" t="s">
         <v>1321</v>
       </c>
       <c r="C6" s="5" t="s">
@@ -18083,7 +18098,7 @@
     </row>
     <row r="7">
       <c r="A7" s="5"/>
-      <c r="B7" s="259" t="s">
+      <c r="B7" s="262" t="s">
         <v>1323</v>
       </c>
       <c r="C7" s="5" t="s">

</xml_diff>

<commit_message>
aacar-6 fix axon routing issue in ventricles
</commit_message>
<xml_diff>
--- a/models/ard-arm-cardiac/source/ard-arm-cardiac.xlsx
+++ b/models/ard-arm-cardiac/source/ard-arm-cardiac.xlsx
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2398" uniqueCount="1393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2398" uniqueCount="1392">
   <si>
     <t>id</t>
   </si>
@@ -2209,7 +2209,7 @@
     <t>ns103_1</t>
   </si>
   <si>
-    <t>A74, A76, A78</t>
+    <t>A74, A78, A78</t>
   </si>
   <si>
     <t>ac-sn-aicg_6</t>
@@ -2408,9 +2408,6 @@
   </si>
   <si>
     <t>ns118_1</t>
-  </si>
-  <si>
-    <t>A74, A78, A78</t>
   </si>
   <si>
     <t>ac-rv0_7</t>
@@ -5711,114 +5708,114 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="108" t="s">
+        <v>1323</v>
+      </c>
+      <c r="B1" s="108" t="s">
         <v>1324</v>
-      </c>
-      <c r="B1" s="108" t="s">
-        <v>1325</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="263" t="s">
+        <v>1325</v>
+      </c>
+      <c r="B2" s="264" t="s">
         <v>1326</v>
-      </c>
-      <c r="B2" s="264" t="s">
-        <v>1327</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="263" t="s">
+        <v>1327</v>
+      </c>
+      <c r="B3" s="265" t="s">
         <v>1328</v>
-      </c>
-      <c r="B3" s="265" t="s">
-        <v>1329</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="263" t="s">
+        <v>1329</v>
+      </c>
+      <c r="B4" s="266" t="s">
         <v>1330</v>
-      </c>
-      <c r="B4" s="266" t="s">
-        <v>1331</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="263" t="s">
+        <v>1331</v>
+      </c>
+      <c r="B5" s="266" t="s">
         <v>1332</v>
-      </c>
-      <c r="B5" s="266" t="s">
-        <v>1333</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="263" t="s">
+        <v>1333</v>
+      </c>
+      <c r="B6" s="266" t="s">
         <v>1334</v>
-      </c>
-      <c r="B6" s="266" t="s">
-        <v>1335</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="263" t="s">
+        <v>1335</v>
+      </c>
+      <c r="B7" s="266" t="s">
         <v>1336</v>
-      </c>
-      <c r="B7" s="266" t="s">
-        <v>1337</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="263" t="s">
+        <v>1337</v>
+      </c>
+      <c r="B8" s="266" t="s">
         <v>1338</v>
-      </c>
-      <c r="B8" s="266" t="s">
-        <v>1339</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="263" t="s">
+        <v>1339</v>
+      </c>
+      <c r="B9" s="266" t="s">
         <v>1340</v>
-      </c>
-      <c r="B9" s="266" t="s">
-        <v>1341</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="263" t="s">
+        <v>1341</v>
+      </c>
+      <c r="B10" s="266" t="s">
         <v>1342</v>
-      </c>
-      <c r="B10" s="266" t="s">
-        <v>1343</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="263" t="s">
+        <v>1343</v>
+      </c>
+      <c r="B11" s="266" t="s">
         <v>1344</v>
-      </c>
-      <c r="B11" s="266" t="s">
-        <v>1345</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="5" t="s">
+        <v>1345</v>
+      </c>
+      <c r="B12" s="267" t="s">
         <v>1346</v>
-      </c>
-      <c r="B12" s="267" t="s">
-        <v>1347</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="25" t="s">
+        <v>1347</v>
+      </c>
+      <c r="B13" s="268" t="s">
         <v>1348</v>
-      </c>
-      <c r="B13" s="268" t="s">
-        <v>1349</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="25" t="s">
+        <v>1349</v>
+      </c>
+      <c r="B14" s="269" t="s">
         <v>1350</v>
-      </c>
-      <c r="B14" s="269" t="s">
-        <v>1351</v>
       </c>
     </row>
   </sheetData>
@@ -5853,16 +5850,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="16" t="s">
+        <v>1351</v>
+      </c>
+      <c r="B1" s="16" t="s">
         <v>1352</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="C1" s="16" t="s">
         <v>1353</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="D1" s="16" t="s">
         <v>1354</v>
-      </c>
-      <c r="D1" s="16" t="s">
-        <v>1355</v>
       </c>
       <c r="E1" s="16"/>
       <c r="F1" s="16"/>
@@ -5878,13 +5875,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="16" t="s">
+        <v>1355</v>
+      </c>
+      <c r="C2" s="16" t="s">
         <v>1356</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="D2" s="16" t="s">
         <v>1357</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>1358</v>
       </c>
       <c r="E2" s="16"/>
       <c r="F2" s="16"/>
@@ -5925,13 +5922,13 @@
     </row>
     <row r="5">
       <c r="A5" s="16" t="s">
+        <v>1358</v>
+      </c>
+      <c r="B5" s="16" t="s">
         <v>1359</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="C5" s="16" t="s">
         <v>1360</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>1361</v>
       </c>
       <c r="D5" s="16"/>
       <c r="E5" s="16"/>
@@ -5948,10 +5945,10 @@
         <v>0</v>
       </c>
       <c r="B6" s="16" t="s">
+        <v>1361</v>
+      </c>
+      <c r="C6" s="14" t="s">
         <v>1362</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>1363</v>
       </c>
       <c r="D6" s="16"/>
       <c r="E6" s="16"/>
@@ -5966,10 +5963,10 @@
     <row r="7">
       <c r="A7" s="16"/>
       <c r="B7" s="16" t="s">
-        <v>1364</v>
+        <v>1363</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>1363</v>
+        <v>1362</v>
       </c>
       <c r="D7" s="16"/>
       <c r="E7" s="16"/>
@@ -5984,10 +5981,10 @@
     <row r="8">
       <c r="A8" s="16"/>
       <c r="B8" s="16" t="s">
-        <v>1365</v>
+        <v>1364</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>1363</v>
+        <v>1362</v>
       </c>
       <c r="D8" s="16"/>
       <c r="E8" s="16"/>
@@ -6002,10 +5999,10 @@
     <row r="9">
       <c r="A9" s="16"/>
       <c r="B9" s="16" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1363</v>
+        <v>1362</v>
       </c>
       <c r="D9" s="16"/>
       <c r="E9" s="16"/>
@@ -6033,10 +6030,10 @@
     </row>
     <row r="11">
       <c r="A11" s="16" t="s">
+        <v>1366</v>
+      </c>
+      <c r="B11" s="16" t="s">
         <v>1367</v>
-      </c>
-      <c r="B11" s="16" t="s">
-        <v>1368</v>
       </c>
       <c r="C11" s="16"/>
       <c r="D11" s="16"/>
@@ -6051,10 +6048,10 @@
     </row>
     <row r="12">
       <c r="A12" s="16" t="s">
+        <v>1368</v>
+      </c>
+      <c r="B12" s="270" t="s">
         <v>1369</v>
-      </c>
-      <c r="B12" s="270" t="s">
-        <v>1370</v>
       </c>
       <c r="C12" s="16"/>
       <c r="D12" s="16"/>
@@ -6069,10 +6066,10 @@
     </row>
     <row r="13">
       <c r="A13" s="16" t="s">
+        <v>1370</v>
+      </c>
+      <c r="B13" s="270" t="s">
         <v>1371</v>
-      </c>
-      <c r="B13" s="270" t="s">
-        <v>1372</v>
       </c>
       <c r="C13" s="16"/>
       <c r="D13" s="16"/>
@@ -6087,10 +6084,10 @@
     </row>
     <row r="14">
       <c r="A14" s="16" t="s">
+        <v>1372</v>
+      </c>
+      <c r="B14" s="270" t="s">
         <v>1373</v>
-      </c>
-      <c r="B14" s="270" t="s">
-        <v>1374</v>
       </c>
       <c r="C14" s="16"/>
       <c r="D14" s="16"/>
@@ -6105,10 +6102,10 @@
     </row>
     <row r="15">
       <c r="A15" s="16" t="s">
+        <v>1374</v>
+      </c>
+      <c r="B15" s="270" t="s">
         <v>1375</v>
-      </c>
-      <c r="B15" s="270" t="s">
-        <v>1376</v>
       </c>
       <c r="C15" s="16"/>
       <c r="D15" s="16"/>
@@ -6123,10 +6120,10 @@
     </row>
     <row r="16">
       <c r="A16" s="14" t="s">
+        <v>1376</v>
+      </c>
+      <c r="B16" s="93" t="s">
         <v>1377</v>
-      </c>
-      <c r="B16" s="93" t="s">
-        <v>1378</v>
       </c>
       <c r="C16" s="16"/>
       <c r="D16" s="16"/>
@@ -6141,10 +6138,10 @@
     </row>
     <row r="17">
       <c r="A17" s="14" t="s">
-        <v>1379</v>
+        <v>1378</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
       <c r="C17" s="16"/>
       <c r="D17" s="16"/>
@@ -6173,10 +6170,10 @@
     </row>
     <row r="19">
       <c r="A19" s="16" t="s">
+        <v>1379</v>
+      </c>
+      <c r="B19" s="93" t="s">
         <v>1380</v>
-      </c>
-      <c r="B19" s="93" t="s">
-        <v>1381</v>
       </c>
       <c r="C19" s="16"/>
       <c r="D19" s="16"/>
@@ -6191,7 +6188,7 @@
     </row>
     <row r="20">
       <c r="A20" s="16" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
       <c r="B20" s="116" t="s">
         <v>6</v>
@@ -6209,10 +6206,10 @@
     </row>
     <row r="21">
       <c r="A21" s="16" t="s">
+        <v>1382</v>
+      </c>
+      <c r="B21" s="116" t="s">
         <v>1383</v>
-      </c>
-      <c r="B21" s="116" t="s">
-        <v>1384</v>
       </c>
       <c r="L21" s="16"/>
     </row>
@@ -6242,28 +6239,28 @@
     </row>
     <row r="28">
       <c r="A28" s="271" t="s">
+        <v>1384</v>
+      </c>
+      <c r="B28" s="272" t="s">
         <v>1385</v>
-      </c>
-      <c r="B28" s="272" t="s">
-        <v>1386</v>
       </c>
       <c r="L28" s="16"/>
     </row>
     <row r="29">
       <c r="A29" s="271" t="s">
+        <v>1386</v>
+      </c>
+      <c r="B29" s="273" t="s">
         <v>1387</v>
-      </c>
-      <c r="B29" s="273" t="s">
-        <v>1388</v>
       </c>
       <c r="L29" s="16"/>
     </row>
     <row r="30">
       <c r="A30" s="271" t="s">
+        <v>1388</v>
+      </c>
+      <c r="B30" s="267" t="s">
         <v>1389</v>
-      </c>
-      <c r="B30" s="267" t="s">
-        <v>1390</v>
       </c>
       <c r="C30" s="272"/>
       <c r="D30" s="272"/>
@@ -6278,13 +6275,13 @@
     </row>
     <row r="31" hidden="1">
       <c r="A31" s="16" t="s">
-        <v>1391</v>
+        <v>1390</v>
       </c>
       <c r="L31" s="16"/>
     </row>
     <row r="32" hidden="1">
       <c r="A32" s="16" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
       <c r="L32" s="16"/>
     </row>
@@ -13565,17 +13562,17 @@
         <v>709</v>
       </c>
       <c r="L91" s="121" t="s">
-        <v>785</v>
+        <v>718</v>
       </c>
       <c r="M91" s="121"/>
       <c r="N91" s="34"/>
     </row>
     <row r="92">
       <c r="A92" s="127" t="s">
+        <v>785</v>
+      </c>
+      <c r="B92" s="134" t="s">
         <v>786</v>
-      </c>
-      <c r="B92" s="134" t="s">
-        <v>787</v>
       </c>
       <c r="C92" s="148" t="s">
         <v>484</v>
@@ -13588,7 +13585,7 @@
         <v>774</v>
       </c>
       <c r="G92" s="130" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="H92" s="142"/>
       <c r="I92" s="133"/>
@@ -13604,10 +13601,10 @@
     </row>
     <row r="93">
       <c r="A93" s="127" t="s">
+        <v>788</v>
+      </c>
+      <c r="B93" s="134" t="s">
         <v>789</v>
-      </c>
-      <c r="B93" s="134" t="s">
-        <v>790</v>
       </c>
       <c r="C93" s="148" t="s">
         <v>484</v>
@@ -13620,7 +13617,7 @@
         <v>774</v>
       </c>
       <c r="G93" s="130" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="H93" s="142"/>
       <c r="I93" s="133"/>
@@ -13636,10 +13633,10 @@
     </row>
     <row r="94">
       <c r="A94" s="24" t="s">
+        <v>791</v>
+      </c>
+      <c r="B94" s="123" t="s">
         <v>792</v>
-      </c>
-      <c r="B94" s="123" t="s">
-        <v>793</v>
       </c>
       <c r="C94" s="156" t="s">
         <v>480</v>
@@ -13649,7 +13646,7 @@
         <v>370</v>
       </c>
       <c r="F94" s="14" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="G94" s="48"/>
       <c r="H94" s="13"/>
@@ -13666,10 +13663,10 @@
     </row>
     <row r="95">
       <c r="A95" s="24" t="s">
+        <v>794</v>
+      </c>
+      <c r="B95" s="123" t="s">
         <v>795</v>
-      </c>
-      <c r="B95" s="123" t="s">
-        <v>796</v>
       </c>
       <c r="C95" s="156" t="s">
         <v>484</v>
@@ -13679,10 +13676,10 @@
         <v>367</v>
       </c>
       <c r="F95" s="14" t="s">
+        <v>796</v>
+      </c>
+      <c r="G95" s="14" t="s">
         <v>797</v>
-      </c>
-      <c r="G95" s="14" t="s">
-        <v>798</v>
       </c>
       <c r="H95" s="13"/>
       <c r="I95" s="16"/>
@@ -13698,10 +13695,10 @@
     </row>
     <row r="96">
       <c r="A96" s="24" t="s">
+        <v>798</v>
+      </c>
+      <c r="B96" s="123" t="s">
         <v>799</v>
-      </c>
-      <c r="B96" s="123" t="s">
-        <v>800</v>
       </c>
       <c r="C96" s="156" t="s">
         <v>484</v>
@@ -13711,10 +13708,10 @@
         <v>363</v>
       </c>
       <c r="F96" s="14" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="G96" s="5" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="H96" s="13"/>
       <c r="I96" s="16"/>
@@ -13730,10 +13727,10 @@
     </row>
     <row r="97">
       <c r="A97" s="24" t="s">
+        <v>801</v>
+      </c>
+      <c r="B97" s="123" t="s">
         <v>802</v>
-      </c>
-      <c r="B97" s="123" t="s">
-        <v>803</v>
       </c>
       <c r="C97" s="156" t="s">
         <v>484</v>
@@ -13743,10 +13740,10 @@
         <v>363</v>
       </c>
       <c r="F97" s="14" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="G97" s="5" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="H97" s="13"/>
       <c r="I97" s="16"/>
@@ -13762,10 +13759,10 @@
     </row>
     <row r="98">
       <c r="A98" s="24" t="s">
+        <v>804</v>
+      </c>
+      <c r="B98" s="123" t="s">
         <v>805</v>
-      </c>
-      <c r="B98" s="123" t="s">
-        <v>806</v>
       </c>
       <c r="C98" s="156" t="s">
         <v>484</v>
@@ -13775,10 +13772,10 @@
         <v>363</v>
       </c>
       <c r="F98" s="14" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="G98" s="5" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="H98" s="13"/>
       <c r="I98" s="16"/>
@@ -13794,10 +13791,10 @@
     </row>
     <row r="99">
       <c r="A99" s="24" t="s">
+        <v>807</v>
+      </c>
+      <c r="B99" s="123" t="s">
         <v>808</v>
-      </c>
-      <c r="B99" s="123" t="s">
-        <v>809</v>
       </c>
       <c r="C99" s="156" t="s">
         <v>484</v>
@@ -13807,10 +13804,10 @@
         <v>363</v>
       </c>
       <c r="F99" s="14" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="G99" s="14" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="H99" s="13"/>
       <c r="I99" s="16"/>
@@ -13826,10 +13823,10 @@
     </row>
     <row r="100">
       <c r="A100" s="24" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="B100" s="123" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="C100" s="156" t="s">
         <v>484</v>
@@ -13839,10 +13836,10 @@
         <v>363</v>
       </c>
       <c r="F100" s="14" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="G100" s="14" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="H100" s="13"/>
       <c r="I100" s="16"/>
@@ -13858,10 +13855,10 @@
     </row>
     <row r="101">
       <c r="A101" s="24" t="s">
+        <v>812</v>
+      </c>
+      <c r="B101" s="123" t="s">
         <v>813</v>
-      </c>
-      <c r="B101" s="123" t="s">
-        <v>814</v>
       </c>
       <c r="C101" s="156" t="s">
         <v>480</v>
@@ -13871,7 +13868,7 @@
         <v>370</v>
       </c>
       <c r="F101" s="14" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="G101" s="25"/>
       <c r="H101" s="13"/>
@@ -13888,10 +13885,10 @@
     </row>
     <row r="102">
       <c r="A102" s="24" t="s">
+        <v>815</v>
+      </c>
+      <c r="B102" s="123" t="s">
         <v>816</v>
-      </c>
-      <c r="B102" s="123" t="s">
-        <v>817</v>
       </c>
       <c r="C102" s="156" t="s">
         <v>484</v>
@@ -13901,10 +13898,10 @@
         <v>367</v>
       </c>
       <c r="F102" s="14" t="s">
+        <v>817</v>
+      </c>
+      <c r="G102" s="14" t="s">
         <v>818</v>
-      </c>
-      <c r="G102" s="14" t="s">
-        <v>819</v>
       </c>
       <c r="H102" s="13"/>
       <c r="I102" s="16"/>
@@ -13913,17 +13910,17 @@
         <v>524</v>
       </c>
       <c r="L102" s="123" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="M102" s="123"/>
       <c r="N102" s="16"/>
     </row>
     <row r="103">
       <c r="A103" s="24" t="s">
+        <v>820</v>
+      </c>
+      <c r="B103" s="123" t="s">
         <v>821</v>
-      </c>
-      <c r="B103" s="123" t="s">
-        <v>822</v>
       </c>
       <c r="C103" s="156" t="s">
         <v>484</v>
@@ -13933,10 +13930,10 @@
         <v>363</v>
       </c>
       <c r="F103" s="14" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="G103" s="14" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="H103" s="13"/>
       <c r="I103" s="16"/>
@@ -13952,10 +13949,10 @@
     </row>
     <row r="104">
       <c r="A104" s="24" t="s">
+        <v>823</v>
+      </c>
+      <c r="B104" s="123" t="s">
         <v>824</v>
-      </c>
-      <c r="B104" s="123" t="s">
-        <v>825</v>
       </c>
       <c r="C104" s="156" t="s">
         <v>484</v>
@@ -13965,10 +13962,10 @@
         <v>363</v>
       </c>
       <c r="F104" s="14" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="G104" s="14" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="H104" s="13"/>
       <c r="I104" s="16"/>
@@ -13984,10 +13981,10 @@
     </row>
     <row r="105">
       <c r="A105" s="24" t="s">
+        <v>826</v>
+      </c>
+      <c r="B105" s="123" t="s">
         <v>827</v>
-      </c>
-      <c r="B105" s="123" t="s">
-        <v>828</v>
       </c>
       <c r="C105" s="156" t="s">
         <v>484</v>
@@ -13997,10 +13994,10 @@
         <v>363</v>
       </c>
       <c r="F105" s="14" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="G105" s="14" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="H105" s="13"/>
       <c r="I105" s="16"/>
@@ -14009,17 +14006,17 @@
         <v>709</v>
       </c>
       <c r="L105" s="123" t="s">
-        <v>785</v>
+        <v>718</v>
       </c>
       <c r="M105" s="123"/>
       <c r="N105" s="16"/>
     </row>
     <row r="106">
       <c r="A106" s="127" t="s">
+        <v>829</v>
+      </c>
+      <c r="B106" s="134" t="s">
         <v>830</v>
-      </c>
-      <c r="B106" s="134" t="s">
-        <v>831</v>
       </c>
       <c r="C106" s="148" t="s">
         <v>484</v>
@@ -14029,10 +14026,10 @@
         <v>363</v>
       </c>
       <c r="F106" s="130" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="G106" s="130" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="H106" s="142"/>
       <c r="I106" s="133"/>
@@ -14048,10 +14045,10 @@
     </row>
     <row r="107">
       <c r="A107" s="24" t="s">
+        <v>832</v>
+      </c>
+      <c r="B107" s="123" t="s">
         <v>833</v>
-      </c>
-      <c r="B107" s="123" t="s">
-        <v>834</v>
       </c>
       <c r="C107" s="156" t="s">
         <v>484</v>
@@ -14061,10 +14058,10 @@
         <v>363</v>
       </c>
       <c r="F107" s="14" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="G107" s="189" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="H107" s="13"/>
       <c r="I107" s="16"/>
@@ -14080,10 +14077,10 @@
     </row>
     <row r="108">
       <c r="A108" s="190" t="s">
+        <v>834</v>
+      </c>
+      <c r="B108" s="123" t="s">
         <v>835</v>
-      </c>
-      <c r="B108" s="123" t="s">
-        <v>836</v>
       </c>
       <c r="C108" s="145" t="s">
         <v>480</v>
@@ -14093,7 +14090,7 @@
         <v>363</v>
       </c>
       <c r="F108" s="32" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="G108" s="138"/>
       <c r="H108" s="36"/>
@@ -14110,10 +14107,10 @@
     </row>
     <row r="109">
       <c r="A109" s="191" t="s">
+        <v>837</v>
+      </c>
+      <c r="B109" s="192" t="s">
         <v>838</v>
-      </c>
-      <c r="B109" s="192" t="s">
-        <v>839</v>
       </c>
       <c r="C109" s="193" t="s">
         <v>484</v>
@@ -14123,10 +14120,10 @@
         <v>373</v>
       </c>
       <c r="F109" s="32" t="s">
+        <v>839</v>
+      </c>
+      <c r="G109" s="32" t="s">
         <v>840</v>
-      </c>
-      <c r="G109" s="32" t="s">
-        <v>841</v>
       </c>
       <c r="H109" s="36"/>
       <c r="I109" s="34"/>
@@ -14142,10 +14139,10 @@
     </row>
     <row r="110">
       <c r="A110" s="191" t="s">
+        <v>841</v>
+      </c>
+      <c r="B110" s="192" t="s">
         <v>842</v>
-      </c>
-      <c r="B110" s="192" t="s">
-        <v>843</v>
       </c>
       <c r="C110" s="193" t="s">
         <v>484</v>
@@ -14155,10 +14152,10 @@
         <v>370</v>
       </c>
       <c r="F110" s="32" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="G110" s="143" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="H110" s="36"/>
       <c r="I110" s="34"/>
@@ -14174,10 +14171,10 @@
     </row>
     <row r="111">
       <c r="A111" s="191" t="s">
+        <v>844</v>
+      </c>
+      <c r="B111" s="192" t="s">
         <v>845</v>
-      </c>
-      <c r="B111" s="192" t="s">
-        <v>846</v>
       </c>
       <c r="C111" s="193" t="s">
         <v>484</v>
@@ -14187,10 +14184,10 @@
         <v>370</v>
       </c>
       <c r="F111" s="32" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="G111" s="143" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="H111" s="36"/>
       <c r="I111" s="34"/>
@@ -14206,10 +14203,10 @@
     </row>
     <row r="112">
       <c r="A112" s="191" t="s">
+        <v>847</v>
+      </c>
+      <c r="B112" s="192" t="s">
         <v>848</v>
-      </c>
-      <c r="B112" s="192" t="s">
-        <v>849</v>
       </c>
       <c r="C112" s="193" t="s">
         <v>484</v>
@@ -14219,10 +14216,10 @@
         <v>370</v>
       </c>
       <c r="F112" s="32" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="G112" s="143" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="H112" s="36"/>
       <c r="I112" s="34"/>
@@ -14231,17 +14228,17 @@
         <v>709</v>
       </c>
       <c r="L112" s="121" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="M112" s="121"/>
       <c r="N112" s="34"/>
     </row>
     <row r="113">
       <c r="A113" s="191" t="s">
+        <v>851</v>
+      </c>
+      <c r="B113" s="192" t="s">
         <v>852</v>
-      </c>
-      <c r="B113" s="192" t="s">
-        <v>853</v>
       </c>
       <c r="C113" s="193" t="s">
         <v>484</v>
@@ -14251,10 +14248,10 @@
         <v>370</v>
       </c>
       <c r="F113" s="32" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="G113" s="32" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="H113" s="36"/>
       <c r="I113" s="34"/>
@@ -14270,10 +14267,10 @@
     </row>
     <row r="114">
       <c r="A114" s="191" t="s">
+        <v>854</v>
+      </c>
+      <c r="B114" s="192" t="s">
         <v>855</v>
-      </c>
-      <c r="B114" s="192" t="s">
-        <v>856</v>
       </c>
       <c r="C114" s="193" t="s">
         <v>484</v>
@@ -14283,10 +14280,10 @@
         <v>370</v>
       </c>
       <c r="F114" s="32" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="G114" s="32" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="H114" s="36"/>
       <c r="I114" s="34"/>
@@ -14302,10 +14299,10 @@
     </row>
     <row r="115">
       <c r="A115" s="60" t="s">
+        <v>857</v>
+      </c>
+      <c r="B115" s="157" t="s">
         <v>858</v>
-      </c>
-      <c r="B115" s="157" t="s">
-        <v>859</v>
       </c>
       <c r="C115" s="196" t="s">
         <v>480</v>
@@ -14315,10 +14312,10 @@
         <v>363</v>
       </c>
       <c r="F115" s="56" t="s">
+        <v>859</v>
+      </c>
+      <c r="G115" s="56" t="s">
         <v>860</v>
-      </c>
-      <c r="G115" s="56" t="s">
-        <v>861</v>
       </c>
       <c r="H115" s="64"/>
       <c r="I115" s="58"/>
@@ -14334,10 +14331,10 @@
     </row>
     <row r="116">
       <c r="A116" s="137" t="s">
+        <v>861</v>
+      </c>
+      <c r="B116" s="121" t="s">
         <v>862</v>
-      </c>
-      <c r="B116" s="121" t="s">
-        <v>863</v>
       </c>
       <c r="C116" s="145" t="s">
         <v>484</v>
@@ -14347,10 +14344,10 @@
         <v>373</v>
       </c>
       <c r="F116" s="32" t="s">
+        <v>863</v>
+      </c>
+      <c r="G116" s="41" t="s">
         <v>864</v>
-      </c>
-      <c r="G116" s="41" t="s">
-        <v>865</v>
       </c>
       <c r="H116" s="36"/>
       <c r="I116" s="34"/>
@@ -14366,10 +14363,10 @@
     </row>
     <row r="117">
       <c r="A117" s="137" t="s">
+        <v>865</v>
+      </c>
+      <c r="B117" s="121" t="s">
         <v>866</v>
-      </c>
-      <c r="B117" s="121" t="s">
-        <v>867</v>
       </c>
       <c r="C117" s="145" t="s">
         <v>484</v>
@@ -14379,10 +14376,10 @@
         <v>370</v>
       </c>
       <c r="F117" s="41" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="G117" s="32" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H117" s="36"/>
       <c r="I117" s="34"/>
@@ -14398,10 +14395,10 @@
     </row>
     <row r="118">
       <c r="A118" s="60" t="s">
+        <v>868</v>
+      </c>
+      <c r="B118" s="157" t="s">
         <v>869</v>
-      </c>
-      <c r="B118" s="157" t="s">
-        <v>870</v>
       </c>
       <c r="C118" s="196" t="s">
         <v>484</v>
@@ -14411,10 +14408,10 @@
         <v>370</v>
       </c>
       <c r="F118" s="41" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="G118" s="56" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="H118" s="64"/>
       <c r="I118" s="58"/>
@@ -14430,10 +14427,10 @@
     </row>
     <row r="119">
       <c r="A119" s="60" t="s">
+        <v>871</v>
+      </c>
+      <c r="B119" s="157" t="s">
         <v>872</v>
-      </c>
-      <c r="B119" s="157" t="s">
-        <v>873</v>
       </c>
       <c r="C119" s="196" t="s">
         <v>484</v>
@@ -14443,10 +14440,10 @@
         <v>370</v>
       </c>
       <c r="F119" s="41" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="G119" s="56" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="H119" s="64"/>
       <c r="I119" s="58"/>
@@ -14455,17 +14452,17 @@
         <v>709</v>
       </c>
       <c r="L119" s="157" t="s">
-        <v>785</v>
+        <v>718</v>
       </c>
       <c r="M119" s="157"/>
       <c r="N119" s="58"/>
     </row>
     <row r="120">
       <c r="A120" s="60" t="s">
+        <v>874</v>
+      </c>
+      <c r="B120" s="157" t="s">
         <v>875</v>
-      </c>
-      <c r="B120" s="157" t="s">
-        <v>876</v>
       </c>
       <c r="C120" s="196" t="s">
         <v>484</v>
@@ -14475,10 +14472,10 @@
         <v>370</v>
       </c>
       <c r="F120" s="41" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="G120" s="56" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="H120" s="64"/>
       <c r="I120" s="58"/>
@@ -14494,10 +14491,10 @@
     </row>
     <row r="121">
       <c r="A121" s="127" t="s">
+        <v>877</v>
+      </c>
+      <c r="B121" s="134" t="s">
         <v>878</v>
-      </c>
-      <c r="B121" s="134" t="s">
-        <v>879</v>
       </c>
       <c r="C121" s="148" t="s">
         <v>484</v>
@@ -14507,10 +14504,10 @@
         <v>370</v>
       </c>
       <c r="F121" s="41" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="G121" s="130" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="H121" s="142"/>
       <c r="I121" s="133"/>
@@ -14526,10 +14523,10 @@
     </row>
     <row r="122">
       <c r="A122" s="24" t="s">
+        <v>880</v>
+      </c>
+      <c r="B122" s="123" t="s">
         <v>881</v>
-      </c>
-      <c r="B122" s="123" t="s">
-        <v>882</v>
       </c>
       <c r="C122" s="197" t="s">
         <v>480</v>
@@ -14539,10 +14536,10 @@
         <v>370</v>
       </c>
       <c r="F122" s="14" t="s">
+        <v>882</v>
+      </c>
+      <c r="G122" s="14" t="s">
         <v>883</v>
-      </c>
-      <c r="G122" s="14" t="s">
-        <v>884</v>
       </c>
       <c r="H122" s="13"/>
       <c r="I122" s="16"/>
@@ -14558,10 +14555,10 @@
     </row>
     <row r="123">
       <c r="A123" s="24" t="s">
+        <v>884</v>
+      </c>
+      <c r="B123" s="123" t="s">
         <v>885</v>
-      </c>
-      <c r="B123" s="123" t="s">
-        <v>886</v>
       </c>
       <c r="C123" s="197" t="s">
         <v>484</v>
@@ -14571,10 +14568,10 @@
         <v>363</v>
       </c>
       <c r="F123" s="14" t="s">
+        <v>886</v>
+      </c>
+      <c r="G123" s="5" t="s">
         <v>887</v>
-      </c>
-      <c r="G123" s="5" t="s">
-        <v>888</v>
       </c>
       <c r="H123" s="13"/>
       <c r="I123" s="16"/>
@@ -14590,10 +14587,10 @@
     </row>
     <row r="124">
       <c r="A124" s="24" t="s">
+        <v>888</v>
+      </c>
+      <c r="B124" s="123" t="s">
         <v>889</v>
-      </c>
-      <c r="B124" s="123" t="s">
-        <v>890</v>
       </c>
       <c r="C124" s="197" t="s">
         <v>480</v>
@@ -14603,7 +14600,7 @@
         <v>370</v>
       </c>
       <c r="F124" s="14" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="G124" s="48"/>
       <c r="H124" s="13"/>
@@ -14620,10 +14617,10 @@
     </row>
     <row r="125">
       <c r="A125" s="24" t="s">
+        <v>891</v>
+      </c>
+      <c r="B125" s="123" t="s">
         <v>892</v>
-      </c>
-      <c r="B125" s="123" t="s">
-        <v>893</v>
       </c>
       <c r="C125" s="197" t="s">
         <v>484</v>
@@ -14633,10 +14630,10 @@
         <v>363</v>
       </c>
       <c r="F125" s="14" t="s">
+        <v>893</v>
+      </c>
+      <c r="G125" s="5" t="s">
         <v>894</v>
-      </c>
-      <c r="G125" s="5" t="s">
-        <v>895</v>
       </c>
       <c r="H125" s="13"/>
       <c r="I125" s="16"/>
@@ -14652,10 +14649,10 @@
     </row>
     <row r="126">
       <c r="A126" s="137" t="s">
+        <v>895</v>
+      </c>
+      <c r="B126" s="121" t="s">
         <v>896</v>
-      </c>
-      <c r="B126" s="121" t="s">
-        <v>897</v>
       </c>
       <c r="C126" s="145" t="s">
         <v>480</v>
@@ -14665,10 +14662,10 @@
         <v>373</v>
       </c>
       <c r="F126" s="32" t="s">
+        <v>897</v>
+      </c>
+      <c r="G126" s="32" t="s">
         <v>898</v>
-      </c>
-      <c r="G126" s="32" t="s">
-        <v>899</v>
       </c>
       <c r="H126" s="36"/>
       <c r="I126" s="34"/>
@@ -14677,17 +14674,17 @@
         <v>512</v>
       </c>
       <c r="L126" s="147" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="M126" s="147"/>
       <c r="N126" s="34"/>
     </row>
     <row r="127">
       <c r="A127" s="137" t="s">
+        <v>900</v>
+      </c>
+      <c r="B127" s="121" t="s">
         <v>901</v>
-      </c>
-      <c r="B127" s="121" t="s">
-        <v>902</v>
       </c>
       <c r="C127" s="145" t="s">
         <v>484</v>
@@ -14697,10 +14694,10 @@
         <v>363</v>
       </c>
       <c r="F127" s="32" t="s">
+        <v>902</v>
+      </c>
+      <c r="G127" s="32" t="s">
         <v>903</v>
-      </c>
-      <c r="G127" s="32" t="s">
-        <v>904</v>
       </c>
       <c r="H127" s="36"/>
       <c r="I127" s="34"/>
@@ -14709,17 +14706,17 @@
         <v>257</v>
       </c>
       <c r="L127" s="147" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="M127" s="147"/>
       <c r="N127" s="34"/>
     </row>
     <row r="128">
       <c r="A128" s="137" t="s">
+        <v>905</v>
+      </c>
+      <c r="B128" s="117" t="s">
         <v>906</v>
-      </c>
-      <c r="B128" s="117" t="s">
-        <v>907</v>
       </c>
       <c r="C128" s="145" t="s">
         <v>480</v>
@@ -14729,10 +14726,10 @@
         <v>370</v>
       </c>
       <c r="F128" s="32" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="G128" s="143" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="H128" s="36"/>
       <c r="I128" s="34"/>
@@ -14748,10 +14745,10 @@
     </row>
     <row r="129">
       <c r="A129" s="137" t="s">
+        <v>908</v>
+      </c>
+      <c r="B129" s="117" t="s">
         <v>909</v>
-      </c>
-      <c r="B129" s="117" t="s">
-        <v>910</v>
       </c>
       <c r="C129" s="145" t="s">
         <v>480</v>
@@ -14761,10 +14758,10 @@
         <v>370</v>
       </c>
       <c r="F129" s="32" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="G129" s="143" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="H129" s="36"/>
       <c r="I129" s="34"/>
@@ -14780,10 +14777,10 @@
     </row>
     <row r="130">
       <c r="A130" s="137" t="s">
+        <v>911</v>
+      </c>
+      <c r="B130" s="117" t="s">
         <v>912</v>
-      </c>
-      <c r="B130" s="117" t="s">
-        <v>913</v>
       </c>
       <c r="C130" s="145" t="s">
         <v>480</v>
@@ -14793,10 +14790,10 @@
         <v>370</v>
       </c>
       <c r="F130" s="32" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="G130" s="143" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="H130" s="36"/>
       <c r="I130" s="34"/>
@@ -14812,10 +14809,10 @@
     </row>
     <row r="131">
       <c r="A131" s="137" t="s">
+        <v>914</v>
+      </c>
+      <c r="B131" s="117" t="s">
         <v>915</v>
-      </c>
-      <c r="B131" s="117" t="s">
-        <v>916</v>
       </c>
       <c r="C131" s="145" t="s">
         <v>480</v>
@@ -14825,10 +14822,10 @@
         <v>373</v>
       </c>
       <c r="F131" s="32" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="G131" s="143" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="H131" s="36"/>
       <c r="I131" s="34"/>
@@ -14837,17 +14834,17 @@
         <v>0.0</v>
       </c>
       <c r="L131" s="147" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="M131" s="147"/>
       <c r="N131" s="34"/>
     </row>
     <row r="132">
       <c r="A132" s="137" t="s">
+        <v>918</v>
+      </c>
+      <c r="B132" s="117" t="s">
         <v>919</v>
-      </c>
-      <c r="B132" s="117" t="s">
-        <v>920</v>
       </c>
       <c r="C132" s="145" t="s">
         <v>480</v>
@@ -14857,10 +14854,10 @@
         <v>373</v>
       </c>
       <c r="F132" s="32" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="G132" s="143" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="H132" s="36"/>
       <c r="I132" s="34"/>
@@ -14869,17 +14866,17 @@
         <v>0.0</v>
       </c>
       <c r="L132" s="147" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="M132" s="147"/>
       <c r="N132" s="34"/>
     </row>
     <row r="133">
       <c r="A133" s="137" t="s">
+        <v>921</v>
+      </c>
+      <c r="B133" s="117" t="s">
         <v>922</v>
-      </c>
-      <c r="B133" s="117" t="s">
-        <v>923</v>
       </c>
       <c r="C133" s="145" t="s">
         <v>480</v>
@@ -14889,10 +14886,10 @@
         <v>370</v>
       </c>
       <c r="F133" s="32" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="G133" s="143" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="H133" s="36"/>
       <c r="I133" s="34"/>
@@ -14908,10 +14905,10 @@
     </row>
     <row r="134">
       <c r="A134" s="137" t="s">
+        <v>924</v>
+      </c>
+      <c r="B134" s="117" t="s">
         <v>925</v>
-      </c>
-      <c r="B134" s="117" t="s">
-        <v>926</v>
       </c>
       <c r="C134" s="145" t="s">
         <v>480</v>
@@ -14921,10 +14918,10 @@
         <v>370</v>
       </c>
       <c r="F134" s="32" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="G134" s="32" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="H134" s="36"/>
       <c r="I134" s="34"/>
@@ -14933,17 +14930,17 @@
         <v>709</v>
       </c>
       <c r="L134" s="147" t="s">
-        <v>785</v>
+        <v>718</v>
       </c>
       <c r="M134" s="147"/>
       <c r="N134" s="32"/>
     </row>
     <row r="135">
       <c r="A135" s="137" t="s">
+        <v>927</v>
+      </c>
+      <c r="B135" s="117" t="s">
         <v>928</v>
-      </c>
-      <c r="B135" s="117" t="s">
-        <v>929</v>
       </c>
       <c r="C135" s="145" t="s">
         <v>480</v>
@@ -14953,10 +14950,10 @@
         <v>370</v>
       </c>
       <c r="F135" s="32" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="G135" s="143" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="H135" s="36"/>
       <c r="I135" s="34"/>
@@ -14972,10 +14969,10 @@
     </row>
     <row r="136">
       <c r="A136" s="137" t="s">
+        <v>930</v>
+      </c>
+      <c r="B136" s="117" t="s">
         <v>931</v>
-      </c>
-      <c r="B136" s="117" t="s">
-        <v>932</v>
       </c>
       <c r="C136" s="145" t="s">
         <v>480</v>
@@ -14985,10 +14982,10 @@
         <v>370</v>
       </c>
       <c r="F136" s="32" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="G136" s="32" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="H136" s="36"/>
       <c r="I136" s="34"/>
@@ -14997,17 +14994,17 @@
         <v>704</v>
       </c>
       <c r="L136" s="147" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="M136" s="147"/>
       <c r="N136" s="32"/>
     </row>
     <row r="137">
       <c r="A137" s="137" t="s">
+        <v>934</v>
+      </c>
+      <c r="B137" s="117" t="s">
         <v>935</v>
-      </c>
-      <c r="B137" s="117" t="s">
-        <v>936</v>
       </c>
       <c r="C137" s="145" t="s">
         <v>480</v>
@@ -15017,10 +15014,10 @@
         <v>370</v>
       </c>
       <c r="F137" s="32" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="G137" s="32" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="H137" s="36"/>
       <c r="I137" s="34"/>
@@ -15029,17 +15026,17 @@
         <v>709</v>
       </c>
       <c r="L137" s="147" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="M137" s="147"/>
       <c r="N137" s="32"/>
     </row>
     <row r="138">
       <c r="A138" s="137" t="s">
+        <v>938</v>
+      </c>
+      <c r="B138" s="117" t="s">
         <v>939</v>
-      </c>
-      <c r="B138" s="117" t="s">
-        <v>940</v>
       </c>
       <c r="C138" s="145" t="s">
         <v>480</v>
@@ -15049,10 +15046,10 @@
         <v>373</v>
       </c>
       <c r="F138" s="32" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="G138" s="143" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="H138" s="36"/>
       <c r="I138" s="34"/>
@@ -15068,10 +15065,10 @@
     </row>
     <row r="139">
       <c r="A139" s="137" t="s">
+        <v>941</v>
+      </c>
+      <c r="B139" s="117" t="s">
         <v>942</v>
-      </c>
-      <c r="B139" s="117" t="s">
-        <v>943</v>
       </c>
       <c r="C139" s="145" t="s">
         <v>480</v>
@@ -15081,29 +15078,29 @@
         <v>370</v>
       </c>
       <c r="F139" s="32" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="G139" s="143" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="H139" s="36"/>
       <c r="I139" s="34"/>
       <c r="J139" s="34"/>
       <c r="K139" s="121" t="s">
+        <v>944</v>
+      </c>
+      <c r="L139" s="147" t="s">
         <v>945</v>
-      </c>
-      <c r="L139" s="147" t="s">
-        <v>946</v>
       </c>
       <c r="M139" s="147"/>
       <c r="N139" s="34"/>
     </row>
     <row r="140">
       <c r="A140" s="200" t="s">
+        <v>946</v>
+      </c>
+      <c r="B140" s="201" t="s">
         <v>947</v>
-      </c>
-      <c r="B140" s="201" t="s">
-        <v>948</v>
       </c>
       <c r="C140" s="202" t="s">
         <v>480</v>
@@ -15113,29 +15110,29 @@
         <v>370</v>
       </c>
       <c r="F140" s="32" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="G140" s="143" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="H140" s="204"/>
       <c r="I140" s="205"/>
       <c r="J140" s="205"/>
       <c r="K140" s="206" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="L140" s="207" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="M140" s="207"/>
       <c r="N140" s="205"/>
     </row>
     <row r="141">
       <c r="A141" s="24" t="s">
+        <v>950</v>
+      </c>
+      <c r="B141" s="115" t="s">
         <v>951</v>
-      </c>
-      <c r="B141" s="115" t="s">
-        <v>952</v>
       </c>
       <c r="C141" s="197" t="s">
         <v>480</v>
@@ -15145,10 +15142,10 @@
         <v>373</v>
       </c>
       <c r="F141" s="14" t="s">
+        <v>952</v>
+      </c>
+      <c r="G141" s="208" t="s">
         <v>953</v>
-      </c>
-      <c r="G141" s="208" t="s">
-        <v>954</v>
       </c>
       <c r="H141" s="13"/>
       <c r="I141" s="16"/>
@@ -15164,10 +15161,10 @@
     </row>
     <row r="142">
       <c r="A142" s="24" t="s">
+        <v>954</v>
+      </c>
+      <c r="B142" s="115" t="s">
         <v>955</v>
-      </c>
-      <c r="B142" s="115" t="s">
-        <v>956</v>
       </c>
       <c r="C142" s="197" t="s">
         <v>484</v>
@@ -15177,10 +15174,10 @@
         <v>363</v>
       </c>
       <c r="F142" s="14" t="s">
+        <v>956</v>
+      </c>
+      <c r="G142" s="14" t="s">
         <v>957</v>
-      </c>
-      <c r="G142" s="14" t="s">
-        <v>958</v>
       </c>
       <c r="H142" s="13"/>
       <c r="I142" s="16"/>
@@ -15196,10 +15193,10 @@
     </row>
     <row r="143">
       <c r="A143" s="24" t="s">
+        <v>958</v>
+      </c>
+      <c r="B143" s="115" t="s">
         <v>959</v>
-      </c>
-      <c r="B143" s="115" t="s">
-        <v>960</v>
       </c>
       <c r="C143" s="197" t="s">
         <v>480</v>
@@ -15209,10 +15206,10 @@
         <v>373</v>
       </c>
       <c r="F143" s="14" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="G143" s="208" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="H143" s="13"/>
       <c r="I143" s="16"/>
@@ -15228,10 +15225,10 @@
     </row>
     <row r="144">
       <c r="A144" s="24" t="s">
+        <v>961</v>
+      </c>
+      <c r="B144" s="115" t="s">
         <v>962</v>
-      </c>
-      <c r="B144" s="115" t="s">
-        <v>963</v>
       </c>
       <c r="C144" s="197" t="s">
         <v>484</v>
@@ -15241,10 +15238,10 @@
         <v>363</v>
       </c>
       <c r="F144" s="5" t="s">
+        <v>963</v>
+      </c>
+      <c r="G144" s="5" t="s">
         <v>964</v>
-      </c>
-      <c r="G144" s="5" t="s">
-        <v>965</v>
       </c>
       <c r="H144" s="13"/>
       <c r="I144" s="16"/>
@@ -15260,10 +15257,10 @@
     </row>
     <row r="145">
       <c r="A145" s="127" t="s">
+        <v>965</v>
+      </c>
+      <c r="B145" s="115" t="s">
         <v>966</v>
-      </c>
-      <c r="B145" s="115" t="s">
-        <v>967</v>
       </c>
       <c r="C145" s="197" t="s">
         <v>480</v>
@@ -15273,10 +15270,10 @@
         <v>370</v>
       </c>
       <c r="F145" s="208" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="G145" s="5" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="H145" s="13"/>
       <c r="I145" s="16"/>
@@ -15292,10 +15289,10 @@
     </row>
     <row r="146">
       <c r="A146" s="127" t="s">
+        <v>968</v>
+      </c>
+      <c r="B146" s="115" t="s">
         <v>969</v>
-      </c>
-      <c r="B146" s="115" t="s">
-        <v>970</v>
       </c>
       <c r="C146" s="197" t="s">
         <v>480</v>
@@ -15305,10 +15302,10 @@
         <v>370</v>
       </c>
       <c r="F146" s="208" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="G146" s="5" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="H146" s="13"/>
       <c r="I146" s="16"/>
@@ -15324,10 +15321,10 @@
     </row>
     <row r="147">
       <c r="A147" s="137" t="s">
+        <v>971</v>
+      </c>
+      <c r="B147" s="117" t="s">
         <v>972</v>
-      </c>
-      <c r="B147" s="117" t="s">
-        <v>973</v>
       </c>
       <c r="C147" s="145" t="s">
         <v>480</v>
@@ -15337,10 +15334,10 @@
         <v>373</v>
       </c>
       <c r="F147" s="32" t="s">
+        <v>973</v>
+      </c>
+      <c r="G147" s="143" t="s">
         <v>974</v>
-      </c>
-      <c r="G147" s="143" t="s">
-        <v>975</v>
       </c>
       <c r="H147" s="36"/>
       <c r="I147" s="34"/>
@@ -15349,17 +15346,17 @@
         <v>512</v>
       </c>
       <c r="L147" s="147" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="M147" s="147"/>
       <c r="N147" s="34"/>
     </row>
     <row r="148">
       <c r="A148" s="137" t="s">
+        <v>976</v>
+      </c>
+      <c r="B148" s="117" t="s">
         <v>977</v>
-      </c>
-      <c r="B148" s="117" t="s">
-        <v>978</v>
       </c>
       <c r="C148" s="145" t="s">
         <v>484</v>
@@ -15369,29 +15366,29 @@
         <v>363</v>
       </c>
       <c r="F148" s="32" t="s">
+        <v>978</v>
+      </c>
+      <c r="G148" s="32" t="s">
         <v>979</v>
-      </c>
-      <c r="G148" s="32" t="s">
-        <v>980</v>
       </c>
       <c r="H148" s="38"/>
       <c r="I148" s="34"/>
       <c r="J148" s="34"/>
       <c r="K148" s="211" t="s">
+        <v>980</v>
+      </c>
+      <c r="L148" s="5" t="s">
         <v>981</v>
-      </c>
-      <c r="L148" s="5" t="s">
-        <v>982</v>
       </c>
       <c r="M148" s="5"/>
       <c r="N148" s="34"/>
     </row>
     <row r="149">
       <c r="A149" s="137" t="s">
+        <v>982</v>
+      </c>
+      <c r="B149" s="117" t="s">
         <v>983</v>
-      </c>
-      <c r="B149" s="117" t="s">
-        <v>984</v>
       </c>
       <c r="C149" s="145" t="s">
         <v>480</v>
@@ -15401,10 +15398,10 @@
         <v>373</v>
       </c>
       <c r="F149" s="32" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="G149" s="143" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="H149" s="38"/>
       <c r="I149" s="34"/>
@@ -15413,17 +15410,17 @@
         <v>512</v>
       </c>
       <c r="L149" s="212" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="M149" s="212"/>
       <c r="N149" s="34"/>
     </row>
     <row r="150">
       <c r="A150" s="137" t="s">
+        <v>986</v>
+      </c>
+      <c r="B150" s="117" t="s">
         <v>987</v>
-      </c>
-      <c r="B150" s="117" t="s">
-        <v>988</v>
       </c>
       <c r="C150" s="145" t="s">
         <v>484</v>
@@ -15433,29 +15430,29 @@
         <v>363</v>
       </c>
       <c r="F150" s="32" t="s">
+        <v>988</v>
+      </c>
+      <c r="G150" s="143" t="s">
         <v>989</v>
-      </c>
-      <c r="G150" s="143" t="s">
-        <v>990</v>
       </c>
       <c r="H150" s="36"/>
       <c r="I150" s="34"/>
       <c r="J150" s="34"/>
       <c r="K150" s="211" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="L150" s="5" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="M150" s="5"/>
       <c r="N150" s="34"/>
     </row>
     <row r="151">
       <c r="A151" s="137" t="s">
+        <v>991</v>
+      </c>
+      <c r="B151" s="117" t="s">
         <v>992</v>
-      </c>
-      <c r="B151" s="117" t="s">
-        <v>993</v>
       </c>
       <c r="C151" s="145" t="s">
         <v>480</v>
@@ -15465,10 +15462,10 @@
         <v>373</v>
       </c>
       <c r="F151" s="32" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="G151" s="143" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="H151" s="36"/>
       <c r="I151" s="34"/>
@@ -15477,17 +15474,17 @@
         <v>512</v>
       </c>
       <c r="L151" s="147" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="M151" s="147"/>
       <c r="N151" s="34"/>
     </row>
     <row r="152">
       <c r="A152" s="137" t="s">
+        <v>995</v>
+      </c>
+      <c r="B152" s="117" t="s">
         <v>996</v>
-      </c>
-      <c r="B152" s="117" t="s">
-        <v>997</v>
       </c>
       <c r="C152" s="145" t="s">
         <v>484</v>
@@ -15497,29 +15494,29 @@
         <v>363</v>
       </c>
       <c r="F152" s="32" t="s">
+        <v>997</v>
+      </c>
+      <c r="G152" s="143" t="s">
         <v>998</v>
-      </c>
-      <c r="G152" s="143" t="s">
-        <v>999</v>
       </c>
       <c r="H152" s="36"/>
       <c r="I152" s="34"/>
       <c r="J152" s="34"/>
       <c r="K152" s="211" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="L152" s="5" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="M152" s="5"/>
       <c r="N152" s="34"/>
     </row>
     <row r="153">
       <c r="A153" s="137" t="s">
+        <v>1000</v>
+      </c>
+      <c r="B153" s="117" t="s">
         <v>1001</v>
-      </c>
-      <c r="B153" s="117" t="s">
-        <v>1002</v>
       </c>
       <c r="C153" s="145" t="s">
         <v>480</v>
@@ -15529,10 +15526,10 @@
         <v>373</v>
       </c>
       <c r="F153" s="32" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="G153" s="143" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="H153" s="36"/>
       <c r="I153" s="34"/>
@@ -15541,17 +15538,17 @@
         <v>512</v>
       </c>
       <c r="L153" s="149" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="M153" s="149"/>
       <c r="N153" s="34"/>
     </row>
     <row r="154">
       <c r="A154" s="24" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B154" s="115" t="s">
         <v>1005</v>
-      </c>
-      <c r="B154" s="115" t="s">
-        <v>1006</v>
       </c>
       <c r="C154" s="156" t="s">
         <v>484</v>
@@ -15561,29 +15558,29 @@
         <v>363</v>
       </c>
       <c r="F154" s="14" t="s">
+        <v>1006</v>
+      </c>
+      <c r="G154" s="5" t="s">
         <v>1007</v>
-      </c>
-      <c r="G154" s="5" t="s">
-        <v>1008</v>
       </c>
       <c r="H154" s="13"/>
       <c r="I154" s="16"/>
       <c r="J154" s="16"/>
       <c r="K154" s="211" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="L154" s="5" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="M154" s="5"/>
       <c r="N154" s="16"/>
     </row>
     <row r="155">
       <c r="A155" s="24" t="s">
+        <v>1009</v>
+      </c>
+      <c r="B155" s="115" t="s">
         <v>1010</v>
-      </c>
-      <c r="B155" s="115" t="s">
-        <v>1011</v>
       </c>
       <c r="C155" s="156" t="s">
         <v>480</v>
@@ -15593,10 +15590,10 @@
         <v>373</v>
       </c>
       <c r="F155" s="14" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="G155" s="215" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="H155" s="13"/>
       <c r="I155" s="16"/>
@@ -15605,17 +15602,17 @@
         <v>512</v>
       </c>
       <c r="L155" s="209" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="M155" s="209"/>
       <c r="N155" s="16"/>
     </row>
     <row r="156">
       <c r="A156" s="24" t="s">
+        <v>1013</v>
+      </c>
+      <c r="B156" s="115" t="s">
         <v>1014</v>
-      </c>
-      <c r="B156" s="115" t="s">
-        <v>1015</v>
       </c>
       <c r="C156" s="156" t="s">
         <v>484</v>
@@ -15625,29 +15622,29 @@
         <v>363</v>
       </c>
       <c r="F156" s="14" t="s">
+        <v>1015</v>
+      </c>
+      <c r="G156" s="5" t="s">
         <v>1016</v>
-      </c>
-      <c r="G156" s="5" t="s">
-        <v>1017</v>
       </c>
       <c r="H156" s="13"/>
       <c r="I156" s="16"/>
       <c r="J156" s="16"/>
       <c r="K156" s="211" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="L156" s="5" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="M156" s="5"/>
       <c r="N156" s="16"/>
     </row>
     <row r="157">
       <c r="A157" s="24" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B157" s="115" t="s">
         <v>1019</v>
-      </c>
-      <c r="B157" s="115" t="s">
-        <v>1020</v>
       </c>
       <c r="C157" s="156" t="s">
         <v>480</v>
@@ -15657,10 +15654,10 @@
         <v>373</v>
       </c>
       <c r="F157" s="14" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="G157" s="215" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="H157" s="13"/>
       <c r="I157" s="16"/>
@@ -15669,17 +15666,17 @@
         <v>512</v>
       </c>
       <c r="L157" s="209" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="M157" s="209"/>
       <c r="N157" s="16"/>
     </row>
     <row r="158">
       <c r="A158" s="24" t="s">
+        <v>1022</v>
+      </c>
+      <c r="B158" s="115" t="s">
         <v>1023</v>
-      </c>
-      <c r="B158" s="115" t="s">
-        <v>1024</v>
       </c>
       <c r="C158" s="156" t="s">
         <v>484</v>
@@ -15689,29 +15686,29 @@
         <v>363</v>
       </c>
       <c r="F158" s="14" t="s">
+        <v>1024</v>
+      </c>
+      <c r="G158" s="131" t="s">
         <v>1025</v>
-      </c>
-      <c r="G158" s="131" t="s">
-        <v>1026</v>
       </c>
       <c r="H158" s="13"/>
       <c r="I158" s="16"/>
       <c r="J158" s="16"/>
       <c r="K158" s="211" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="L158" s="5" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="M158" s="5"/>
       <c r="N158" s="16"/>
     </row>
     <row r="159">
       <c r="A159" s="24" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B159" s="115" t="s">
         <v>1028</v>
-      </c>
-      <c r="B159" s="115" t="s">
-        <v>1029</v>
       </c>
       <c r="C159" s="156" t="s">
         <v>480</v>
@@ -15721,10 +15718,10 @@
         <v>373</v>
       </c>
       <c r="F159" s="14" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="G159" s="215" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="H159" s="13"/>
       <c r="I159" s="16"/>
@@ -15733,17 +15730,17 @@
         <v>512</v>
       </c>
       <c r="L159" s="209" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="M159" s="209"/>
       <c r="N159" s="16"/>
     </row>
     <row r="160">
       <c r="A160" s="24" t="s">
+        <v>1031</v>
+      </c>
+      <c r="B160" s="115" t="s">
         <v>1032</v>
-      </c>
-      <c r="B160" s="115" t="s">
-        <v>1033</v>
       </c>
       <c r="C160" s="156" t="s">
         <v>484</v>
@@ -15753,29 +15750,29 @@
         <v>363</v>
       </c>
       <c r="F160" s="14" t="s">
+        <v>1033</v>
+      </c>
+      <c r="G160" s="131" t="s">
         <v>1034</v>
-      </c>
-      <c r="G160" s="131" t="s">
-        <v>1035</v>
       </c>
       <c r="H160" s="13"/>
       <c r="I160" s="16"/>
       <c r="J160" s="16"/>
       <c r="K160" s="211" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="L160" s="5" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="M160" s="5"/>
       <c r="N160" s="16"/>
     </row>
     <row r="161">
       <c r="A161" s="24" t="s">
+        <v>1036</v>
+      </c>
+      <c r="B161" s="115" t="s">
         <v>1037</v>
-      </c>
-      <c r="B161" s="115" t="s">
-        <v>1038</v>
       </c>
       <c r="C161" s="156" t="s">
         <v>480</v>
@@ -15785,10 +15782,10 @@
         <v>373</v>
       </c>
       <c r="F161" s="14" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="G161" s="215" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="H161" s="13"/>
       <c r="I161" s="16"/>
@@ -15797,17 +15794,17 @@
         <v>512</v>
       </c>
       <c r="L161" s="209" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="M161" s="209"/>
       <c r="N161" s="16"/>
     </row>
     <row r="162">
       <c r="A162" s="24" t="s">
+        <v>1040</v>
+      </c>
+      <c r="B162" s="115" t="s">
         <v>1041</v>
-      </c>
-      <c r="B162" s="115" t="s">
-        <v>1042</v>
       </c>
       <c r="C162" s="156" t="s">
         <v>484</v>
@@ -15817,29 +15814,29 @@
         <v>363</v>
       </c>
       <c r="F162" s="14" t="s">
+        <v>1042</v>
+      </c>
+      <c r="G162" s="131" t="s">
         <v>1043</v>
-      </c>
-      <c r="G162" s="131" t="s">
-        <v>1044</v>
       </c>
       <c r="H162" s="13"/>
       <c r="I162" s="16"/>
       <c r="J162" s="16"/>
       <c r="K162" s="211" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="L162" s="5" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="M162" s="5"/>
       <c r="N162" s="16"/>
     </row>
     <row r="163">
       <c r="A163" s="24" t="s">
+        <v>1045</v>
+      </c>
+      <c r="B163" s="115" t="s">
         <v>1046</v>
-      </c>
-      <c r="B163" s="115" t="s">
-        <v>1047</v>
       </c>
       <c r="C163" s="156" t="s">
         <v>480</v>
@@ -15849,10 +15846,10 @@
         <v>373</v>
       </c>
       <c r="F163" s="14" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="G163" s="215" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="H163" s="13"/>
       <c r="I163" s="16"/>
@@ -15861,17 +15858,17 @@
         <v>512</v>
       </c>
       <c r="L163" s="209" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="M163" s="209"/>
       <c r="N163" s="16"/>
     </row>
     <row r="164">
       <c r="A164" s="24" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B164" s="115" t="s">
         <v>1050</v>
-      </c>
-      <c r="B164" s="115" t="s">
-        <v>1051</v>
       </c>
       <c r="C164" s="156" t="s">
         <v>484</v>
@@ -15881,29 +15878,29 @@
         <v>363</v>
       </c>
       <c r="F164" s="14" t="s">
+        <v>1051</v>
+      </c>
+      <c r="G164" s="131" t="s">
         <v>1052</v>
-      </c>
-      <c r="G164" s="131" t="s">
-        <v>1053</v>
       </c>
       <c r="H164" s="13"/>
       <c r="I164" s="16"/>
       <c r="J164" s="16"/>
       <c r="K164" s="211" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="L164" s="5" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="M164" s="5"/>
       <c r="N164" s="16"/>
     </row>
     <row r="165">
       <c r="A165" s="24" t="s">
+        <v>1054</v>
+      </c>
+      <c r="B165" s="115" t="s">
         <v>1055</v>
-      </c>
-      <c r="B165" s="115" t="s">
-        <v>1056</v>
       </c>
       <c r="C165" s="156" t="s">
         <v>480</v>
@@ -15913,7 +15910,7 @@
         <v>370</v>
       </c>
       <c r="F165" s="215" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="G165" s="5"/>
       <c r="H165" s="13"/>
@@ -15930,10 +15927,10 @@
     </row>
     <row r="166">
       <c r="A166" s="24" t="s">
+        <v>1056</v>
+      </c>
+      <c r="B166" s="115" t="s">
         <v>1057</v>
-      </c>
-      <c r="B166" s="115" t="s">
-        <v>1058</v>
       </c>
       <c r="C166" s="156" t="s">
         <v>480</v>
@@ -15943,7 +15940,7 @@
         <v>370</v>
       </c>
       <c r="F166" s="215" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="G166" s="14"/>
       <c r="H166" s="13"/>
@@ -15960,10 +15957,10 @@
     </row>
     <row r="167">
       <c r="A167" s="24" t="s">
+        <v>1058</v>
+      </c>
+      <c r="B167" s="115" t="s">
         <v>1059</v>
-      </c>
-      <c r="B167" s="115" t="s">
-        <v>1060</v>
       </c>
       <c r="C167" s="156" t="s">
         <v>484</v>
@@ -15973,7 +15970,7 @@
         <v>370</v>
       </c>
       <c r="F167" s="215" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="G167" s="14"/>
       <c r="H167" s="25"/>
@@ -15983,17 +15980,17 @@
         <v>709</v>
       </c>
       <c r="L167" s="209" t="s">
-        <v>785</v>
+        <v>718</v>
       </c>
       <c r="M167" s="209"/>
       <c r="N167" s="16"/>
     </row>
     <row r="168">
       <c r="A168" s="18" t="s">
+        <v>1060</v>
+      </c>
+      <c r="B168" s="115" t="s">
         <v>1061</v>
-      </c>
-      <c r="B168" s="115" t="s">
-        <v>1062</v>
       </c>
       <c r="C168" s="156" t="s">
         <v>484</v>
@@ -16003,7 +16000,7 @@
         <v>370</v>
       </c>
       <c r="F168" s="215" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="G168" s="14"/>
       <c r="H168" s="25"/>
@@ -16020,10 +16017,10 @@
     </row>
     <row r="169">
       <c r="A169" s="18" t="s">
+        <v>1062</v>
+      </c>
+      <c r="B169" s="115" t="s">
         <v>1063</v>
-      </c>
-      <c r="B169" s="115" t="s">
-        <v>1064</v>
       </c>
       <c r="C169" s="156" t="s">
         <v>484</v>
@@ -16033,7 +16030,7 @@
         <v>370</v>
       </c>
       <c r="F169" s="215" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="G169" s="14"/>
       <c r="H169" s="25"/>
@@ -16083,24 +16080,24 @@
         <v>2</v>
       </c>
       <c r="D1" s="218" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="E1" s="216" t="s">
         <v>16</v>
       </c>
       <c r="F1" s="219" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="220" t="s">
+        <v>1066</v>
+      </c>
+      <c r="B2" s="221" t="s">
         <v>1067</v>
       </c>
-      <c r="B2" s="221" t="s">
+      <c r="C2" s="222" t="s">
         <v>1068</v>
-      </c>
-      <c r="C2" s="222" t="s">
-        <v>1069</v>
       </c>
       <c r="D2" s="222"/>
       <c r="E2" s="223"/>
@@ -16108,29 +16105,29 @@
     </row>
     <row r="3">
       <c r="A3" s="220" t="s">
+        <v>1069</v>
+      </c>
+      <c r="B3" s="221" t="s">
         <v>1070</v>
       </c>
-      <c r="B3" s="221" t="s">
+      <c r="C3" s="221" t="s">
         <v>1071</v>
-      </c>
-      <c r="C3" s="221" t="s">
-        <v>1072</v>
       </c>
       <c r="D3" s="221"/>
       <c r="E3" s="225"/>
       <c r="F3" s="219" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="220" t="s">
+        <v>1073</v>
+      </c>
+      <c r="B4" s="221" t="s">
         <v>1074</v>
       </c>
-      <c r="B4" s="221" t="s">
+      <c r="C4" s="221" t="s">
         <v>1075</v>
-      </c>
-      <c r="C4" s="221" t="s">
-        <v>1076</v>
       </c>
       <c r="D4" s="221"/>
       <c r="E4" s="226"/>
@@ -16138,13 +16135,13 @@
     </row>
     <row r="5">
       <c r="A5" s="220" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B5" s="221" t="s">
         <v>1077</v>
       </c>
-      <c r="B5" s="221" t="s">
+      <c r="C5" s="221" t="s">
         <v>1078</v>
-      </c>
-      <c r="C5" s="221" t="s">
-        <v>1079</v>
       </c>
       <c r="D5" s="221"/>
       <c r="E5" s="226"/>
@@ -16152,13 +16149,13 @@
     </row>
     <row r="6">
       <c r="A6" s="220" t="s">
+        <v>1079</v>
+      </c>
+      <c r="B6" s="227" t="s">
         <v>1080</v>
       </c>
-      <c r="B6" s="227" t="s">
+      <c r="C6" s="221" t="s">
         <v>1081</v>
-      </c>
-      <c r="C6" s="221" t="s">
-        <v>1082</v>
       </c>
       <c r="D6" s="221"/>
       <c r="E6" s="225"/>
@@ -16166,13 +16163,13 @@
     </row>
     <row r="7">
       <c r="A7" s="220" t="s">
+        <v>1082</v>
+      </c>
+      <c r="B7" s="228" t="s">
         <v>1083</v>
       </c>
-      <c r="B7" s="228" t="s">
+      <c r="C7" s="221" t="s">
         <v>1084</v>
-      </c>
-      <c r="C7" s="221" t="s">
-        <v>1085</v>
       </c>
       <c r="D7" s="221"/>
       <c r="E7" s="219"/>
@@ -16180,13 +16177,13 @@
     </row>
     <row r="8">
       <c r="A8" s="220" t="s">
+        <v>1085</v>
+      </c>
+      <c r="B8" s="228" t="s">
         <v>1086</v>
       </c>
-      <c r="B8" s="228" t="s">
-        <v>1087</v>
-      </c>
       <c r="C8" s="221" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="D8" s="221"/>
       <c r="E8" s="219"/>
@@ -16194,13 +16191,13 @@
     </row>
     <row r="9">
       <c r="A9" s="220" t="s">
+        <v>1087</v>
+      </c>
+      <c r="B9" s="228" t="s">
         <v>1088</v>
       </c>
-      <c r="B9" s="228" t="s">
+      <c r="C9" s="229" t="s">
         <v>1089</v>
-      </c>
-      <c r="C9" s="229" t="s">
-        <v>1090</v>
       </c>
       <c r="D9" s="229"/>
       <c r="E9" s="230"/>
@@ -16208,13 +16205,13 @@
     </row>
     <row r="10">
       <c r="A10" s="220" t="s">
+        <v>1090</v>
+      </c>
+      <c r="B10" s="228" t="s">
         <v>1091</v>
       </c>
-      <c r="B10" s="228" t="s">
+      <c r="C10" s="221" t="s">
         <v>1092</v>
-      </c>
-      <c r="C10" s="221" t="s">
-        <v>1093</v>
       </c>
       <c r="D10" s="221"/>
       <c r="E10" s="219"/>
@@ -16222,13 +16219,13 @@
     </row>
     <row r="11">
       <c r="A11" s="220" t="s">
+        <v>1093</v>
+      </c>
+      <c r="B11" s="221" t="s">
         <v>1094</v>
       </c>
-      <c r="B11" s="221" t="s">
+      <c r="C11" s="221" t="s">
         <v>1095</v>
-      </c>
-      <c r="C11" s="221" t="s">
-        <v>1096</v>
       </c>
       <c r="D11" s="221"/>
       <c r="E11" s="224"/>
@@ -16236,13 +16233,13 @@
     </row>
     <row r="12">
       <c r="A12" s="220" t="s">
+        <v>1096</v>
+      </c>
+      <c r="B12" s="231" t="s">
         <v>1097</v>
       </c>
-      <c r="B12" s="231" t="s">
+      <c r="C12" s="231" t="s">
         <v>1098</v>
-      </c>
-      <c r="C12" s="231" t="s">
-        <v>1099</v>
       </c>
       <c r="D12" s="231"/>
       <c r="E12" s="224"/>
@@ -16250,13 +16247,13 @@
     </row>
     <row r="13">
       <c r="A13" s="220" t="s">
+        <v>1099</v>
+      </c>
+      <c r="B13" s="232" t="s">
         <v>1100</v>
       </c>
-      <c r="B13" s="232" t="s">
+      <c r="C13" s="231" t="s">
         <v>1101</v>
-      </c>
-      <c r="C13" s="231" t="s">
-        <v>1102</v>
       </c>
       <c r="D13" s="231"/>
       <c r="E13" s="224"/>
@@ -16264,13 +16261,13 @@
     </row>
     <row r="14">
       <c r="A14" s="220" t="s">
+        <v>1102</v>
+      </c>
+      <c r="B14" s="232" t="s">
         <v>1103</v>
       </c>
-      <c r="B14" s="232" t="s">
+      <c r="C14" s="231" t="s">
         <v>1104</v>
-      </c>
-      <c r="C14" s="231" t="s">
-        <v>1105</v>
       </c>
       <c r="D14" s="231"/>
       <c r="E14" s="224"/>
@@ -16278,13 +16275,13 @@
     </row>
     <row r="15">
       <c r="A15" s="220" t="s">
+        <v>1105</v>
+      </c>
+      <c r="B15" s="232" t="s">
         <v>1106</v>
       </c>
-      <c r="B15" s="232" t="s">
+      <c r="C15" s="231" t="s">
         <v>1107</v>
-      </c>
-      <c r="C15" s="231" t="s">
-        <v>1108</v>
       </c>
       <c r="D15" s="231"/>
       <c r="E15" s="224"/>
@@ -16292,13 +16289,13 @@
     </row>
     <row r="16">
       <c r="A16" s="220" t="s">
+        <v>1108</v>
+      </c>
+      <c r="B16" s="232" t="s">
         <v>1109</v>
       </c>
-      <c r="B16" s="232" t="s">
+      <c r="C16" s="231" t="s">
         <v>1110</v>
-      </c>
-      <c r="C16" s="231" t="s">
-        <v>1111</v>
       </c>
       <c r="D16" s="231"/>
       <c r="E16" s="224"/>
@@ -16306,13 +16303,13 @@
     </row>
     <row r="17">
       <c r="A17" s="220" t="s">
+        <v>1111</v>
+      </c>
+      <c r="B17" s="232" t="s">
         <v>1112</v>
       </c>
-      <c r="B17" s="232" t="s">
+      <c r="C17" s="231" t="s">
         <v>1113</v>
-      </c>
-      <c r="C17" s="231" t="s">
-        <v>1114</v>
       </c>
       <c r="D17" s="231"/>
       <c r="E17" s="224"/>
@@ -16320,13 +16317,13 @@
     </row>
     <row r="18">
       <c r="A18" s="220" t="s">
+        <v>1114</v>
+      </c>
+      <c r="B18" s="232" t="s">
         <v>1115</v>
       </c>
-      <c r="B18" s="232" t="s">
+      <c r="C18" s="231" t="s">
         <v>1116</v>
-      </c>
-      <c r="C18" s="231" t="s">
-        <v>1117</v>
       </c>
       <c r="D18" s="231"/>
       <c r="E18" s="224"/>
@@ -16334,13 +16331,13 @@
     </row>
     <row r="19">
       <c r="A19" s="220" t="s">
+        <v>1117</v>
+      </c>
+      <c r="B19" s="232" t="s">
         <v>1118</v>
       </c>
-      <c r="B19" s="232" t="s">
+      <c r="C19" s="231" t="s">
         <v>1119</v>
-      </c>
-      <c r="C19" s="231" t="s">
-        <v>1120</v>
       </c>
       <c r="D19" s="231"/>
       <c r="E19" s="224"/>
@@ -16348,13 +16345,13 @@
     </row>
     <row r="20">
       <c r="A20" s="220" t="s">
+        <v>1120</v>
+      </c>
+      <c r="B20" s="232" t="s">
         <v>1121</v>
       </c>
-      <c r="B20" s="232" t="s">
-        <v>1122</v>
-      </c>
       <c r="C20" s="233" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="D20" s="233"/>
       <c r="E20" s="224"/>
@@ -16362,13 +16359,13 @@
     </row>
     <row r="21">
       <c r="A21" s="220" t="s">
+        <v>1122</v>
+      </c>
+      <c r="B21" s="234" t="s">
         <v>1123</v>
       </c>
-      <c r="B21" s="234" t="s">
+      <c r="C21" s="231" t="s">
         <v>1124</v>
-      </c>
-      <c r="C21" s="231" t="s">
-        <v>1125</v>
       </c>
       <c r="D21" s="231"/>
       <c r="E21" s="224"/>
@@ -16376,29 +16373,29 @@
     </row>
     <row r="22">
       <c r="A22" s="220" t="s">
+        <v>1125</v>
+      </c>
+      <c r="B22" s="232" t="s">
         <v>1126</v>
       </c>
-      <c r="B22" s="232" t="s">
+      <c r="C22" s="5" t="s">
         <v>1127</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="D22" s="235" t="s">
         <v>1128</v>
-      </c>
-      <c r="D22" s="235" t="s">
-        <v>1129</v>
       </c>
       <c r="E22" s="219"/>
       <c r="F22" s="224"/>
     </row>
     <row r="23">
       <c r="A23" s="220" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B23" s="236" t="s">
         <v>1130</v>
       </c>
-      <c r="B23" s="236" t="s">
+      <c r="C23" s="237" t="s">
         <v>1131</v>
-      </c>
-      <c r="C23" s="237" t="s">
-        <v>1132</v>
       </c>
       <c r="D23" s="237"/>
       <c r="E23" s="224"/>
@@ -16406,13 +16403,13 @@
     </row>
     <row r="24">
       <c r="A24" s="220" t="s">
+        <v>1132</v>
+      </c>
+      <c r="B24" s="236" t="s">
         <v>1133</v>
       </c>
-      <c r="B24" s="236" t="s">
+      <c r="C24" s="237" t="s">
         <v>1134</v>
-      </c>
-      <c r="C24" s="237" t="s">
-        <v>1135</v>
       </c>
       <c r="D24" s="237"/>
       <c r="E24" s="224"/>
@@ -16420,13 +16417,13 @@
     </row>
     <row r="25">
       <c r="A25" s="220" t="s">
+        <v>1135</v>
+      </c>
+      <c r="B25" s="236" t="s">
         <v>1136</v>
       </c>
-      <c r="B25" s="236" t="s">
-        <v>1137</v>
-      </c>
       <c r="C25" s="5" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="D25" s="237" t="s">
         <v>453</v>
@@ -16436,13 +16433,13 @@
     </row>
     <row r="26">
       <c r="A26" s="220" t="s">
+        <v>1137</v>
+      </c>
+      <c r="B26" s="231" t="s">
         <v>1138</v>
       </c>
-      <c r="B26" s="231" t="s">
+      <c r="C26" s="231" t="s">
         <v>1139</v>
-      </c>
-      <c r="C26" s="231" t="s">
-        <v>1140</v>
       </c>
       <c r="D26" s="231"/>
       <c r="E26" s="219"/>
@@ -16450,13 +16447,13 @@
     </row>
     <row r="27">
       <c r="A27" s="220" t="s">
+        <v>1140</v>
+      </c>
+      <c r="B27" s="231" t="s">
         <v>1141</v>
       </c>
-      <c r="B27" s="231" t="s">
+      <c r="C27" s="231" t="s">
         <v>1142</v>
-      </c>
-      <c r="C27" s="231" t="s">
-        <v>1143</v>
       </c>
       <c r="D27" s="231"/>
       <c r="E27" s="224"/>
@@ -16464,13 +16461,13 @@
     </row>
     <row r="28">
       <c r="A28" s="220" t="s">
+        <v>1143</v>
+      </c>
+      <c r="B28" s="231" t="s">
         <v>1144</v>
       </c>
-      <c r="B28" s="231" t="s">
+      <c r="C28" s="231" t="s">
         <v>1145</v>
-      </c>
-      <c r="C28" s="231" t="s">
-        <v>1146</v>
       </c>
       <c r="D28" s="231"/>
       <c r="E28" s="224"/>
@@ -16478,143 +16475,143 @@
     </row>
     <row r="29">
       <c r="A29" s="220" t="s">
+        <v>1146</v>
+      </c>
+      <c r="B29" s="238" t="s">
         <v>1147</v>
       </c>
-      <c r="B29" s="238" t="s">
+      <c r="C29" s="228" t="s">
         <v>1148</v>
-      </c>
-      <c r="C29" s="228" t="s">
-        <v>1149</v>
       </c>
       <c r="D29" s="228"/>
       <c r="E29" s="239"/>
     </row>
     <row r="30">
       <c r="A30" s="220" t="s">
+        <v>1149</v>
+      </c>
+      <c r="B30" s="238" t="s">
         <v>1150</v>
       </c>
-      <c r="B30" s="238" t="s">
+      <c r="C30" s="228" t="s">
         <v>1151</v>
-      </c>
-      <c r="C30" s="228" t="s">
-        <v>1152</v>
       </c>
       <c r="D30" s="228"/>
       <c r="E30" s="239"/>
     </row>
     <row r="31">
       <c r="A31" s="220" t="s">
+        <v>1152</v>
+      </c>
+      <c r="B31" s="238" t="s">
         <v>1153</v>
       </c>
-      <c r="B31" s="238" t="s">
+      <c r="C31" s="228" t="s">
         <v>1154</v>
-      </c>
-      <c r="C31" s="228" t="s">
-        <v>1155</v>
       </c>
       <c r="D31" s="228"/>
       <c r="E31" s="239"/>
     </row>
     <row r="32">
       <c r="A32" s="220" t="s">
+        <v>1155</v>
+      </c>
+      <c r="B32" s="238" t="s">
         <v>1156</v>
       </c>
-      <c r="B32" s="238" t="s">
+      <c r="C32" s="228" t="s">
         <v>1157</v>
-      </c>
-      <c r="C32" s="228" t="s">
-        <v>1158</v>
       </c>
       <c r="D32" s="228"/>
       <c r="E32" s="239"/>
     </row>
     <row r="33">
       <c r="A33" s="220" t="s">
+        <v>1158</v>
+      </c>
+      <c r="B33" s="238" t="s">
         <v>1159</v>
       </c>
-      <c r="B33" s="238" t="s">
+      <c r="C33" s="228" t="s">
         <v>1160</v>
-      </c>
-      <c r="C33" s="228" t="s">
-        <v>1161</v>
       </c>
       <c r="D33" s="228"/>
       <c r="E33" s="239"/>
     </row>
     <row r="34">
       <c r="A34" s="220" t="s">
+        <v>1161</v>
+      </c>
+      <c r="B34" s="238" t="s">
         <v>1162</v>
       </c>
-      <c r="B34" s="238" t="s">
+      <c r="C34" s="228" t="s">
         <v>1163</v>
-      </c>
-      <c r="C34" s="228" t="s">
-        <v>1164</v>
       </c>
       <c r="D34" s="228"/>
       <c r="E34" s="239"/>
     </row>
     <row r="35">
       <c r="A35" s="220" t="s">
+        <v>1164</v>
+      </c>
+      <c r="B35" s="238" t="s">
         <v>1165</v>
       </c>
-      <c r="B35" s="238" t="s">
+      <c r="C35" s="228" t="s">
         <v>1166</v>
-      </c>
-      <c r="C35" s="228" t="s">
-        <v>1167</v>
       </c>
       <c r="D35" s="228"/>
       <c r="E35" s="239"/>
     </row>
     <row r="36">
       <c r="A36" s="220" t="s">
+        <v>1167</v>
+      </c>
+      <c r="B36" s="238" t="s">
         <v>1168</v>
       </c>
-      <c r="B36" s="238" t="s">
+      <c r="C36" s="228" t="s">
         <v>1169</v>
-      </c>
-      <c r="C36" s="228" t="s">
-        <v>1170</v>
       </c>
       <c r="D36" s="228"/>
       <c r="E36" s="239"/>
     </row>
     <row r="37">
       <c r="A37" s="220" t="s">
+        <v>1170</v>
+      </c>
+      <c r="B37" s="238" t="s">
         <v>1171</v>
       </c>
-      <c r="B37" s="238" t="s">
+      <c r="C37" s="228" t="s">
         <v>1172</v>
-      </c>
-      <c r="C37" s="228" t="s">
-        <v>1173</v>
       </c>
       <c r="D37" s="228"/>
       <c r="E37" s="239"/>
     </row>
     <row r="38">
       <c r="A38" s="220" t="s">
+        <v>1173</v>
+      </c>
+      <c r="B38" s="238" t="s">
         <v>1174</v>
       </c>
-      <c r="B38" s="238" t="s">
+      <c r="C38" s="228" t="s">
         <v>1175</v>
-      </c>
-      <c r="C38" s="228" t="s">
-        <v>1176</v>
       </c>
       <c r="D38" s="228"/>
       <c r="E38" s="239"/>
     </row>
     <row r="39">
       <c r="A39" s="220" t="s">
+        <v>1176</v>
+      </c>
+      <c r="B39" s="240" t="s">
         <v>1177</v>
       </c>
-      <c r="B39" s="240" t="s">
+      <c r="C39" s="236" t="s">
         <v>1178</v>
-      </c>
-      <c r="C39" s="236" t="s">
-        <v>1179</v>
       </c>
       <c r="D39" s="236"/>
       <c r="E39" s="241"/>
@@ -16622,13 +16619,13 @@
     </row>
     <row r="40">
       <c r="A40" s="220" t="s">
+        <v>1179</v>
+      </c>
+      <c r="B40" s="240" t="s">
         <v>1180</v>
       </c>
-      <c r="B40" s="240" t="s">
+      <c r="C40" s="236" t="s">
         <v>1181</v>
-      </c>
-      <c r="C40" s="236" t="s">
-        <v>1182</v>
       </c>
       <c r="D40" s="236"/>
       <c r="E40" s="242"/>
@@ -16636,13 +16633,13 @@
     </row>
     <row r="41">
       <c r="A41" s="220" t="s">
+        <v>1182</v>
+      </c>
+      <c r="B41" s="240" t="s">
         <v>1183</v>
       </c>
-      <c r="B41" s="240" t="s">
+      <c r="C41" s="236" t="s">
         <v>1184</v>
-      </c>
-      <c r="C41" s="236" t="s">
-        <v>1185</v>
       </c>
       <c r="D41" s="236"/>
       <c r="E41" s="241"/>
@@ -16650,13 +16647,13 @@
     </row>
     <row r="42">
       <c r="A42" s="220" t="s">
+        <v>1185</v>
+      </c>
+      <c r="B42" s="240" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C42" s="243" t="s">
         <v>1186</v>
-      </c>
-      <c r="B42" s="240" t="s">
-        <v>1081</v>
-      </c>
-      <c r="C42" s="243" t="s">
-        <v>1187</v>
       </c>
       <c r="D42" s="243"/>
       <c r="E42" s="224"/>
@@ -16664,13 +16661,13 @@
     </row>
     <row r="43">
       <c r="A43" s="220" t="s">
+        <v>1187</v>
+      </c>
+      <c r="B43" s="244" t="s">
         <v>1188</v>
       </c>
-      <c r="B43" s="244" t="s">
+      <c r="C43" s="243" t="s">
         <v>1189</v>
-      </c>
-      <c r="C43" s="243" t="s">
-        <v>1190</v>
       </c>
       <c r="D43" s="243"/>
       <c r="E43" s="224"/>
@@ -16678,13 +16675,13 @@
     </row>
     <row r="44">
       <c r="A44" s="220" t="s">
+        <v>1190</v>
+      </c>
+      <c r="B44" s="244" t="s">
         <v>1191</v>
       </c>
-      <c r="B44" s="244" t="s">
+      <c r="C44" s="245" t="s">
         <v>1192</v>
-      </c>
-      <c r="C44" s="245" t="s">
-        <v>1193</v>
       </c>
       <c r="D44" s="245"/>
       <c r="E44" s="224"/>
@@ -16692,10 +16689,10 @@
     </row>
     <row r="45" ht="20.25" customHeight="1">
       <c r="A45" s="220" t="s">
+        <v>1193</v>
+      </c>
+      <c r="B45" s="14" t="s">
         <v>1194</v>
-      </c>
-      <c r="B45" s="14" t="s">
-        <v>1195</v>
       </c>
       <c r="C45" s="246" t="s">
         <v>308</v>
@@ -16706,10 +16703,10 @@
     </row>
     <row r="46">
       <c r="A46" s="220" t="s">
+        <v>1195</v>
+      </c>
+      <c r="B46" s="14" t="s">
         <v>1196</v>
-      </c>
-      <c r="B46" s="14" t="s">
-        <v>1197</v>
       </c>
       <c r="C46" s="15" t="s">
         <v>312</v>
@@ -16720,10 +16717,10 @@
     </row>
     <row r="47">
       <c r="A47" s="220" t="s">
+        <v>1197</v>
+      </c>
+      <c r="B47" s="14" t="s">
         <v>1198</v>
-      </c>
-      <c r="B47" s="14" t="s">
-        <v>1199</v>
       </c>
       <c r="C47" s="223" t="s">
         <v>315</v>
@@ -16734,10 +16731,10 @@
     </row>
     <row r="48">
       <c r="A48" s="220" t="s">
+        <v>1199</v>
+      </c>
+      <c r="B48" s="14" t="s">
         <v>1200</v>
-      </c>
-      <c r="B48" s="14" t="s">
-        <v>1201</v>
       </c>
       <c r="C48" s="223" t="s">
         <v>318</v>
@@ -16748,10 +16745,10 @@
     </row>
     <row r="49">
       <c r="A49" s="220" t="s">
+        <v>1201</v>
+      </c>
+      <c r="B49" s="14" t="s">
         <v>1202</v>
-      </c>
-      <c r="B49" s="14" t="s">
-        <v>1203</v>
       </c>
       <c r="C49" s="144" t="s">
         <v>321</v>
@@ -16762,10 +16759,10 @@
     </row>
     <row r="50">
       <c r="A50" s="220" t="s">
+        <v>1203</v>
+      </c>
+      <c r="B50" s="14" t="s">
         <v>1204</v>
-      </c>
-      <c r="B50" s="14" t="s">
-        <v>1205</v>
       </c>
       <c r="C50" s="144" t="s">
         <v>324</v>
@@ -16776,10 +16773,10 @@
     </row>
     <row r="51">
       <c r="A51" s="220" t="s">
+        <v>1205</v>
+      </c>
+      <c r="B51" s="14" t="s">
         <v>1206</v>
-      </c>
-      <c r="B51" s="14" t="s">
-        <v>1207</v>
       </c>
       <c r="C51" s="223" t="s">
         <v>327</v>
@@ -16790,10 +16787,10 @@
     </row>
     <row r="52">
       <c r="A52" s="220" t="s">
+        <v>1207</v>
+      </c>
+      <c r="B52" s="14" t="s">
         <v>1208</v>
-      </c>
-      <c r="B52" s="14" t="s">
-        <v>1209</v>
       </c>
       <c r="C52" s="144" t="s">
         <v>330</v>
@@ -16804,10 +16801,10 @@
     </row>
     <row r="53">
       <c r="A53" s="220" t="s">
+        <v>1209</v>
+      </c>
+      <c r="B53" s="14" t="s">
         <v>1210</v>
-      </c>
-      <c r="B53" s="14" t="s">
-        <v>1211</v>
       </c>
       <c r="C53" s="223" t="s">
         <v>333</v>
@@ -16818,10 +16815,10 @@
     </row>
     <row r="54">
       <c r="A54" s="247" t="s">
+        <v>1211</v>
+      </c>
+      <c r="B54" s="248" t="s">
         <v>1212</v>
-      </c>
-      <c r="B54" s="248" t="s">
-        <v>1213</v>
       </c>
       <c r="C54" s="249" t="s">
         <v>336</v>
@@ -16832,13 +16829,13 @@
     </row>
     <row r="55">
       <c r="A55" s="220" t="s">
+        <v>1213</v>
+      </c>
+      <c r="B55" s="5" t="s">
         <v>1214</v>
       </c>
-      <c r="B55" s="5" t="s">
+      <c r="C55" s="5" t="s">
         <v>1215</v>
-      </c>
-      <c r="C55" s="5" t="s">
-        <v>1216</v>
       </c>
       <c r="D55" s="5"/>
       <c r="E55" s="16"/>
@@ -16874,13 +16871,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>1216</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>1217</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>1218</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>1219</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>12</v>
@@ -16891,7 +16888,7 @@
     </row>
     <row r="2">
       <c r="A2" s="24" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="C2" s="14" t="s">
         <v>481</v>
@@ -16907,7 +16904,7 @@
     </row>
     <row r="3">
       <c r="A3" s="24" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="C3" s="14" t="s">
         <v>491</v>
@@ -16923,7 +16920,7 @@
     </row>
     <row r="4">
       <c r="A4" s="24" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="C4" s="14" t="s">
         <v>499</v>
@@ -16939,7 +16936,7 @@
     </row>
     <row r="5">
       <c r="A5" s="24" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="B5" s="16"/>
       <c r="C5" s="14" t="s">
@@ -16956,7 +16953,7 @@
     </row>
     <row r="6">
       <c r="A6" s="24" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="B6" s="16"/>
       <c r="C6" s="14" t="s">
@@ -16973,7 +16970,7 @@
     </row>
     <row r="7">
       <c r="A7" s="24" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="B7" s="16"/>
       <c r="C7" s="14" t="s">
@@ -16990,7 +16987,7 @@
     </row>
     <row r="8">
       <c r="A8" s="24" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
       <c r="B8" s="16"/>
       <c r="C8" s="14" t="s">
@@ -17007,7 +17004,7 @@
     </row>
     <row r="9">
       <c r="A9" s="24" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="B9" s="16"/>
       <c r="C9" s="14" t="s">
@@ -17024,7 +17021,7 @@
     </row>
     <row r="10">
       <c r="A10" s="24" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
       <c r="B10" s="16"/>
       <c r="C10" s="14" t="s">
@@ -17041,7 +17038,7 @@
     </row>
     <row r="11">
       <c r="A11" s="24" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
       <c r="B11" s="16"/>
       <c r="C11" s="14" t="s">
@@ -17058,7 +17055,7 @@
     </row>
     <row r="12">
       <c r="A12" s="24" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
       <c r="B12" s="16"/>
       <c r="C12" s="14" t="s">
@@ -17075,7 +17072,7 @@
     </row>
     <row r="13">
       <c r="A13" s="60" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
       <c r="B13" s="58"/>
       <c r="C13" s="56" t="s">
@@ -17092,7 +17089,7 @@
     </row>
     <row r="14">
       <c r="A14" s="60" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
       <c r="B14" s="58"/>
       <c r="C14" s="56" t="s">
@@ -17109,7 +17106,7 @@
     </row>
     <row r="15">
       <c r="A15" s="60" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="B15" s="58"/>
       <c r="C15" s="56" t="s">
@@ -17126,7 +17123,7 @@
     </row>
     <row r="16">
       <c r="A16" s="60" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
       <c r="B16" s="58"/>
       <c r="C16" s="56" t="s">
@@ -17143,7 +17140,7 @@
     </row>
     <row r="17">
       <c r="A17" s="60" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
       <c r="B17" s="58"/>
       <c r="C17" s="56" t="s">
@@ -17160,7 +17157,7 @@
     </row>
     <row r="18">
       <c r="A18" s="60" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
       <c r="B18" s="58"/>
       <c r="C18" s="56" t="s">
@@ -17177,7 +17174,7 @@
     </row>
     <row r="19">
       <c r="A19" s="24" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
       <c r="B19" s="16"/>
       <c r="C19" s="14" t="s">
@@ -17194,7 +17191,7 @@
     </row>
     <row r="20">
       <c r="A20" s="24" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
       <c r="B20" s="16"/>
       <c r="C20" s="14" t="s">
@@ -17211,7 +17208,7 @@
     </row>
     <row r="21">
       <c r="A21" s="24" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
       <c r="B21" s="16"/>
       <c r="C21" s="14" t="s">
@@ -17228,7 +17225,7 @@
     </row>
     <row r="22">
       <c r="A22" s="24" t="s">
-        <v>1240</v>
+        <v>1239</v>
       </c>
       <c r="B22" s="16"/>
       <c r="C22" s="14" t="s">
@@ -17245,7 +17242,7 @@
     </row>
     <row r="23">
       <c r="A23" s="24" t="s">
-        <v>1241</v>
+        <v>1240</v>
       </c>
       <c r="B23" s="16"/>
       <c r="C23" s="14" t="s">
@@ -17262,7 +17259,7 @@
     </row>
     <row r="24">
       <c r="A24" s="24" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
       <c r="B24" s="16"/>
       <c r="C24" s="14" t="s">
@@ -17279,14 +17276,14 @@
     </row>
     <row r="25">
       <c r="A25" s="24" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
       <c r="B25" s="16"/>
       <c r="C25" s="14" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="D25" s="14" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="E25" s="24" t="s">
         <v>416</v>
@@ -17296,14 +17293,14 @@
     </row>
     <row r="26">
       <c r="A26" s="24" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="B26" s="16"/>
       <c r="C26" s="14" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="D26" s="14" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="E26" s="24" t="s">
         <v>419</v>
@@ -17313,14 +17310,14 @@
     </row>
     <row r="27">
       <c r="A27" s="24" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
       <c r="B27" s="16"/>
       <c r="C27" s="14" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="D27" s="14" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="E27" s="24" t="s">
         <v>422</v>
@@ -17330,14 +17327,14 @@
     </row>
     <row r="28">
       <c r="A28" s="24" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
       <c r="B28" s="16"/>
       <c r="C28" s="14" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="D28" s="14" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="E28" s="24" t="s">
         <v>425</v>
@@ -17347,14 +17344,14 @@
     </row>
     <row r="29">
       <c r="A29" s="24" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
       <c r="B29" s="16"/>
       <c r="C29" s="14" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="D29" s="14" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="E29" s="24" t="s">
         <v>428</v>
@@ -17364,14 +17361,14 @@
     </row>
     <row r="30">
       <c r="A30" s="24" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
       <c r="B30" s="16"/>
       <c r="C30" s="14" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="D30" s="14" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="E30" s="24" t="s">
         <v>431</v>
@@ -17381,14 +17378,14 @@
     </row>
     <row r="31">
       <c r="A31" s="24" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
       <c r="B31" s="16"/>
       <c r="C31" s="14" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="D31" s="14" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="E31" s="24" t="s">
         <v>273</v>
@@ -17398,14 +17395,14 @@
     </row>
     <row r="32">
       <c r="A32" s="24" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
       <c r="B32" s="16"/>
       <c r="C32" s="14" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="D32" s="14" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="E32" s="24" t="s">
         <v>436</v>
@@ -17415,14 +17412,14 @@
     </row>
     <row r="33">
       <c r="A33" s="24" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
       <c r="B33" s="16"/>
       <c r="C33" s="14" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="D33" s="14" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="E33" s="24" t="s">
         <v>439</v>
@@ -17432,14 +17429,14 @@
     </row>
     <row r="34">
       <c r="A34" s="24" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
       <c r="B34" s="16"/>
       <c r="C34" s="14" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="D34" s="14" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="E34" s="24" t="s">
         <v>91</v>
@@ -17449,14 +17446,14 @@
     </row>
     <row r="35">
       <c r="A35" s="24" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
       <c r="B35" s="16"/>
       <c r="C35" s="14" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="D35" s="14" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="E35" s="24" t="s">
         <v>96</v>
@@ -17466,14 +17463,14 @@
     </row>
     <row r="36">
       <c r="A36" s="24" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
       <c r="B36" s="16"/>
       <c r="C36" s="14" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="D36" s="14" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="E36" s="24" t="s">
         <v>100</v>
@@ -17483,14 +17480,14 @@
     </row>
     <row r="37">
       <c r="A37" s="24" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
       <c r="B37" s="16"/>
       <c r="C37" s="14" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="D37" s="14" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="E37" s="24" t="s">
         <v>104</v>
@@ -17500,14 +17497,14 @@
     </row>
     <row r="38">
       <c r="A38" s="24" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="B38" s="16"/>
       <c r="C38" s="14" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="D38" s="14" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="E38" s="24" t="s">
         <v>108</v>
@@ -17517,14 +17514,14 @@
     </row>
     <row r="39">
       <c r="A39" s="24" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="B39" s="16"/>
       <c r="C39" s="14" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="D39" s="14" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="E39" s="24" t="s">
         <v>112</v>
@@ -17534,14 +17531,14 @@
     </row>
     <row r="40">
       <c r="A40" s="24" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
       <c r="B40" s="16"/>
       <c r="C40" s="14" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="D40" s="14" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="E40" s="24" t="s">
         <v>116</v>
@@ -17551,14 +17548,14 @@
     </row>
     <row r="41">
       <c r="A41" s="24" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
       <c r="B41" s="16"/>
       <c r="C41" s="14" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="D41" s="14" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="E41" s="24" t="s">
         <v>120</v>
@@ -17568,14 +17565,14 @@
     </row>
     <row r="42">
       <c r="A42" s="24" t="s">
-        <v>1260</v>
+        <v>1259</v>
       </c>
       <c r="B42" s="16"/>
       <c r="C42" s="14" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="D42" s="14" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="E42" s="24" t="s">
         <v>124</v>
@@ -17615,10 +17612,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>1260</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>1261</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>1262</v>
       </c>
     </row>
     <row r="2">
@@ -17628,7 +17625,7 @@
       <c r="B2" s="16"/>
       <c r="C2" s="16"/>
       <c r="D2" s="16" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="E2" s="16"/>
       <c r="F2" s="16"/>
@@ -17640,7 +17637,7 @@
       <c r="B3" s="16"/>
       <c r="C3" s="16"/>
       <c r="D3" s="16" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
       <c r="E3" s="16"/>
       <c r="F3" s="16"/>
@@ -17687,22 +17684,22 @@
         <v>462</v>
       </c>
       <c r="E1" s="253" t="s">
+        <v>1264</v>
+      </c>
+      <c r="F1" s="253" t="s">
         <v>1265</v>
       </c>
-      <c r="F1" s="253" t="s">
+      <c r="G1" s="5" t="s">
         <v>1266</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>1267</v>
       </c>
       <c r="H1" s="254" t="s">
         <v>471</v>
       </c>
       <c r="I1" s="5" t="s">
+        <v>1267</v>
+      </c>
+      <c r="J1" s="5" t="s">
         <v>1268</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>1269</v>
       </c>
     </row>
     <row r="2">
@@ -17710,16 +17707,16 @@
         <v>380</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>1269</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>1270</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>1271</v>
       </c>
       <c r="D2" s="255"/>
       <c r="F2" s="254"/>
       <c r="H2" s="256"/>
       <c r="J2" s="5" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
     </row>
     <row r="3">
@@ -17727,17 +17724,17 @@
         <v>383</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>1272</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>1273</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>1274</v>
       </c>
       <c r="D3" s="256"/>
       <c r="E3" s="254"/>
       <c r="F3" s="254"/>
       <c r="H3" s="254"/>
       <c r="J3" s="5" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
     </row>
     <row r="4">
@@ -17745,17 +17742,17 @@
         <v>386</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>1275</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>1276</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>1277</v>
       </c>
       <c r="D4" s="256"/>
       <c r="E4" s="254"/>
       <c r="F4" s="254"/>
       <c r="H4" s="254"/>
       <c r="J4" s="5" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
     </row>
     <row r="5">
@@ -17763,17 +17760,17 @@
         <v>388</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>1277</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>1278</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>1279</v>
       </c>
       <c r="D5" s="254"/>
       <c r="E5" s="254"/>
       <c r="F5" s="254"/>
       <c r="H5" s="256"/>
       <c r="J5" s="5" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="6">
@@ -17781,10 +17778,10 @@
         <v>391</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>1280</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>1281</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>1282</v>
       </c>
       <c r="D6" s="254"/>
       <c r="E6" s="116"/>
@@ -17793,7 +17790,7 @@
         <v>458</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="7">
@@ -17801,17 +17798,17 @@
         <v>398</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>1283</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>1284</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>1285</v>
       </c>
       <c r="D7" s="254"/>
       <c r="E7" s="254"/>
       <c r="F7" s="254"/>
       <c r="H7" s="254"/>
       <c r="J7" s="5" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="8">
@@ -17819,10 +17816,10 @@
         <v>412</v>
       </c>
       <c r="B8" s="5" t="s">
+        <v>1286</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>1287</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>1288</v>
       </c>
       <c r="D8" s="254"/>
       <c r="E8" s="254"/>
@@ -17830,7 +17827,7 @@
       <c r="G8" s="254"/>
       <c r="H8" s="254"/>
       <c r="J8" s="5" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
     </row>
     <row r="9">
@@ -17838,17 +17835,17 @@
         <v>418</v>
       </c>
       <c r="B9" s="5" t="s">
+        <v>1289</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>1290</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>1291</v>
       </c>
       <c r="D9" s="254"/>
       <c r="E9" s="254"/>
       <c r="F9" s="254"/>
       <c r="H9" s="254"/>
       <c r="J9" s="5" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="10">
@@ -17856,17 +17853,17 @@
         <v>424</v>
       </c>
       <c r="B10" s="5" t="s">
+        <v>1291</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>1292</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>1293</v>
       </c>
       <c r="D10" s="254"/>
       <c r="E10" s="254"/>
       <c r="F10" s="254"/>
       <c r="H10" s="256"/>
       <c r="J10" s="5" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
     </row>
     <row r="11">
@@ -17874,10 +17871,10 @@
         <v>430</v>
       </c>
       <c r="B11" s="5" t="s">
+        <v>1294</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>1295</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>1296</v>
       </c>
       <c r="D11" s="254"/>
       <c r="E11" s="254"/>
@@ -17885,7 +17882,7 @@
       <c r="G11" s="254"/>
       <c r="H11" s="254"/>
       <c r="J11" s="14" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
     </row>
     <row r="12">
@@ -17893,10 +17890,10 @@
         <v>415</v>
       </c>
       <c r="B12" s="5" t="s">
+        <v>1296</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>1297</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>1298</v>
       </c>
       <c r="D12" s="254"/>
       <c r="E12" s="254"/>
@@ -17904,7 +17901,7 @@
       <c r="G12" s="254"/>
       <c r="H12" s="254"/>
       <c r="J12" s="5" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
     </row>
     <row r="13">
@@ -17912,17 +17909,17 @@
         <v>421</v>
       </c>
       <c r="B13" s="5" t="s">
+        <v>1298</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>1299</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>1300</v>
       </c>
       <c r="D13" s="254"/>
       <c r="E13" s="254"/>
       <c r="F13" s="254"/>
       <c r="H13" s="254"/>
       <c r="J13" s="5" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="14">
@@ -17930,17 +17927,17 @@
         <v>427</v>
       </c>
       <c r="B14" s="5" t="s">
+        <v>1300</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>1301</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>1302</v>
       </c>
       <c r="D14" s="254"/>
       <c r="E14" s="254"/>
       <c r="F14" s="254"/>
       <c r="H14" s="256"/>
       <c r="J14" s="5" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
     </row>
     <row r="15">
@@ -17948,10 +17945,10 @@
         <v>433</v>
       </c>
       <c r="B15" s="5" t="s">
+        <v>1302</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>1303</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>1304</v>
       </c>
       <c r="D15" s="254"/>
       <c r="E15" s="254"/>
@@ -17959,7 +17956,7 @@
       <c r="G15" s="254"/>
       <c r="H15" s="254"/>
       <c r="J15" s="14" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
     </row>
     <row r="16">
@@ -17967,10 +17964,10 @@
         <v>435</v>
       </c>
       <c r="B16" s="5" t="s">
+        <v>1304</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>1305</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>1306</v>
       </c>
       <c r="D16" s="256"/>
       <c r="E16" s="254"/>
@@ -17979,7 +17976,7 @@
         <v>458</v>
       </c>
       <c r="J16" s="258" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
     </row>
     <row r="17">
@@ -17987,18 +17984,18 @@
         <v>438</v>
       </c>
       <c r="B17" s="5" t="s">
+        <v>1306</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>1307</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>1308</v>
       </c>
       <c r="E17" s="254"/>
       <c r="F17" s="259"/>
       <c r="H17" s="260" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="J17" s="258" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
     </row>
     <row r="18">
@@ -18006,10 +18003,10 @@
         <v>442</v>
       </c>
       <c r="B18" s="5" t="s">
+        <v>1309</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>1310</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>1311</v>
       </c>
       <c r="E18" s="254"/>
       <c r="F18" s="259"/>
@@ -18017,7 +18014,7 @@
         <v>458</v>
       </c>
       <c r="J18" s="258" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
     </row>
   </sheetData>
@@ -18043,66 +18040,66 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="261" t="s">
+        <v>1312</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>1313</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="5" t="s">
         <v>1314</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>1315</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="261" t="s">
+        <v>1315</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>1316</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>1317</v>
-      </c>
       <c r="C3" s="5" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="261" t="s">
+        <v>1317</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>1318</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>1319</v>
-      </c>
       <c r="C4" s="5" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" s="5" t="s">
-        <v>1320</v>
+        <v>1319</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="5"/>
       <c r="B6" s="262" t="s">
+        <v>1320</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>1321</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>1322</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="5"/>
       <c r="B7" s="262" t="s">
-        <v>1323</v>
+        <v>1322</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
aacar-11 remove incorrect duplicate terminals in right ventricle
</commit_message>
<xml_diff>
--- a/models/ard-arm-cardiac/source/ard-arm-cardiac.xlsx
+++ b/models/ard-arm-cardiac/source/ard-arm-cardiac.xlsx
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2557" uniqueCount="1492">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2543" uniqueCount="1488">
   <si>
     <t>id</t>
   </si>
@@ -3013,25 +3013,10 @@
     <t>A74,A75,A75</t>
   </si>
   <si>
-    <t>dc-sn-rv_11</t>
-  </si>
-  <si>
-    <t>Dendrite from heart_layer 5 of heart to right ventricle and aorta_Neuron 11 (aacar)</t>
-  </si>
-  <si>
-    <t>ns168_3</t>
-  </si>
-  <si>
-    <t>dc-sn-rv2_11</t>
-  </si>
-  <si>
-    <t>Dendrite from heart_layer 5 to heart rv2_Neuron 11 (aacar)</t>
-  </si>
-  <si>
-    <t>ns168_4</t>
-  </si>
-  <si>
-    <t>dc-sn-la-mus_11</t>
+    <t>dc-sn-rv-mus_11</t>
+  </si>
+  <si>
+    <t>Dendrite from heart to right ventricle layer 2_Neuron 11 (aacar)</t>
   </si>
   <si>
     <t>ns168_1</t>
@@ -3040,7 +3025,10 @@
     <t>A74,A76</t>
   </si>
   <si>
-    <t>dc-sn-la-end_11</t>
+    <t>dc-sn-rv-end_11</t>
+  </si>
+  <si>
+    <t>Dendrite from heart to right ventricle layer 1_Neuron 11 (aacar)</t>
   </si>
   <si>
     <t>ns168_2</t>
@@ -6063,122 +6051,122 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="114" t="s">
-        <v>1421</v>
+        <v>1417</v>
       </c>
       <c r="B1" s="114" t="s">
-        <v>1422</v>
+        <v>1418</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="283" t="s">
-        <v>1423</v>
+        <v>1419</v>
       </c>
       <c r="B2" s="284" t="s">
-        <v>1424</v>
+        <v>1420</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="283" t="s">
-        <v>1425</v>
+        <v>1421</v>
       </c>
       <c r="B3" s="284" t="s">
-        <v>1426</v>
+        <v>1422</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="283" t="s">
-        <v>1427</v>
+        <v>1423</v>
       </c>
       <c r="B4" s="285" t="s">
-        <v>1428</v>
+        <v>1424</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="283" t="s">
-        <v>1429</v>
+        <v>1425</v>
       </c>
       <c r="B5" s="285" t="s">
-        <v>1430</v>
+        <v>1426</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="283" t="s">
-        <v>1431</v>
+        <v>1427</v>
       </c>
       <c r="B6" s="285" t="s">
-        <v>1432</v>
+        <v>1428</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="283" t="s">
-        <v>1433</v>
+        <v>1429</v>
       </c>
       <c r="B7" s="285" t="s">
-        <v>1434</v>
+        <v>1430</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="283" t="s">
-        <v>1435</v>
+        <v>1431</v>
       </c>
       <c r="B8" s="285" t="s">
-        <v>1436</v>
+        <v>1432</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="283" t="s">
-        <v>1437</v>
+        <v>1433</v>
       </c>
       <c r="B9" s="285" t="s">
-        <v>1438</v>
+        <v>1434</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="283" t="s">
-        <v>1439</v>
+        <v>1435</v>
       </c>
       <c r="B10" s="285" t="s">
-        <v>1440</v>
+        <v>1436</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="283" t="s">
-        <v>1441</v>
+        <v>1437</v>
       </c>
       <c r="B11" s="285" t="s">
-        <v>1442</v>
+        <v>1438</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="5" t="s">
-        <v>1443</v>
+        <v>1439</v>
       </c>
       <c r="B12" s="284" t="s">
-        <v>1444</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="31" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="B13" s="284" t="s">
-        <v>1446</v>
+        <v>1442</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="31" t="s">
-        <v>1447</v>
+        <v>1443</v>
       </c>
       <c r="B14" s="284" t="s">
-        <v>1448</v>
+        <v>1444</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="14" t="s">
-        <v>1449</v>
+        <v>1445</v>
       </c>
       <c r="B15" s="116" t="s">
-        <v>1450</v>
+        <v>1446</v>
       </c>
     </row>
   </sheetData>
@@ -6214,16 +6202,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="16" t="s">
-        <v>1451</v>
+        <v>1447</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>1452</v>
+        <v>1448</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>1453</v>
+        <v>1449</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>1454</v>
+        <v>1450</v>
       </c>
       <c r="E1" s="16"/>
       <c r="F1" s="16"/>
@@ -6239,13 +6227,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>1455</v>
+        <v>1451</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>1456</v>
+        <v>1452</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>1457</v>
+        <v>1453</v>
       </c>
       <c r="E2" s="16"/>
       <c r="F2" s="16"/>
@@ -6286,13 +6274,13 @@
     </row>
     <row r="5">
       <c r="A5" s="16" t="s">
-        <v>1458</v>
+        <v>1454</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>1459</v>
+        <v>1455</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>1460</v>
+        <v>1456</v>
       </c>
       <c r="D5" s="16"/>
       <c r="E5" s="16"/>
@@ -6309,10 +6297,10 @@
         <v>0</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>1461</v>
+        <v>1457</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>1462</v>
+        <v>1458</v>
       </c>
       <c r="D6" s="16"/>
       <c r="E6" s="16"/>
@@ -6327,10 +6315,10 @@
     <row r="7">
       <c r="A7" s="16"/>
       <c r="B7" s="16" t="s">
-        <v>1463</v>
+        <v>1459</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>1462</v>
+        <v>1458</v>
       </c>
       <c r="D7" s="16"/>
       <c r="E7" s="16"/>
@@ -6345,10 +6333,10 @@
     <row r="8">
       <c r="A8" s="16"/>
       <c r="B8" s="16" t="s">
-        <v>1464</v>
+        <v>1460</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>1462</v>
+        <v>1458</v>
       </c>
       <c r="D8" s="16"/>
       <c r="E8" s="16"/>
@@ -6363,10 +6351,10 @@
     <row r="9">
       <c r="A9" s="16"/>
       <c r="B9" s="16" t="s">
-        <v>1465</v>
+        <v>1461</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1462</v>
+        <v>1458</v>
       </c>
       <c r="D9" s="16"/>
       <c r="E9" s="16"/>
@@ -6394,10 +6382,10 @@
     </row>
     <row r="11">
       <c r="A11" s="16" t="s">
-        <v>1466</v>
+        <v>1462</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>1467</v>
+        <v>1463</v>
       </c>
       <c r="C11" s="16"/>
       <c r="D11" s="16"/>
@@ -6412,10 +6400,10 @@
     </row>
     <row r="12">
       <c r="A12" s="16" t="s">
-        <v>1468</v>
+        <v>1464</v>
       </c>
       <c r="B12" s="286" t="s">
-        <v>1469</v>
+        <v>1465</v>
       </c>
       <c r="C12" s="16"/>
       <c r="D12" s="16"/>
@@ -6430,10 +6418,10 @@
     </row>
     <row r="13">
       <c r="A13" s="16" t="s">
-        <v>1470</v>
+        <v>1466</v>
       </c>
       <c r="B13" s="286" t="s">
-        <v>1471</v>
+        <v>1467</v>
       </c>
       <c r="C13" s="16"/>
       <c r="D13" s="16"/>
@@ -6448,10 +6436,10 @@
     </row>
     <row r="14">
       <c r="A14" s="16" t="s">
-        <v>1472</v>
+        <v>1468</v>
       </c>
       <c r="B14" s="286" t="s">
-        <v>1473</v>
+        <v>1469</v>
       </c>
       <c r="C14" s="16"/>
       <c r="D14" s="16"/>
@@ -6466,10 +6454,10 @@
     </row>
     <row r="15">
       <c r="A15" s="16" t="s">
-        <v>1474</v>
+        <v>1470</v>
       </c>
       <c r="B15" s="286" t="s">
-        <v>1475</v>
+        <v>1471</v>
       </c>
       <c r="C15" s="16"/>
       <c r="D15" s="16"/>
@@ -6484,10 +6472,10 @@
     </row>
     <row r="16">
       <c r="A16" s="14" t="s">
-        <v>1476</v>
+        <v>1472</v>
       </c>
       <c r="B16" s="98" t="s">
-        <v>1477</v>
+        <v>1473</v>
       </c>
       <c r="C16" s="16"/>
       <c r="D16" s="16"/>
@@ -6502,10 +6490,10 @@
     </row>
     <row r="17">
       <c r="A17" s="14" t="s">
-        <v>1478</v>
+        <v>1474</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>1368</v>
+        <v>1364</v>
       </c>
       <c r="C17" s="16"/>
       <c r="D17" s="16"/>
@@ -6534,10 +6522,10 @@
     </row>
     <row r="19">
       <c r="A19" s="16" t="s">
-        <v>1479</v>
+        <v>1475</v>
       </c>
       <c r="B19" s="98" t="s">
-        <v>1480</v>
+        <v>1476</v>
       </c>
       <c r="C19" s="16"/>
       <c r="D19" s="16"/>
@@ -6552,7 +6540,7 @@
     </row>
     <row r="20">
       <c r="A20" s="16" t="s">
-        <v>1481</v>
+        <v>1477</v>
       </c>
       <c r="B20" s="123" t="s">
         <v>6</v>
@@ -6570,10 +6558,10 @@
     </row>
     <row r="21">
       <c r="A21" s="16" t="s">
-        <v>1482</v>
+        <v>1478</v>
       </c>
       <c r="B21" s="123" t="s">
-        <v>1483</v>
+        <v>1479</v>
       </c>
       <c r="L21" s="16"/>
     </row>
@@ -6603,28 +6591,28 @@
     </row>
     <row r="28">
       <c r="A28" s="287" t="s">
-        <v>1484</v>
+        <v>1480</v>
       </c>
       <c r="B28" s="288" t="s">
-        <v>1485</v>
+        <v>1481</v>
       </c>
       <c r="L28" s="16"/>
     </row>
     <row r="29">
       <c r="A29" s="287" t="s">
-        <v>1486</v>
+        <v>1482</v>
       </c>
       <c r="B29" s="289" t="s">
-        <v>1487</v>
+        <v>1483</v>
       </c>
       <c r="L29" s="16"/>
     </row>
     <row r="30">
       <c r="A30" s="287" t="s">
-        <v>1488</v>
+        <v>1484</v>
       </c>
       <c r="B30" s="290" t="s">
-        <v>1489</v>
+        <v>1485</v>
       </c>
       <c r="C30" s="288"/>
       <c r="D30" s="288"/>
@@ -6639,13 +6627,13 @@
     </row>
     <row r="31" hidden="1">
       <c r="A31" s="16" t="s">
-        <v>1490</v>
+        <v>1486</v>
       </c>
       <c r="L31" s="16"/>
     </row>
     <row r="32" hidden="1">
       <c r="A32" s="16" t="s">
-        <v>1491</v>
+        <v>1487</v>
       </c>
       <c r="L32" s="16"/>
     </row>
@@ -15746,29 +15734,29 @@
         <v>374</v>
       </c>
       <c r="F140" s="38" t="s">
-        <v>946</v>
-      </c>
-      <c r="G140" s="151" t="s">
+        <v>964</v>
+      </c>
+      <c r="G140" s="38" t="s">
         <v>988</v>
       </c>
       <c r="H140" s="42"/>
       <c r="I140" s="40"/>
       <c r="J140" s="40"/>
-      <c r="K140" s="144">
-        <v>1.0</v>
+      <c r="K140" s="216" t="s">
+        <v>744</v>
       </c>
       <c r="L140" s="155" t="s">
-        <v>287</v>
+        <v>989</v>
       </c>
       <c r="M140" s="155"/>
-      <c r="N140" s="40"/>
+      <c r="N140" s="38"/>
     </row>
     <row r="141">
       <c r="A141" s="140" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="B141" s="214" t="s">
-        <v>990</v>
+        <v>991</v>
       </c>
       <c r="C141" s="156" t="s">
         <v>509</v>
@@ -15778,61 +15766,61 @@
         <v>374</v>
       </c>
       <c r="F141" s="38" t="s">
-        <v>946</v>
-      </c>
-      <c r="G141" s="151" t="s">
-        <v>991</v>
+        <v>968</v>
+      </c>
+      <c r="G141" s="38" t="s">
+        <v>992</v>
       </c>
       <c r="H141" s="42"/>
       <c r="I141" s="40"/>
       <c r="J141" s="40"/>
-      <c r="K141" s="144">
-        <v>2.0</v>
+      <c r="K141" s="216" t="s">
+        <v>749</v>
       </c>
       <c r="L141" s="155" t="s">
-        <v>287</v>
+        <v>993</v>
       </c>
       <c r="M141" s="155"/>
-      <c r="N141" s="40"/>
+      <c r="N141" s="38"/>
     </row>
     <row r="142">
       <c r="A142" s="140" t="s">
-        <v>992</v>
+        <v>994</v>
       </c>
       <c r="B142" s="214" t="s">
-        <v>957</v>
+        <v>995</v>
       </c>
       <c r="C142" s="156" t="s">
         <v>509</v>
       </c>
       <c r="D142" s="45"/>
-      <c r="E142" s="142" t="s">
-        <v>374</v>
+      <c r="E142" s="140" t="s">
+        <v>377</v>
       </c>
       <c r="F142" s="38" t="s">
         <v>964</v>
       </c>
-      <c r="G142" s="38" t="s">
-        <v>993</v>
+      <c r="G142" s="151" t="s">
+        <v>996</v>
       </c>
       <c r="H142" s="42"/>
       <c r="I142" s="40"/>
       <c r="J142" s="40"/>
-      <c r="K142" s="216" t="s">
-        <v>744</v>
+      <c r="K142" s="144">
+        <v>0.0</v>
       </c>
       <c r="L142" s="155" t="s">
-        <v>994</v>
+        <v>277</v>
       </c>
       <c r="M142" s="155"/>
-      <c r="N142" s="38"/>
+      <c r="N142" s="40"/>
     </row>
     <row r="143">
       <c r="A143" s="140" t="s">
-        <v>995</v>
+        <v>997</v>
       </c>
       <c r="B143" s="214" t="s">
-        <v>960</v>
+        <v>998</v>
       </c>
       <c r="C143" s="156" t="s">
         <v>509</v>
@@ -15842,125 +15830,125 @@
         <v>374</v>
       </c>
       <c r="F143" s="38" t="s">
-        <v>968</v>
-      </c>
-      <c r="G143" s="38" t="s">
         <v>996</v>
+      </c>
+      <c r="G143" s="151" t="s">
+        <v>999</v>
       </c>
       <c r="H143" s="42"/>
       <c r="I143" s="40"/>
       <c r="J143" s="40"/>
-      <c r="K143" s="216" t="s">
-        <v>749</v>
+      <c r="K143" s="144" t="s">
+        <v>1000</v>
       </c>
       <c r="L143" s="155" t="s">
-        <v>997</v>
+        <v>1001</v>
       </c>
       <c r="M143" s="155"/>
-      <c r="N143" s="38"/>
+      <c r="N143" s="40"/>
     </row>
     <row r="144">
-      <c r="A144" s="140" t="s">
-        <v>998</v>
-      </c>
-      <c r="B144" s="214" t="s">
-        <v>999</v>
-      </c>
-      <c r="C144" s="156" t="s">
+      <c r="A144" s="217" t="s">
+        <v>1002</v>
+      </c>
+      <c r="B144" s="218" t="s">
+        <v>1003</v>
+      </c>
+      <c r="C144" s="219" t="s">
         <v>509</v>
       </c>
-      <c r="D144" s="45"/>
-      <c r="E144" s="140" t="s">
+      <c r="D144" s="219"/>
+      <c r="E144" s="220" t="s">
+        <v>374</v>
+      </c>
+      <c r="F144" s="38" t="s">
+        <v>996</v>
+      </c>
+      <c r="G144" s="151" t="s">
+        <v>1004</v>
+      </c>
+      <c r="H144" s="221"/>
+      <c r="I144" s="222"/>
+      <c r="J144" s="222"/>
+      <c r="K144" s="223" t="s">
+        <v>1000</v>
+      </c>
+      <c r="L144" s="224" t="s">
+        <v>1005</v>
+      </c>
+      <c r="M144" s="224"/>
+      <c r="N144" s="222"/>
+    </row>
+    <row r="145">
+      <c r="A145" s="20" t="s">
+        <v>1006</v>
+      </c>
+      <c r="B145" s="122" t="s">
+        <v>1007</v>
+      </c>
+      <c r="C145" s="212" t="s">
+        <v>509</v>
+      </c>
+      <c r="D145" s="31"/>
+      <c r="E145" s="20" t="s">
         <v>377</v>
       </c>
-      <c r="F144" s="38" t="s">
-        <v>964</v>
-      </c>
-      <c r="G144" s="151" t="s">
-        <v>1000</v>
-      </c>
-      <c r="H144" s="42"/>
-      <c r="I144" s="40"/>
-      <c r="J144" s="40"/>
-      <c r="K144" s="144">
+      <c r="F145" s="14" t="s">
+        <v>1008</v>
+      </c>
+      <c r="G145" s="225" t="s">
+        <v>1009</v>
+      </c>
+      <c r="H145" s="13"/>
+      <c r="I145" s="16"/>
+      <c r="J145" s="16"/>
+      <c r="K145" s="128">
         <v>0.0</v>
       </c>
-      <c r="L144" s="155" t="s">
-        <v>277</v>
-      </c>
-      <c r="M144" s="155"/>
-      <c r="N144" s="40"/>
-    </row>
-    <row r="145">
-      <c r="A145" s="140" t="s">
-        <v>1001</v>
-      </c>
-      <c r="B145" s="214" t="s">
-        <v>1002</v>
-      </c>
-      <c r="C145" s="156" t="s">
-        <v>509</v>
-      </c>
-      <c r="D145" s="45"/>
-      <c r="E145" s="142" t="s">
-        <v>374</v>
-      </c>
-      <c r="F145" s="38" t="s">
-        <v>1000</v>
-      </c>
-      <c r="G145" s="151" t="s">
-        <v>1003</v>
-      </c>
-      <c r="H145" s="42"/>
-      <c r="I145" s="40"/>
-      <c r="J145" s="40"/>
-      <c r="K145" s="144" t="s">
-        <v>1004</v>
-      </c>
-      <c r="L145" s="155" t="s">
-        <v>1005</v>
-      </c>
-      <c r="M145" s="155"/>
-      <c r="N145" s="40"/>
+      <c r="L145" s="158" t="s">
+        <v>233</v>
+      </c>
+      <c r="M145" s="158"/>
+      <c r="N145" s="16"/>
     </row>
     <row r="146">
-      <c r="A146" s="217" t="s">
-        <v>1006</v>
-      </c>
-      <c r="B146" s="218" t="s">
-        <v>1007</v>
-      </c>
-      <c r="C146" s="219" t="s">
-        <v>509</v>
-      </c>
-      <c r="D146" s="219"/>
-      <c r="E146" s="220" t="s">
-        <v>374</v>
-      </c>
-      <c r="F146" s="38" t="s">
-        <v>1000</v>
-      </c>
-      <c r="G146" s="151" t="s">
-        <v>1008</v>
-      </c>
-      <c r="H146" s="221"/>
-      <c r="I146" s="222"/>
-      <c r="J146" s="222"/>
-      <c r="K146" s="223" t="s">
-        <v>1004</v>
-      </c>
-      <c r="L146" s="224" t="s">
-        <v>1009</v>
-      </c>
-      <c r="M146" s="224"/>
-      <c r="N146" s="222"/>
+      <c r="A146" s="20" t="s">
+        <v>1010</v>
+      </c>
+      <c r="B146" s="122" t="s">
+        <v>1011</v>
+      </c>
+      <c r="C146" s="212" t="s">
+        <v>514</v>
+      </c>
+      <c r="D146" s="31"/>
+      <c r="E146" s="20" t="s">
+        <v>367</v>
+      </c>
+      <c r="F146" s="14" t="s">
+        <v>1012</v>
+      </c>
+      <c r="G146" s="14" t="s">
+        <v>1013</v>
+      </c>
+      <c r="H146" s="13"/>
+      <c r="I146" s="16"/>
+      <c r="J146" s="16"/>
+      <c r="K146" s="128">
+        <v>0.0</v>
+      </c>
+      <c r="L146" s="158" t="s">
+        <v>233</v>
+      </c>
+      <c r="M146" s="158"/>
+      <c r="N146" s="16"/>
     </row>
     <row r="147">
       <c r="A147" s="20" t="s">
-        <v>1010</v>
+        <v>1014</v>
       </c>
       <c r="B147" s="122" t="s">
-        <v>1011</v>
+        <v>1015</v>
       </c>
       <c r="C147" s="212" t="s">
         <v>509</v>
@@ -15970,10 +15958,10 @@
         <v>377</v>
       </c>
       <c r="F147" s="14" t="s">
-        <v>1012</v>
+        <v>1016</v>
       </c>
       <c r="G147" s="225" t="s">
-        <v>1013</v>
+        <v>1009</v>
       </c>
       <c r="H147" s="13"/>
       <c r="I147" s="16"/>
@@ -15982,17 +15970,17 @@
         <v>0.0</v>
       </c>
       <c r="L147" s="158" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="M147" s="158"/>
       <c r="N147" s="16"/>
     </row>
     <row r="148">
       <c r="A148" s="20" t="s">
-        <v>1014</v>
+        <v>1017</v>
       </c>
       <c r="B148" s="122" t="s">
-        <v>1015</v>
+        <v>1018</v>
       </c>
       <c r="C148" s="212" t="s">
         <v>514</v>
@@ -16001,11 +15989,11 @@
       <c r="E148" s="20" t="s">
         <v>367</v>
       </c>
-      <c r="F148" s="14" t="s">
-        <v>1016</v>
-      </c>
-      <c r="G148" s="14" t="s">
-        <v>1017</v>
+      <c r="F148" s="5" t="s">
+        <v>1019</v>
+      </c>
+      <c r="G148" s="5" t="s">
+        <v>1020</v>
       </c>
       <c r="H148" s="13"/>
       <c r="I148" s="16"/>
@@ -16014,177 +16002,177 @@
         <v>0.0</v>
       </c>
       <c r="L148" s="158" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="M148" s="158"/>
       <c r="N148" s="16"/>
     </row>
     <row r="149">
-      <c r="A149" s="20" t="s">
-        <v>1018</v>
+      <c r="A149" s="130" t="s">
+        <v>1021</v>
       </c>
       <c r="B149" s="122" t="s">
-        <v>1019</v>
+        <v>1022</v>
       </c>
       <c r="C149" s="212" t="s">
         <v>509</v>
       </c>
       <c r="D149" s="31"/>
-      <c r="E149" s="20" t="s">
-        <v>377</v>
-      </c>
-      <c r="F149" s="14" t="s">
-        <v>1020</v>
-      </c>
-      <c r="G149" s="225" t="s">
-        <v>1013</v>
+      <c r="E149" s="21" t="s">
+        <v>374</v>
+      </c>
+      <c r="F149" s="225" t="s">
+        <v>1009</v>
+      </c>
+      <c r="G149" s="5" t="s">
+        <v>1023</v>
       </c>
       <c r="H149" s="13"/>
       <c r="I149" s="16"/>
       <c r="J149" s="16"/>
-      <c r="K149" s="128">
-        <v>0.0</v>
+      <c r="K149" s="128" t="s">
+        <v>1000</v>
       </c>
       <c r="L149" s="158" t="s">
-        <v>228</v>
+        <v>1024</v>
       </c>
       <c r="M149" s="158"/>
       <c r="N149" s="16"/>
     </row>
     <row r="150">
-      <c r="A150" s="20" t="s">
-        <v>1021</v>
+      <c r="A150" s="130" t="s">
+        <v>1025</v>
       </c>
       <c r="B150" s="122" t="s">
-        <v>1022</v>
+        <v>1026</v>
       </c>
       <c r="C150" s="212" t="s">
-        <v>514</v>
+        <v>509</v>
       </c>
       <c r="D150" s="31"/>
-      <c r="E150" s="20" t="s">
-        <v>367</v>
-      </c>
-      <c r="F150" s="5" t="s">
-        <v>1023</v>
+      <c r="E150" s="21" t="s">
+        <v>374</v>
+      </c>
+      <c r="F150" s="225" t="s">
+        <v>1009</v>
       </c>
       <c r="G150" s="5" t="s">
-        <v>1024</v>
+        <v>1027</v>
       </c>
       <c r="H150" s="13"/>
       <c r="I150" s="16"/>
       <c r="J150" s="16"/>
-      <c r="K150" s="128">
-        <v>0.0</v>
+      <c r="K150" s="128" t="s">
+        <v>1000</v>
       </c>
       <c r="L150" s="158" t="s">
-        <v>228</v>
+        <v>1028</v>
       </c>
       <c r="M150" s="158"/>
       <c r="N150" s="16"/>
     </row>
     <row r="151">
-      <c r="A151" s="130" t="s">
-        <v>1025</v>
-      </c>
-      <c r="B151" s="122" t="s">
-        <v>1026</v>
-      </c>
-      <c r="C151" s="212" t="s">
+      <c r="A151" s="140" t="s">
+        <v>1029</v>
+      </c>
+      <c r="B151" s="214" t="s">
+        <v>1030</v>
+      </c>
+      <c r="C151" s="156" t="s">
         <v>509</v>
       </c>
-      <c r="D151" s="31"/>
-      <c r="E151" s="21" t="s">
-        <v>374</v>
-      </c>
-      <c r="F151" s="225" t="s">
-        <v>1013</v>
-      </c>
-      <c r="G151" s="5" t="s">
-        <v>1027</v>
-      </c>
-      <c r="H151" s="13"/>
-      <c r="I151" s="16"/>
-      <c r="J151" s="16"/>
-      <c r="K151" s="128" t="s">
-        <v>1004</v>
-      </c>
-      <c r="L151" s="158" t="s">
-        <v>1028</v>
-      </c>
-      <c r="M151" s="158"/>
-      <c r="N151" s="16"/>
+      <c r="D151" s="45"/>
+      <c r="E151" s="140" t="s">
+        <v>377</v>
+      </c>
+      <c r="F151" s="38" t="s">
+        <v>1031</v>
+      </c>
+      <c r="G151" s="151" t="s">
+        <v>1032</v>
+      </c>
+      <c r="H151" s="42"/>
+      <c r="I151" s="40"/>
+      <c r="J151" s="40"/>
+      <c r="K151" s="137" t="s">
+        <v>615</v>
+      </c>
+      <c r="L151" s="155" t="s">
+        <v>1033</v>
+      </c>
+      <c r="M151" s="155"/>
+      <c r="N151" s="40"/>
     </row>
     <row r="152">
-      <c r="A152" s="130" t="s">
-        <v>1029</v>
-      </c>
-      <c r="B152" s="122" t="s">
-        <v>1030</v>
-      </c>
-      <c r="C152" s="212" t="s">
-        <v>509</v>
-      </c>
-      <c r="D152" s="31"/>
-      <c r="E152" s="21" t="s">
-        <v>374</v>
-      </c>
-      <c r="F152" s="225" t="s">
-        <v>1013</v>
-      </c>
-      <c r="G152" s="5" t="s">
-        <v>1031</v>
-      </c>
-      <c r="H152" s="13"/>
-      <c r="I152" s="16"/>
-      <c r="J152" s="16"/>
-      <c r="K152" s="128" t="s">
-        <v>1004</v>
-      </c>
-      <c r="L152" s="158" t="s">
-        <v>1032</v>
-      </c>
-      <c r="M152" s="158"/>
-      <c r="N152" s="16"/>
+      <c r="A152" s="140" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B152" s="214" t="s">
+        <v>1035</v>
+      </c>
+      <c r="C152" s="156" t="s">
+        <v>514</v>
+      </c>
+      <c r="D152" s="226"/>
+      <c r="E152" s="140" t="s">
+        <v>367</v>
+      </c>
+      <c r="F152" s="38" t="s">
+        <v>1036</v>
+      </c>
+      <c r="G152" s="38" t="s">
+        <v>1037</v>
+      </c>
+      <c r="H152" s="44"/>
+      <c r="I152" s="40"/>
+      <c r="J152" s="40"/>
+      <c r="K152" s="227" t="s">
+        <v>1038</v>
+      </c>
+      <c r="L152" s="5" t="s">
+        <v>1039</v>
+      </c>
+      <c r="M152" s="5"/>
+      <c r="N152" s="40"/>
     </row>
     <row r="153">
       <c r="A153" s="140" t="s">
-        <v>1033</v>
+        <v>1040</v>
       </c>
       <c r="B153" s="214" t="s">
-        <v>1034</v>
+        <v>1041</v>
       </c>
       <c r="C153" s="156" t="s">
         <v>509</v>
       </c>
-      <c r="D153" s="45"/>
+      <c r="D153" s="226"/>
       <c r="E153" s="140" t="s">
         <v>377</v>
       </c>
       <c r="F153" s="38" t="s">
-        <v>1035</v>
+        <v>1042</v>
       </c>
       <c r="G153" s="151" t="s">
-        <v>1036</v>
-      </c>
-      <c r="H153" s="42"/>
+        <v>1032</v>
+      </c>
+      <c r="H153" s="44"/>
       <c r="I153" s="40"/>
       <c r="J153" s="40"/>
       <c r="K153" s="137" t="s">
         <v>615</v>
       </c>
-      <c r="L153" s="155" t="s">
-        <v>1037</v>
-      </c>
-      <c r="M153" s="155"/>
+      <c r="L153" s="228" t="s">
+        <v>1043</v>
+      </c>
+      <c r="M153" s="228"/>
       <c r="N153" s="40"/>
     </row>
     <row r="154">
       <c r="A154" s="140" t="s">
-        <v>1038</v>
+        <v>1044</v>
       </c>
       <c r="B154" s="214" t="s">
-        <v>1039</v>
+        <v>1045</v>
       </c>
       <c r="C154" s="156" t="s">
         <v>514</v>
@@ -16194,29 +16182,29 @@
         <v>367</v>
       </c>
       <c r="F154" s="38" t="s">
-        <v>1040</v>
-      </c>
-      <c r="G154" s="38" t="s">
-        <v>1041</v>
-      </c>
-      <c r="H154" s="44"/>
+        <v>1046</v>
+      </c>
+      <c r="G154" s="151" t="s">
+        <v>1047</v>
+      </c>
+      <c r="H154" s="42"/>
       <c r="I154" s="40"/>
       <c r="J154" s="40"/>
       <c r="K154" s="227" t="s">
-        <v>1042</v>
+        <v>1048</v>
       </c>
       <c r="L154" s="5" t="s">
-        <v>1043</v>
+        <v>1049</v>
       </c>
       <c r="M154" s="5"/>
       <c r="N154" s="40"/>
     </row>
     <row r="155">
       <c r="A155" s="140" t="s">
-        <v>1044</v>
+        <v>1050</v>
       </c>
       <c r="B155" s="214" t="s">
-        <v>1045</v>
+        <v>1051</v>
       </c>
       <c r="C155" s="156" t="s">
         <v>509</v>
@@ -16226,29 +16214,29 @@
         <v>377</v>
       </c>
       <c r="F155" s="38" t="s">
-        <v>1046</v>
+        <v>1052</v>
       </c>
       <c r="G155" s="151" t="s">
-        <v>1036</v>
-      </c>
-      <c r="H155" s="44"/>
+        <v>1032</v>
+      </c>
+      <c r="H155" s="42"/>
       <c r="I155" s="40"/>
       <c r="J155" s="40"/>
       <c r="K155" s="137" t="s">
         <v>615</v>
       </c>
-      <c r="L155" s="228" t="s">
-        <v>1047</v>
-      </c>
-      <c r="M155" s="228"/>
+      <c r="L155" s="155" t="s">
+        <v>1053</v>
+      </c>
+      <c r="M155" s="155"/>
       <c r="N155" s="40"/>
     </row>
     <row r="156">
       <c r="A156" s="140" t="s">
-        <v>1048</v>
+        <v>1054</v>
       </c>
       <c r="B156" s="214" t="s">
-        <v>1049</v>
+        <v>1055</v>
       </c>
       <c r="C156" s="156" t="s">
         <v>514</v>
@@ -16258,29 +16246,29 @@
         <v>367</v>
       </c>
       <c r="F156" s="38" t="s">
-        <v>1050</v>
+        <v>1056</v>
       </c>
       <c r="G156" s="151" t="s">
-        <v>1051</v>
+        <v>1057</v>
       </c>
       <c r="H156" s="42"/>
       <c r="I156" s="40"/>
       <c r="J156" s="40"/>
       <c r="K156" s="227" t="s">
-        <v>1052</v>
+        <v>1038</v>
       </c>
       <c r="L156" s="5" t="s">
-        <v>1053</v>
+        <v>1058</v>
       </c>
       <c r="M156" s="5"/>
       <c r="N156" s="40"/>
     </row>
     <row r="157">
       <c r="A157" s="140" t="s">
-        <v>1054</v>
+        <v>1059</v>
       </c>
       <c r="B157" s="214" t="s">
-        <v>1055</v>
+        <v>1060</v>
       </c>
       <c r="C157" s="156" t="s">
         <v>509</v>
@@ -16290,10 +16278,10 @@
         <v>377</v>
       </c>
       <c r="F157" s="38" t="s">
-        <v>1056</v>
+        <v>1061</v>
       </c>
       <c r="G157" s="151" t="s">
-        <v>1036</v>
+        <v>1032</v>
       </c>
       <c r="H157" s="42"/>
       <c r="I157" s="40"/>
@@ -16301,82 +16289,82 @@
       <c r="K157" s="137" t="s">
         <v>615</v>
       </c>
-      <c r="L157" s="155" t="s">
-        <v>1057</v>
-      </c>
-      <c r="M157" s="155"/>
+      <c r="L157" s="229" t="s">
+        <v>1062</v>
+      </c>
+      <c r="M157" s="229"/>
       <c r="N157" s="40"/>
     </row>
     <row r="158">
-      <c r="A158" s="140" t="s">
-        <v>1058</v>
-      </c>
-      <c r="B158" s="214" t="s">
-        <v>1059</v>
-      </c>
-      <c r="C158" s="156" t="s">
+      <c r="A158" s="20" t="s">
+        <v>1063</v>
+      </c>
+      <c r="B158" s="122" t="s">
+        <v>1064</v>
+      </c>
+      <c r="C158" s="157" t="s">
         <v>514</v>
       </c>
-      <c r="D158" s="226"/>
-      <c r="E158" s="140" t="s">
+      <c r="D158" s="230"/>
+      <c r="E158" s="231" t="s">
         <v>367</v>
       </c>
-      <c r="F158" s="38" t="s">
-        <v>1060</v>
-      </c>
-      <c r="G158" s="151" t="s">
-        <v>1061</v>
-      </c>
-      <c r="H158" s="42"/>
-      <c r="I158" s="40"/>
-      <c r="J158" s="40"/>
+      <c r="F158" s="14" t="s">
+        <v>1065</v>
+      </c>
+      <c r="G158" s="5" t="s">
+        <v>1066</v>
+      </c>
+      <c r="H158" s="13"/>
+      <c r="I158" s="16"/>
+      <c r="J158" s="16"/>
       <c r="K158" s="227" t="s">
-        <v>1042</v>
+        <v>1038</v>
       </c>
       <c r="L158" s="5" t="s">
-        <v>1062</v>
+        <v>1067</v>
       </c>
       <c r="M158" s="5"/>
-      <c r="N158" s="40"/>
+      <c r="N158" s="16"/>
     </row>
     <row r="159">
-      <c r="A159" s="140" t="s">
-        <v>1063</v>
-      </c>
-      <c r="B159" s="214" t="s">
-        <v>1064</v>
-      </c>
-      <c r="C159" s="156" t="s">
+      <c r="A159" s="20" t="s">
+        <v>1068</v>
+      </c>
+      <c r="B159" s="122" t="s">
+        <v>1069</v>
+      </c>
+      <c r="C159" s="157" t="s">
         <v>509</v>
       </c>
-      <c r="D159" s="226"/>
-      <c r="E159" s="140" t="s">
+      <c r="D159" s="230"/>
+      <c r="E159" s="20" t="s">
         <v>377</v>
       </c>
-      <c r="F159" s="38" t="s">
-        <v>1065</v>
-      </c>
-      <c r="G159" s="151" t="s">
-        <v>1036</v>
-      </c>
-      <c r="H159" s="42"/>
-      <c r="I159" s="40"/>
-      <c r="J159" s="40"/>
-      <c r="K159" s="137" t="s">
+      <c r="F159" s="14" t="s">
+        <v>1070</v>
+      </c>
+      <c r="G159" s="232" t="s">
+        <v>1032</v>
+      </c>
+      <c r="H159" s="13"/>
+      <c r="I159" s="16"/>
+      <c r="J159" s="16"/>
+      <c r="K159" s="128" t="s">
         <v>615</v>
       </c>
-      <c r="L159" s="229" t="s">
-        <v>1066</v>
-      </c>
-      <c r="M159" s="229"/>
-      <c r="N159" s="40"/>
+      <c r="L159" s="158" t="s">
+        <v>1071</v>
+      </c>
+      <c r="M159" s="158"/>
+      <c r="N159" s="16"/>
     </row>
     <row r="160">
       <c r="A160" s="20" t="s">
-        <v>1067</v>
+        <v>1072</v>
       </c>
       <c r="B160" s="122" t="s">
-        <v>1068</v>
+        <v>1073</v>
       </c>
       <c r="C160" s="157" t="s">
         <v>514</v>
@@ -16386,29 +16374,29 @@
         <v>367</v>
       </c>
       <c r="F160" s="14" t="s">
-        <v>1069</v>
+        <v>1074</v>
       </c>
       <c r="G160" s="5" t="s">
-        <v>1070</v>
+        <v>1075</v>
       </c>
       <c r="H160" s="13"/>
       <c r="I160" s="16"/>
       <c r="J160" s="16"/>
       <c r="K160" s="227" t="s">
-        <v>1042</v>
+        <v>1038</v>
       </c>
       <c r="L160" s="5" t="s">
-        <v>1071</v>
+        <v>1076</v>
       </c>
       <c r="M160" s="5"/>
       <c r="N160" s="16"/>
     </row>
     <row r="161">
       <c r="A161" s="20" t="s">
-        <v>1072</v>
+        <v>1077</v>
       </c>
       <c r="B161" s="122" t="s">
-        <v>1073</v>
+        <v>1078</v>
       </c>
       <c r="C161" s="157" t="s">
         <v>509</v>
@@ -16418,10 +16406,10 @@
         <v>377</v>
       </c>
       <c r="F161" s="14" t="s">
-        <v>1074</v>
+        <v>1079</v>
       </c>
       <c r="G161" s="232" t="s">
-        <v>1036</v>
+        <v>1032</v>
       </c>
       <c r="H161" s="13"/>
       <c r="I161" s="16"/>
@@ -16430,17 +16418,17 @@
         <v>615</v>
       </c>
       <c r="L161" s="158" t="s">
-        <v>1075</v>
+        <v>1080</v>
       </c>
       <c r="M161" s="158"/>
       <c r="N161" s="16"/>
     </row>
     <row r="162">
       <c r="A162" s="20" t="s">
-        <v>1076</v>
+        <v>1081</v>
       </c>
       <c r="B162" s="122" t="s">
-        <v>1077</v>
+        <v>1082</v>
       </c>
       <c r="C162" s="157" t="s">
         <v>514</v>
@@ -16450,29 +16438,29 @@
         <v>367</v>
       </c>
       <c r="F162" s="14" t="s">
-        <v>1078</v>
-      </c>
-      <c r="G162" s="5" t="s">
-        <v>1079</v>
+        <v>1083</v>
+      </c>
+      <c r="G162" s="134" t="s">
+        <v>1084</v>
       </c>
       <c r="H162" s="13"/>
       <c r="I162" s="16"/>
       <c r="J162" s="16"/>
       <c r="K162" s="227" t="s">
-        <v>1042</v>
+        <v>1038</v>
       </c>
       <c r="L162" s="5" t="s">
-        <v>1080</v>
-      </c>
-      <c r="M162" s="5"/>
-      <c r="N162" s="16"/>
+        <v>1085</v>
+      </c>
+      <c r="M162" s="15"/>
+      <c r="N162" s="15"/>
     </row>
     <row r="163">
       <c r="A163" s="20" t="s">
-        <v>1081</v>
+        <v>1086</v>
       </c>
       <c r="B163" s="122" t="s">
-        <v>1082</v>
+        <v>1087</v>
       </c>
       <c r="C163" s="157" t="s">
         <v>509</v>
@@ -16482,10 +16470,10 @@
         <v>377</v>
       </c>
       <c r="F163" s="14" t="s">
-        <v>1083</v>
+        <v>1088</v>
       </c>
       <c r="G163" s="232" t="s">
-        <v>1036</v>
+        <v>1032</v>
       </c>
       <c r="H163" s="13"/>
       <c r="I163" s="16"/>
@@ -16494,17 +16482,17 @@
         <v>615</v>
       </c>
       <c r="L163" s="158" t="s">
-        <v>1084</v>
-      </c>
-      <c r="M163" s="158"/>
-      <c r="N163" s="16"/>
+        <v>1089</v>
+      </c>
+      <c r="M163" s="15"/>
+      <c r="N163" s="15"/>
     </row>
     <row r="164">
       <c r="A164" s="20" t="s">
-        <v>1085</v>
+        <v>1090</v>
       </c>
       <c r="B164" s="122" t="s">
-        <v>1086</v>
+        <v>1091</v>
       </c>
       <c r="C164" s="157" t="s">
         <v>514</v>
@@ -16514,29 +16502,29 @@
         <v>367</v>
       </c>
       <c r="F164" s="14" t="s">
-        <v>1087</v>
+        <v>1092</v>
       </c>
       <c r="G164" s="134" t="s">
-        <v>1088</v>
+        <v>1093</v>
       </c>
       <c r="H164" s="13"/>
       <c r="I164" s="16"/>
       <c r="J164" s="16"/>
       <c r="K164" s="227" t="s">
-        <v>1042</v>
+        <v>1038</v>
       </c>
       <c r="L164" s="5" t="s">
-        <v>1089</v>
+        <v>1094</v>
       </c>
       <c r="M164" s="15"/>
       <c r="N164" s="15"/>
     </row>
     <row r="165">
       <c r="A165" s="20" t="s">
-        <v>1090</v>
+        <v>1095</v>
       </c>
       <c r="B165" s="122" t="s">
-        <v>1091</v>
+        <v>1096</v>
       </c>
       <c r="C165" s="157" t="s">
         <v>509</v>
@@ -16546,10 +16534,10 @@
         <v>377</v>
       </c>
       <c r="F165" s="14" t="s">
-        <v>1092</v>
+        <v>1097</v>
       </c>
       <c r="G165" s="232" t="s">
-        <v>1036</v>
+        <v>1032</v>
       </c>
       <c r="H165" s="13"/>
       <c r="I165" s="16"/>
@@ -16558,17 +16546,17 @@
         <v>615</v>
       </c>
       <c r="L165" s="158" t="s">
-        <v>1093</v>
+        <v>1098</v>
       </c>
       <c r="M165" s="15"/>
       <c r="N165" s="15"/>
     </row>
     <row r="166">
       <c r="A166" s="20" t="s">
-        <v>1094</v>
+        <v>1099</v>
       </c>
       <c r="B166" s="122" t="s">
-        <v>1095</v>
+        <v>1100</v>
       </c>
       <c r="C166" s="157" t="s">
         <v>514</v>
@@ -16578,29 +16566,29 @@
         <v>367</v>
       </c>
       <c r="F166" s="14" t="s">
-        <v>1096</v>
+        <v>1101</v>
       </c>
       <c r="G166" s="134" t="s">
-        <v>1097</v>
+        <v>1102</v>
       </c>
       <c r="H166" s="13"/>
       <c r="I166" s="16"/>
       <c r="J166" s="16"/>
       <c r="K166" s="227" t="s">
-        <v>1042</v>
+        <v>1038</v>
       </c>
       <c r="L166" s="5" t="s">
-        <v>1098</v>
+        <v>1103</v>
       </c>
       <c r="M166" s="15"/>
       <c r="N166" s="15"/>
     </row>
     <row r="167">
       <c r="A167" s="20" t="s">
-        <v>1099</v>
+        <v>1104</v>
       </c>
       <c r="B167" s="122" t="s">
-        <v>1100</v>
+        <v>1105</v>
       </c>
       <c r="C167" s="157" t="s">
         <v>509</v>
@@ -16610,10 +16598,10 @@
         <v>377</v>
       </c>
       <c r="F167" s="14" t="s">
-        <v>1101</v>
+        <v>1106</v>
       </c>
       <c r="G167" s="232" t="s">
-        <v>1036</v>
+        <v>1032</v>
       </c>
       <c r="H167" s="13"/>
       <c r="I167" s="16"/>
@@ -16622,17 +16610,17 @@
         <v>615</v>
       </c>
       <c r="L167" s="158" t="s">
-        <v>1102</v>
+        <v>1107</v>
       </c>
       <c r="M167" s="15"/>
-      <c r="N167" s="15"/>
+      <c r="N167" s="19"/>
     </row>
     <row r="168">
       <c r="A168" s="20" t="s">
-        <v>1103</v>
+        <v>1108</v>
       </c>
       <c r="B168" s="122" t="s">
-        <v>1104</v>
+        <v>1109</v>
       </c>
       <c r="C168" s="157" t="s">
         <v>514</v>
@@ -16642,86 +16630,82 @@
         <v>367</v>
       </c>
       <c r="F168" s="14" t="s">
-        <v>1105</v>
+        <v>1110</v>
       </c>
       <c r="G168" s="134" t="s">
-        <v>1106</v>
+        <v>1111</v>
       </c>
       <c r="H168" s="13"/>
       <c r="I168" s="16"/>
       <c r="J168" s="16"/>
       <c r="K168" s="227" t="s">
-        <v>1042</v>
+        <v>1038</v>
       </c>
       <c r="L168" s="5" t="s">
-        <v>1107</v>
+        <v>1112</v>
       </c>
       <c r="M168" s="15"/>
-      <c r="N168" s="15"/>
+      <c r="N168" s="19"/>
     </row>
     <row r="169">
       <c r="A169" s="20" t="s">
-        <v>1108</v>
+        <v>1113</v>
       </c>
       <c r="B169" s="122" t="s">
-        <v>1109</v>
+        <v>1114</v>
       </c>
       <c r="C169" s="157" t="s">
         <v>509</v>
       </c>
       <c r="D169" s="230"/>
-      <c r="E169" s="20" t="s">
-        <v>377</v>
-      </c>
-      <c r="F169" s="14" t="s">
-        <v>1110</v>
-      </c>
-      <c r="G169" s="232" t="s">
-        <v>1036</v>
-      </c>
+      <c r="E169" s="21" t="s">
+        <v>374</v>
+      </c>
+      <c r="F169" s="232" t="s">
+        <v>1032</v>
+      </c>
+      <c r="G169" s="5"/>
       <c r="H169" s="13"/>
       <c r="I169" s="16"/>
       <c r="J169" s="16"/>
-      <c r="K169" s="128" t="s">
-        <v>615</v>
+      <c r="K169" s="128">
+        <v>0.0</v>
       </c>
       <c r="L169" s="158" t="s">
-        <v>1111</v>
-      </c>
-      <c r="M169" s="15"/>
-      <c r="N169" s="19"/>
+        <v>277</v>
+      </c>
+      <c r="M169" s="158"/>
+      <c r="N169" s="16"/>
     </row>
     <row r="170">
       <c r="A170" s="20" t="s">
-        <v>1112</v>
+        <v>1115</v>
       </c>
       <c r="B170" s="122" t="s">
-        <v>1113</v>
+        <v>1116</v>
       </c>
       <c r="C170" s="157" t="s">
-        <v>514</v>
+        <v>509</v>
       </c>
       <c r="D170" s="230"/>
-      <c r="E170" s="231" t="s">
-        <v>367</v>
-      </c>
-      <c r="F170" s="14" t="s">
-        <v>1114</v>
-      </c>
-      <c r="G170" s="134" t="s">
-        <v>1115</v>
-      </c>
+      <c r="E170" s="21" t="s">
+        <v>374</v>
+      </c>
+      <c r="F170" s="232" t="s">
+        <v>1032</v>
+      </c>
+      <c r="G170" s="14"/>
       <c r="H170" s="13"/>
       <c r="I170" s="16"/>
       <c r="J170" s="16"/>
-      <c r="K170" s="227" t="s">
-        <v>1042</v>
-      </c>
-      <c r="L170" s="5" t="s">
-        <v>1116</v>
-      </c>
-      <c r="M170" s="15"/>
-      <c r="N170" s="19"/>
+      <c r="K170" s="128" t="s">
+        <v>744</v>
+      </c>
+      <c r="L170" s="158" t="s">
+        <v>754</v>
+      </c>
+      <c r="M170" s="158"/>
+      <c r="N170" s="16"/>
     </row>
     <row r="171">
       <c r="A171" s="20" t="s">
@@ -16731,60 +16715,60 @@
         <v>1118</v>
       </c>
       <c r="C171" s="157" t="s">
-        <v>509</v>
-      </c>
-      <c r="D171" s="230"/>
+        <v>514</v>
+      </c>
+      <c r="D171" s="31"/>
       <c r="E171" s="21" t="s">
         <v>374</v>
       </c>
       <c r="F171" s="232" t="s">
-        <v>1036</v>
-      </c>
-      <c r="G171" s="5"/>
-      <c r="H171" s="13"/>
+        <v>1032</v>
+      </c>
+      <c r="G171" s="14"/>
+      <c r="H171" s="31"/>
       <c r="I171" s="16"/>
       <c r="J171" s="16"/>
-      <c r="K171" s="128">
-        <v>0.0</v>
+      <c r="K171" s="128" t="s">
+        <v>749</v>
       </c>
       <c r="L171" s="158" t="s">
-        <v>277</v>
+        <v>758</v>
       </c>
       <c r="M171" s="158"/>
       <c r="N171" s="16"/>
     </row>
     <row r="172">
-      <c r="A172" s="20" t="s">
+      <c r="A172" s="18" t="s">
         <v>1119</v>
       </c>
       <c r="B172" s="122" t="s">
         <v>1120</v>
       </c>
       <c r="C172" s="157" t="s">
-        <v>509</v>
-      </c>
-      <c r="D172" s="230"/>
+        <v>514</v>
+      </c>
+      <c r="D172" s="31"/>
       <c r="E172" s="21" t="s">
         <v>374</v>
       </c>
       <c r="F172" s="232" t="s">
-        <v>1036</v>
+        <v>1032</v>
       </c>
       <c r="G172" s="14"/>
-      <c r="H172" s="13"/>
+      <c r="H172" s="31"/>
       <c r="I172" s="16"/>
       <c r="J172" s="16"/>
       <c r="K172" s="128" t="s">
         <v>744</v>
       </c>
       <c r="L172" s="158" t="s">
-        <v>754</v>
+        <v>745</v>
       </c>
       <c r="M172" s="158"/>
       <c r="N172" s="16"/>
     </row>
     <row r="173">
-      <c r="A173" s="20" t="s">
+      <c r="A173" s="18" t="s">
         <v>1121</v>
       </c>
       <c r="B173" s="122" t="s">
@@ -16798,7 +16782,7 @@
         <v>374</v>
       </c>
       <c r="F173" s="232" t="s">
-        <v>1036</v>
+        <v>1032</v>
       </c>
       <c r="G173" s="14"/>
       <c r="H173" s="31"/>
@@ -16808,141 +16792,145 @@
         <v>749</v>
       </c>
       <c r="L173" s="158" t="s">
-        <v>758</v>
+        <v>750</v>
       </c>
       <c r="M173" s="158"/>
       <c r="N173" s="16"/>
     </row>
     <row r="174">
-      <c r="A174" s="18" t="s">
+      <c r="A174" s="20" t="s">
         <v>1123</v>
       </c>
-      <c r="B174" s="122" t="s">
+      <c r="B174" s="125" t="s">
         <v>1124</v>
       </c>
       <c r="C174" s="157" t="s">
-        <v>514</v>
+        <v>509</v>
       </c>
       <c r="D174" s="31"/>
       <c r="E174" s="21" t="s">
         <v>374</v>
       </c>
-      <c r="F174" s="232" t="s">
-        <v>1036</v>
-      </c>
-      <c r="G174" s="14"/>
-      <c r="H174" s="31"/>
+      <c r="F174" s="14" t="s">
+        <v>1125</v>
+      </c>
+      <c r="G174" s="14" t="s">
+        <v>1126</v>
+      </c>
+      <c r="H174" s="13"/>
       <c r="I174" s="16"/>
       <c r="J174" s="16"/>
-      <c r="K174" s="128" t="s">
-        <v>744</v>
-      </c>
-      <c r="L174" s="158" t="s">
-        <v>745</v>
-      </c>
-      <c r="M174" s="158"/>
+      <c r="K174" s="233">
+        <v>12.0</v>
+      </c>
+      <c r="L174" s="233" t="s">
+        <v>42</v>
+      </c>
+      <c r="M174" s="128"/>
       <c r="N174" s="16"/>
     </row>
     <row r="175">
-      <c r="A175" s="18" t="s">
-        <v>1125</v>
-      </c>
-      <c r="B175" s="122" t="s">
-        <v>1126</v>
+      <c r="A175" s="20" t="s">
+        <v>1127</v>
+      </c>
+      <c r="B175" s="125" t="s">
+        <v>1128</v>
       </c>
       <c r="C175" s="157" t="s">
         <v>514</v>
       </c>
       <c r="D175" s="31"/>
-      <c r="E175" s="21" t="s">
-        <v>374</v>
-      </c>
-      <c r="F175" s="232" t="s">
-        <v>1036</v>
-      </c>
-      <c r="G175" s="14"/>
-      <c r="H175" s="31"/>
+      <c r="E175" s="20" t="s">
+        <v>367</v>
+      </c>
+      <c r="F175" s="14" t="s">
+        <v>1129</v>
+      </c>
+      <c r="G175" s="14" t="s">
+        <v>1130</v>
+      </c>
+      <c r="H175" s="13"/>
       <c r="I175" s="16"/>
       <c r="J175" s="16"/>
-      <c r="K175" s="128" t="s">
-        <v>749</v>
-      </c>
-      <c r="L175" s="158" t="s">
-        <v>750</v>
-      </c>
-      <c r="M175" s="158"/>
+      <c r="K175" s="234" t="s">
+        <v>1131</v>
+      </c>
+      <c r="L175" s="233" t="s">
+        <v>1132</v>
+      </c>
+      <c r="M175" s="128"/>
       <c r="N175" s="16"/>
     </row>
     <row r="176">
       <c r="A176" s="20" t="s">
-        <v>1127</v>
+        <v>1133</v>
       </c>
       <c r="B176" s="125" t="s">
-        <v>1128</v>
+        <v>1134</v>
       </c>
       <c r="C176" s="157" t="s">
-        <v>509</v>
+        <v>514</v>
       </c>
       <c r="D176" s="31"/>
-      <c r="E176" s="21" t="s">
-        <v>374</v>
+      <c r="E176" s="20" t="s">
+        <v>367</v>
       </c>
       <c r="F176" s="14" t="s">
         <v>1129</v>
       </c>
       <c r="G176" s="14" t="s">
-        <v>1130</v>
+        <v>1135</v>
       </c>
       <c r="H176" s="13"/>
       <c r="I176" s="16"/>
       <c r="J176" s="16"/>
-      <c r="K176" s="233">
-        <v>12.0</v>
+      <c r="K176" s="234" t="s">
+        <v>46</v>
       </c>
       <c r="L176" s="233" t="s">
-        <v>42</v>
+        <v>1132</v>
       </c>
       <c r="M176" s="128"/>
       <c r="N176" s="16"/>
     </row>
     <row r="177">
       <c r="A177" s="20" t="s">
-        <v>1131</v>
+        <v>1136</v>
       </c>
       <c r="B177" s="125" t="s">
-        <v>1132</v>
+        <v>1137</v>
       </c>
       <c r="C177" s="157" t="s">
-        <v>514</v>
+        <v>509</v>
       </c>
       <c r="D177" s="31"/>
-      <c r="E177" s="20" t="s">
-        <v>367</v>
+      <c r="E177" s="21" t="s">
+        <v>374</v>
       </c>
       <c r="F177" s="14" t="s">
-        <v>1133</v>
+        <v>1138</v>
       </c>
       <c r="G177" s="14" t="s">
-        <v>1134</v>
+        <v>1139</v>
       </c>
       <c r="H177" s="13"/>
       <c r="I177" s="16"/>
       <c r="J177" s="16"/>
-      <c r="K177" s="234" t="s">
-        <v>1135</v>
+      <c r="K177" s="233">
+        <v>2.0</v>
       </c>
       <c r="L177" s="233" t="s">
-        <v>1136</v>
+        <v>42</v>
       </c>
       <c r="M177" s="128"/>
       <c r="N177" s="16"/>
     </row>
     <row r="178">
       <c r="A178" s="20" t="s">
-        <v>1137</v>
+        <v>1140</v>
       </c>
       <c r="B178" s="125" t="s">
-        <v>1138</v>
+        <v>1141</v>
       </c>
       <c r="C178" s="157" t="s">
         <v>514</v>
@@ -16952,86 +16940,22 @@
         <v>367</v>
       </c>
       <c r="F178" s="14" t="s">
-        <v>1133</v>
+        <v>1142</v>
       </c>
       <c r="G178" s="14" t="s">
-        <v>1139</v>
+        <v>1143</v>
       </c>
       <c r="H178" s="13"/>
       <c r="I178" s="16"/>
       <c r="J178" s="16"/>
-      <c r="K178" s="234" t="s">
-        <v>46</v>
-      </c>
-      <c r="L178" s="233" t="s">
-        <v>1136</v>
+      <c r="K178" s="235" t="s">
+        <v>1144</v>
+      </c>
+      <c r="L178" s="236" t="s">
+        <v>1145</v>
       </c>
       <c r="M178" s="128"/>
       <c r="N178" s="16"/>
-    </row>
-    <row r="179">
-      <c r="A179" s="20" t="s">
-        <v>1140</v>
-      </c>
-      <c r="B179" s="125" t="s">
-        <v>1141</v>
-      </c>
-      <c r="C179" s="157" t="s">
-        <v>509</v>
-      </c>
-      <c r="D179" s="31"/>
-      <c r="E179" s="21" t="s">
-        <v>374</v>
-      </c>
-      <c r="F179" s="14" t="s">
-        <v>1142</v>
-      </c>
-      <c r="G179" s="14" t="s">
-        <v>1143</v>
-      </c>
-      <c r="H179" s="13"/>
-      <c r="I179" s="16"/>
-      <c r="J179" s="16"/>
-      <c r="K179" s="233">
-        <v>2.0</v>
-      </c>
-      <c r="L179" s="233" t="s">
-        <v>42</v>
-      </c>
-      <c r="M179" s="128"/>
-      <c r="N179" s="16"/>
-    </row>
-    <row r="180">
-      <c r="A180" s="20" t="s">
-        <v>1144</v>
-      </c>
-      <c r="B180" s="125" t="s">
-        <v>1145</v>
-      </c>
-      <c r="C180" s="157" t="s">
-        <v>514</v>
-      </c>
-      <c r="D180" s="31"/>
-      <c r="E180" s="20" t="s">
-        <v>367</v>
-      </c>
-      <c r="F180" s="14" t="s">
-        <v>1146</v>
-      </c>
-      <c r="G180" s="14" t="s">
-        <v>1147</v>
-      </c>
-      <c r="H180" s="13"/>
-      <c r="I180" s="16"/>
-      <c r="J180" s="16"/>
-      <c r="K180" s="235" t="s">
-        <v>1148</v>
-      </c>
-      <c r="L180" s="236" t="s">
-        <v>1149</v>
-      </c>
-      <c r="M180" s="128"/>
-      <c r="N180" s="16"/>
     </row>
   </sheetData>
   <printOptions gridLines="1" horizontalCentered="1"/>
@@ -17068,24 +16992,24 @@
         <v>2</v>
       </c>
       <c r="D1" s="239" t="s">
-        <v>1150</v>
+        <v>1146</v>
       </c>
       <c r="E1" s="237" t="s">
         <v>16</v>
       </c>
       <c r="F1" s="240" t="s">
-        <v>1151</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="241" t="s">
-        <v>1152</v>
+        <v>1148</v>
       </c>
       <c r="B2" s="242" t="s">
-        <v>1153</v>
+        <v>1149</v>
       </c>
       <c r="C2" s="243" t="s">
-        <v>1154</v>
+        <v>1150</v>
       </c>
       <c r="D2" s="243"/>
       <c r="E2" s="244"/>
@@ -17093,29 +17017,29 @@
     </row>
     <row r="3">
       <c r="A3" s="241" t="s">
-        <v>1155</v>
+        <v>1151</v>
       </c>
       <c r="B3" s="242" t="s">
-        <v>1156</v>
+        <v>1152</v>
       </c>
       <c r="C3" s="242" t="s">
-        <v>1157</v>
+        <v>1153</v>
       </c>
       <c r="D3" s="242"/>
       <c r="E3" s="246"/>
       <c r="F3" s="240" t="s">
-        <v>1158</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="241" t="s">
-        <v>1159</v>
+        <v>1155</v>
       </c>
       <c r="B4" s="242" t="s">
-        <v>1160</v>
+        <v>1156</v>
       </c>
       <c r="C4" s="242" t="s">
-        <v>1161</v>
+        <v>1157</v>
       </c>
       <c r="D4" s="242"/>
       <c r="E4" s="247"/>
@@ -17123,13 +17047,13 @@
     </row>
     <row r="5">
       <c r="A5" s="241" t="s">
-        <v>1162</v>
+        <v>1158</v>
       </c>
       <c r="B5" s="242" t="s">
-        <v>1163</v>
+        <v>1159</v>
       </c>
       <c r="C5" s="242" t="s">
-        <v>1164</v>
+        <v>1160</v>
       </c>
       <c r="D5" s="242"/>
       <c r="E5" s="247"/>
@@ -17137,13 +17061,13 @@
     </row>
     <row r="6">
       <c r="A6" s="241" t="s">
-        <v>1165</v>
+        <v>1161</v>
       </c>
       <c r="B6" s="248" t="s">
-        <v>1166</v>
+        <v>1162</v>
       </c>
       <c r="C6" s="242" t="s">
-        <v>1167</v>
+        <v>1163</v>
       </c>
       <c r="D6" s="242"/>
       <c r="E6" s="246"/>
@@ -17151,13 +17075,13 @@
     </row>
     <row r="7">
       <c r="A7" s="241" t="s">
-        <v>1168</v>
+        <v>1164</v>
       </c>
       <c r="B7" s="249" t="s">
-        <v>1169</v>
+        <v>1165</v>
       </c>
       <c r="C7" s="242" t="s">
-        <v>1170</v>
+        <v>1166</v>
       </c>
       <c r="D7" s="242"/>
       <c r="E7" s="240"/>
@@ -17165,13 +17089,13 @@
     </row>
     <row r="8">
       <c r="A8" s="241" t="s">
-        <v>1171</v>
+        <v>1167</v>
       </c>
       <c r="B8" s="249" t="s">
-        <v>1172</v>
+        <v>1168</v>
       </c>
       <c r="C8" s="242" t="s">
-        <v>1154</v>
+        <v>1150</v>
       </c>
       <c r="D8" s="242"/>
       <c r="E8" s="240"/>
@@ -17179,13 +17103,13 @@
     </row>
     <row r="9">
       <c r="A9" s="241" t="s">
-        <v>1173</v>
+        <v>1169</v>
       </c>
       <c r="B9" s="249" t="s">
-        <v>1174</v>
+        <v>1170</v>
       </c>
       <c r="C9" s="250" t="s">
-        <v>1175</v>
+        <v>1171</v>
       </c>
       <c r="D9" s="250"/>
       <c r="E9" s="251"/>
@@ -17193,13 +17117,13 @@
     </row>
     <row r="10">
       <c r="A10" s="241" t="s">
-        <v>1176</v>
+        <v>1172</v>
       </c>
       <c r="B10" s="249" t="s">
-        <v>1177</v>
+        <v>1173</v>
       </c>
       <c r="C10" s="242" t="s">
-        <v>1178</v>
+        <v>1174</v>
       </c>
       <c r="D10" s="242"/>
       <c r="E10" s="240"/>
@@ -17207,13 +17131,13 @@
     </row>
     <row r="11">
       <c r="A11" s="241" t="s">
-        <v>1179</v>
+        <v>1175</v>
       </c>
       <c r="B11" s="242" t="s">
-        <v>1180</v>
+        <v>1176</v>
       </c>
       <c r="C11" s="242" t="s">
-        <v>1181</v>
+        <v>1177</v>
       </c>
       <c r="D11" s="242"/>
       <c r="E11" s="245"/>
@@ -17221,13 +17145,13 @@
     </row>
     <row r="12">
       <c r="A12" s="241" t="s">
-        <v>1182</v>
+        <v>1178</v>
       </c>
       <c r="B12" s="252" t="s">
-        <v>1183</v>
+        <v>1179</v>
       </c>
       <c r="C12" s="252" t="s">
-        <v>1184</v>
+        <v>1180</v>
       </c>
       <c r="D12" s="252"/>
       <c r="E12" s="245"/>
@@ -17235,13 +17159,13 @@
     </row>
     <row r="13">
       <c r="A13" s="241" t="s">
-        <v>1185</v>
+        <v>1181</v>
       </c>
       <c r="B13" s="253" t="s">
-        <v>1186</v>
+        <v>1182</v>
       </c>
       <c r="C13" s="252" t="s">
-        <v>1187</v>
+        <v>1183</v>
       </c>
       <c r="D13" s="252"/>
       <c r="E13" s="245"/>
@@ -17249,13 +17173,13 @@
     </row>
     <row r="14">
       <c r="A14" s="241" t="s">
-        <v>1188</v>
+        <v>1184</v>
       </c>
       <c r="B14" s="253" t="s">
-        <v>1189</v>
+        <v>1185</v>
       </c>
       <c r="C14" s="252" t="s">
-        <v>1190</v>
+        <v>1186</v>
       </c>
       <c r="D14" s="252"/>
       <c r="E14" s="245"/>
@@ -17263,13 +17187,13 @@
     </row>
     <row r="15">
       <c r="A15" s="241" t="s">
-        <v>1191</v>
+        <v>1187</v>
       </c>
       <c r="B15" s="253" t="s">
-        <v>1192</v>
+        <v>1188</v>
       </c>
       <c r="C15" s="252" t="s">
-        <v>1193</v>
+        <v>1189</v>
       </c>
       <c r="D15" s="252"/>
       <c r="E15" s="245"/>
@@ -17277,13 +17201,13 @@
     </row>
     <row r="16">
       <c r="A16" s="241" t="s">
-        <v>1194</v>
+        <v>1190</v>
       </c>
       <c r="B16" s="253" t="s">
-        <v>1195</v>
+        <v>1191</v>
       </c>
       <c r="C16" s="252" t="s">
-        <v>1196</v>
+        <v>1192</v>
       </c>
       <c r="D16" s="252"/>
       <c r="E16" s="245"/>
@@ -17291,13 +17215,13 @@
     </row>
     <row r="17">
       <c r="A17" s="241" t="s">
-        <v>1197</v>
+        <v>1193</v>
       </c>
       <c r="B17" s="253" t="s">
-        <v>1198</v>
+        <v>1194</v>
       </c>
       <c r="C17" s="252" t="s">
-        <v>1199</v>
+        <v>1195</v>
       </c>
       <c r="D17" s="252"/>
       <c r="E17" s="245"/>
@@ -17305,13 +17229,13 @@
     </row>
     <row r="18">
       <c r="A18" s="241" t="s">
-        <v>1200</v>
+        <v>1196</v>
       </c>
       <c r="B18" s="253" t="s">
-        <v>1201</v>
+        <v>1197</v>
       </c>
       <c r="C18" s="252" t="s">
-        <v>1202</v>
+        <v>1198</v>
       </c>
       <c r="D18" s="252"/>
       <c r="E18" s="245"/>
@@ -17319,13 +17243,13 @@
     </row>
     <row r="19">
       <c r="A19" s="241" t="s">
-        <v>1203</v>
+        <v>1199</v>
       </c>
       <c r="B19" s="253" t="s">
-        <v>1204</v>
+        <v>1200</v>
       </c>
       <c r="C19" s="252" t="s">
-        <v>1205</v>
+        <v>1201</v>
       </c>
       <c r="D19" s="252"/>
       <c r="E19" s="245"/>
@@ -17333,13 +17257,13 @@
     </row>
     <row r="20">
       <c r="A20" s="241" t="s">
-        <v>1206</v>
+        <v>1202</v>
       </c>
       <c r="B20" s="253" t="s">
-        <v>1207</v>
+        <v>1203</v>
       </c>
       <c r="C20" s="254" t="s">
-        <v>1175</v>
+        <v>1171</v>
       </c>
       <c r="D20" s="254"/>
       <c r="E20" s="245"/>
@@ -17347,13 +17271,13 @@
     </row>
     <row r="21">
       <c r="A21" s="241" t="s">
-        <v>1208</v>
+        <v>1204</v>
       </c>
       <c r="B21" s="255" t="s">
-        <v>1209</v>
+        <v>1205</v>
       </c>
       <c r="C21" s="252" t="s">
-        <v>1210</v>
+        <v>1206</v>
       </c>
       <c r="D21" s="252"/>
       <c r="E21" s="245"/>
@@ -17361,29 +17285,29 @@
     </row>
     <row r="22">
       <c r="A22" s="241" t="s">
-        <v>1211</v>
+        <v>1207</v>
       </c>
       <c r="B22" s="253" t="s">
-        <v>1212</v>
+        <v>1208</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>1213</v>
+        <v>1209</v>
       </c>
       <c r="D22" s="256" t="s">
-        <v>1214</v>
+        <v>1210</v>
       </c>
       <c r="E22" s="240"/>
       <c r="F22" s="245"/>
     </row>
     <row r="23">
       <c r="A23" s="241" t="s">
-        <v>1215</v>
+        <v>1211</v>
       </c>
       <c r="B23" s="257" t="s">
-        <v>1216</v>
+        <v>1212</v>
       </c>
       <c r="C23" s="258" t="s">
-        <v>1217</v>
+        <v>1213</v>
       </c>
       <c r="D23" s="258"/>
       <c r="E23" s="245"/>
@@ -17391,13 +17315,13 @@
     </row>
     <row r="24">
       <c r="A24" s="241" t="s">
-        <v>1218</v>
+        <v>1214</v>
       </c>
       <c r="B24" s="257" t="s">
-        <v>1219</v>
+        <v>1215</v>
       </c>
       <c r="C24" s="258" t="s">
-        <v>1220</v>
+        <v>1216</v>
       </c>
       <c r="D24" s="258"/>
       <c r="E24" s="245"/>
@@ -17405,13 +17329,13 @@
     </row>
     <row r="25">
       <c r="A25" s="241" t="s">
-        <v>1221</v>
+        <v>1217</v>
       </c>
       <c r="B25" s="257" t="s">
-        <v>1222</v>
+        <v>1218</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>1213</v>
+        <v>1209</v>
       </c>
       <c r="D25" s="258" t="s">
         <v>458</v>
@@ -17421,13 +17345,13 @@
     </row>
     <row r="26">
       <c r="A26" s="241" t="s">
-        <v>1223</v>
+        <v>1219</v>
       </c>
       <c r="B26" s="252" t="s">
-        <v>1224</v>
+        <v>1220</v>
       </c>
       <c r="C26" s="252" t="s">
-        <v>1225</v>
+        <v>1221</v>
       </c>
       <c r="D26" s="252"/>
       <c r="E26" s="240"/>
@@ -17435,13 +17359,13 @@
     </row>
     <row r="27">
       <c r="A27" s="241" t="s">
-        <v>1226</v>
+        <v>1222</v>
       </c>
       <c r="B27" s="252" t="s">
-        <v>1227</v>
+        <v>1223</v>
       </c>
       <c r="C27" s="252" t="s">
-        <v>1228</v>
+        <v>1224</v>
       </c>
       <c r="D27" s="252"/>
       <c r="E27" s="245"/>
@@ -17449,13 +17373,13 @@
     </row>
     <row r="28">
       <c r="A28" s="241" t="s">
-        <v>1229</v>
+        <v>1225</v>
       </c>
       <c r="B28" s="252" t="s">
-        <v>1230</v>
+        <v>1226</v>
       </c>
       <c r="C28" s="252" t="s">
-        <v>1231</v>
+        <v>1227</v>
       </c>
       <c r="D28" s="252"/>
       <c r="E28" s="245"/>
@@ -17463,143 +17387,143 @@
     </row>
     <row r="29">
       <c r="A29" s="241" t="s">
-        <v>1232</v>
+        <v>1228</v>
       </c>
       <c r="B29" s="259" t="s">
-        <v>1233</v>
+        <v>1229</v>
       </c>
       <c r="C29" s="249" t="s">
-        <v>1234</v>
+        <v>1230</v>
       </c>
       <c r="D29" s="249"/>
       <c r="E29" s="260"/>
     </row>
     <row r="30">
       <c r="A30" s="241" t="s">
-        <v>1235</v>
+        <v>1231</v>
       </c>
       <c r="B30" s="259" t="s">
-        <v>1236</v>
+        <v>1232</v>
       </c>
       <c r="C30" s="249" t="s">
-        <v>1237</v>
+        <v>1233</v>
       </c>
       <c r="D30" s="249"/>
       <c r="E30" s="260"/>
     </row>
     <row r="31">
       <c r="A31" s="241" t="s">
-        <v>1238</v>
+        <v>1234</v>
       </c>
       <c r="B31" s="259" t="s">
-        <v>1239</v>
+        <v>1235</v>
       </c>
       <c r="C31" s="249" t="s">
-        <v>1240</v>
+        <v>1236</v>
       </c>
       <c r="D31" s="249"/>
       <c r="E31" s="260"/>
     </row>
     <row r="32">
       <c r="A32" s="241" t="s">
-        <v>1241</v>
+        <v>1237</v>
       </c>
       <c r="B32" s="259" t="s">
-        <v>1242</v>
+        <v>1238</v>
       </c>
       <c r="C32" s="249" t="s">
-        <v>1243</v>
+        <v>1239</v>
       </c>
       <c r="D32" s="249"/>
       <c r="E32" s="260"/>
     </row>
     <row r="33">
       <c r="A33" s="241" t="s">
-        <v>1244</v>
+        <v>1240</v>
       </c>
       <c r="B33" s="259" t="s">
-        <v>1245</v>
+        <v>1241</v>
       </c>
       <c r="C33" s="249" t="s">
-        <v>1246</v>
+        <v>1242</v>
       </c>
       <c r="D33" s="249"/>
       <c r="E33" s="260"/>
     </row>
     <row r="34">
       <c r="A34" s="241" t="s">
-        <v>1247</v>
+        <v>1243</v>
       </c>
       <c r="B34" s="259" t="s">
-        <v>1248</v>
+        <v>1244</v>
       </c>
       <c r="C34" s="249" t="s">
-        <v>1249</v>
+        <v>1245</v>
       </c>
       <c r="D34" s="249"/>
       <c r="E34" s="260"/>
     </row>
     <row r="35">
       <c r="A35" s="241" t="s">
-        <v>1250</v>
+        <v>1246</v>
       </c>
       <c r="B35" s="259" t="s">
-        <v>1251</v>
+        <v>1247</v>
       </c>
       <c r="C35" s="249" t="s">
-        <v>1252</v>
+        <v>1248</v>
       </c>
       <c r="D35" s="249"/>
       <c r="E35" s="260"/>
     </row>
     <row r="36">
       <c r="A36" s="241" t="s">
-        <v>1253</v>
+        <v>1249</v>
       </c>
       <c r="B36" s="259" t="s">
-        <v>1254</v>
+        <v>1250</v>
       </c>
       <c r="C36" s="249" t="s">
-        <v>1255</v>
+        <v>1251</v>
       </c>
       <c r="D36" s="249"/>
       <c r="E36" s="260"/>
     </row>
     <row r="37">
       <c r="A37" s="241" t="s">
-        <v>1256</v>
+        <v>1252</v>
       </c>
       <c r="B37" s="259" t="s">
-        <v>1257</v>
+        <v>1253</v>
       </c>
       <c r="C37" s="249" t="s">
-        <v>1258</v>
+        <v>1254</v>
       </c>
       <c r="D37" s="249"/>
       <c r="E37" s="260"/>
     </row>
     <row r="38">
       <c r="A38" s="241" t="s">
-        <v>1259</v>
+        <v>1255</v>
       </c>
       <c r="B38" s="259" t="s">
-        <v>1260</v>
+        <v>1256</v>
       </c>
       <c r="C38" s="249" t="s">
-        <v>1261</v>
+        <v>1257</v>
       </c>
       <c r="D38" s="249"/>
       <c r="E38" s="260"/>
     </row>
     <row r="39">
       <c r="A39" s="241" t="s">
-        <v>1262</v>
+        <v>1258</v>
       </c>
       <c r="B39" s="261" t="s">
-        <v>1263</v>
+        <v>1259</v>
       </c>
       <c r="C39" s="257" t="s">
-        <v>1264</v>
+        <v>1260</v>
       </c>
       <c r="D39" s="257"/>
       <c r="E39" s="262"/>
@@ -17607,13 +17531,13 @@
     </row>
     <row r="40">
       <c r="A40" s="241" t="s">
-        <v>1265</v>
+        <v>1261</v>
       </c>
       <c r="B40" s="261" t="s">
-        <v>1266</v>
+        <v>1262</v>
       </c>
       <c r="C40" s="257" t="s">
-        <v>1267</v>
+        <v>1263</v>
       </c>
       <c r="D40" s="257"/>
       <c r="E40" s="263"/>
@@ -17621,13 +17545,13 @@
     </row>
     <row r="41">
       <c r="A41" s="241" t="s">
-        <v>1268</v>
+        <v>1264</v>
       </c>
       <c r="B41" s="261" t="s">
-        <v>1269</v>
+        <v>1265</v>
       </c>
       <c r="C41" s="257" t="s">
-        <v>1270</v>
+        <v>1266</v>
       </c>
       <c r="D41" s="257"/>
       <c r="E41" s="262"/>
@@ -17635,13 +17559,13 @@
     </row>
     <row r="42">
       <c r="A42" s="241" t="s">
-        <v>1271</v>
+        <v>1267</v>
       </c>
       <c r="B42" s="261" t="s">
-        <v>1166</v>
+        <v>1162</v>
       </c>
       <c r="C42" s="264" t="s">
-        <v>1272</v>
+        <v>1268</v>
       </c>
       <c r="D42" s="264"/>
       <c r="E42" s="245"/>
@@ -17649,13 +17573,13 @@
     </row>
     <row r="43">
       <c r="A43" s="241" t="s">
-        <v>1273</v>
+        <v>1269</v>
       </c>
       <c r="B43" s="265" t="s">
-        <v>1274</v>
+        <v>1270</v>
       </c>
       <c r="C43" s="264" t="s">
-        <v>1275</v>
+        <v>1271</v>
       </c>
       <c r="D43" s="264"/>
       <c r="E43" s="245"/>
@@ -17663,13 +17587,13 @@
     </row>
     <row r="44">
       <c r="A44" s="241" t="s">
-        <v>1276</v>
+        <v>1272</v>
       </c>
       <c r="B44" s="265" t="s">
-        <v>1277</v>
+        <v>1273</v>
       </c>
       <c r="C44" s="266" t="s">
-        <v>1278</v>
+        <v>1274</v>
       </c>
       <c r="D44" s="266"/>
       <c r="E44" s="245"/>
@@ -17677,10 +17601,10 @@
     </row>
     <row r="45" ht="20.25" customHeight="1">
       <c r="A45" s="241" t="s">
-        <v>1279</v>
+        <v>1275</v>
       </c>
       <c r="B45" s="14" t="s">
-        <v>1280</v>
+        <v>1276</v>
       </c>
       <c r="C45" s="267" t="s">
         <v>311</v>
@@ -17691,10 +17615,10 @@
     </row>
     <row r="46">
       <c r="A46" s="241" t="s">
-        <v>1281</v>
+        <v>1277</v>
       </c>
       <c r="B46" s="14" t="s">
-        <v>1282</v>
+        <v>1278</v>
       </c>
       <c r="C46" s="15" t="s">
         <v>315</v>
@@ -17705,10 +17629,10 @@
     </row>
     <row r="47">
       <c r="A47" s="241" t="s">
-        <v>1283</v>
+        <v>1279</v>
       </c>
       <c r="B47" s="14" t="s">
-        <v>1284</v>
+        <v>1280</v>
       </c>
       <c r="C47" s="244" t="s">
         <v>318</v>
@@ -17719,10 +17643,10 @@
     </row>
     <row r="48">
       <c r="A48" s="241" t="s">
-        <v>1285</v>
+        <v>1281</v>
       </c>
       <c r="B48" s="14" t="s">
-        <v>1286</v>
+        <v>1282</v>
       </c>
       <c r="C48" s="244" t="s">
         <v>321</v>
@@ -17733,10 +17657,10 @@
     </row>
     <row r="49">
       <c r="A49" s="241" t="s">
-        <v>1287</v>
+        <v>1283</v>
       </c>
       <c r="B49" s="14" t="s">
-        <v>1288</v>
+        <v>1284</v>
       </c>
       <c r="C49" s="152" t="s">
         <v>325</v>
@@ -17747,10 +17671,10 @@
     </row>
     <row r="50">
       <c r="A50" s="241" t="s">
-        <v>1289</v>
+        <v>1285</v>
       </c>
       <c r="B50" s="14" t="s">
-        <v>1290</v>
+        <v>1286</v>
       </c>
       <c r="C50" s="152" t="s">
         <v>328</v>
@@ -17761,10 +17685,10 @@
     </row>
     <row r="51">
       <c r="A51" s="241" t="s">
-        <v>1291</v>
+        <v>1287</v>
       </c>
       <c r="B51" s="14" t="s">
-        <v>1292</v>
+        <v>1288</v>
       </c>
       <c r="C51" s="244" t="s">
         <v>331</v>
@@ -17775,10 +17699,10 @@
     </row>
     <row r="52">
       <c r="A52" s="241" t="s">
-        <v>1293</v>
+        <v>1289</v>
       </c>
       <c r="B52" s="14" t="s">
-        <v>1294</v>
+        <v>1290</v>
       </c>
       <c r="C52" s="152" t="s">
         <v>334</v>
@@ -17789,10 +17713,10 @@
     </row>
     <row r="53">
       <c r="A53" s="241" t="s">
-        <v>1295</v>
+        <v>1291</v>
       </c>
       <c r="B53" s="14" t="s">
-        <v>1296</v>
+        <v>1292</v>
       </c>
       <c r="C53" s="244" t="s">
         <v>337</v>
@@ -17803,10 +17727,10 @@
     </row>
     <row r="54">
       <c r="A54" s="268" t="s">
-        <v>1297</v>
+        <v>1293</v>
       </c>
       <c r="B54" s="269" t="s">
-        <v>1298</v>
+        <v>1294</v>
       </c>
       <c r="C54" s="270" t="s">
         <v>340</v>
@@ -17817,13 +17741,13 @@
     </row>
     <row r="55">
       <c r="A55" s="241" t="s">
-        <v>1299</v>
+        <v>1295</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>1300</v>
+        <v>1296</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>1301</v>
+        <v>1297</v>
       </c>
       <c r="D55" s="5"/>
       <c r="E55" s="16"/>
@@ -17831,13 +17755,13 @@
     </row>
     <row r="56">
       <c r="A56" s="241" t="s">
-        <v>1302</v>
+        <v>1298</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>1303</v>
+        <v>1299</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>1304</v>
+        <v>1300</v>
       </c>
       <c r="D56" s="5"/>
       <c r="E56" s="16"/>
@@ -17873,13 +17797,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>1305</v>
+        <v>1301</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>1306</v>
+        <v>1302</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>1307</v>
+        <v>1303</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>12</v>
@@ -17890,13 +17814,13 @@
     </row>
     <row r="2">
       <c r="A2" s="20" t="s">
-        <v>1308</v>
+        <v>1304</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>1309</v>
+        <v>1305</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>1310</v>
+        <v>1306</v>
       </c>
       <c r="E2" s="20" t="s">
         <v>272</v>
@@ -17906,7 +17830,7 @@
     </row>
     <row r="3">
       <c r="A3" s="20" t="s">
-        <v>1311</v>
+        <v>1307</v>
       </c>
       <c r="C3" s="14" t="s">
         <v>510</v>
@@ -17922,7 +17846,7 @@
     </row>
     <row r="4">
       <c r="A4" s="20" t="s">
-        <v>1312</v>
+        <v>1308</v>
       </c>
       <c r="C4" s="14" t="s">
         <v>519</v>
@@ -17938,7 +17862,7 @@
     </row>
     <row r="5">
       <c r="A5" s="20" t="s">
-        <v>1313</v>
+        <v>1309</v>
       </c>
       <c r="B5" s="16"/>
       <c r="C5" s="14" t="s">
@@ -17955,7 +17879,7 @@
     </row>
     <row r="6">
       <c r="A6" s="20" t="s">
-        <v>1314</v>
+        <v>1310</v>
       </c>
       <c r="B6" s="16"/>
       <c r="C6" s="14" t="s">
@@ -17972,7 +17896,7 @@
     </row>
     <row r="7">
       <c r="A7" s="20" t="s">
-        <v>1315</v>
+        <v>1311</v>
       </c>
       <c r="B7" s="16"/>
       <c r="C7" s="14" t="s">
@@ -17989,7 +17913,7 @@
     </row>
     <row r="8">
       <c r="A8" s="20" t="s">
-        <v>1316</v>
+        <v>1312</v>
       </c>
       <c r="B8" s="16"/>
       <c r="C8" s="14" t="s">
@@ -18006,7 +17930,7 @@
     </row>
     <row r="9">
       <c r="A9" s="20" t="s">
-        <v>1317</v>
+        <v>1313</v>
       </c>
       <c r="B9" s="16"/>
       <c r="C9" s="14" t="s">
@@ -18023,7 +17947,7 @@
     </row>
     <row r="10">
       <c r="A10" s="20" t="s">
-        <v>1318</v>
+        <v>1314</v>
       </c>
       <c r="B10" s="16"/>
       <c r="C10" s="14" t="s">
@@ -18040,7 +17964,7 @@
     </row>
     <row r="11">
       <c r="A11" s="20" t="s">
-        <v>1319</v>
+        <v>1315</v>
       </c>
       <c r="B11" s="16"/>
       <c r="C11" s="14" t="s">
@@ -18057,7 +17981,7 @@
     </row>
     <row r="12">
       <c r="A12" s="20" t="s">
-        <v>1320</v>
+        <v>1316</v>
       </c>
       <c r="B12" s="16"/>
       <c r="C12" s="14" t="s">
@@ -18074,7 +17998,7 @@
     </row>
     <row r="13">
       <c r="A13" s="20" t="s">
-        <v>1321</v>
+        <v>1317</v>
       </c>
       <c r="B13" s="16"/>
       <c r="C13" s="14" t="s">
@@ -18091,7 +18015,7 @@
     </row>
     <row r="14">
       <c r="A14" s="66" t="s">
-        <v>1322</v>
+        <v>1318</v>
       </c>
       <c r="B14" s="64"/>
       <c r="C14" s="62" t="s">
@@ -18108,7 +18032,7 @@
     </row>
     <row r="15">
       <c r="A15" s="66" t="s">
-        <v>1323</v>
+        <v>1319</v>
       </c>
       <c r="B15" s="64"/>
       <c r="C15" s="62" t="s">
@@ -18125,7 +18049,7 @@
     </row>
     <row r="16">
       <c r="A16" s="66" t="s">
-        <v>1324</v>
+        <v>1320</v>
       </c>
       <c r="B16" s="64"/>
       <c r="C16" s="62" t="s">
@@ -18142,7 +18066,7 @@
     </row>
     <row r="17">
       <c r="A17" s="66" t="s">
-        <v>1325</v>
+        <v>1321</v>
       </c>
       <c r="B17" s="64"/>
       <c r="C17" s="62" t="s">
@@ -18159,7 +18083,7 @@
     </row>
     <row r="18">
       <c r="A18" s="66" t="s">
-        <v>1326</v>
+        <v>1322</v>
       </c>
       <c r="B18" s="64"/>
       <c r="C18" s="62" t="s">
@@ -18176,7 +18100,7 @@
     </row>
     <row r="19">
       <c r="A19" s="66" t="s">
-        <v>1327</v>
+        <v>1323</v>
       </c>
       <c r="B19" s="64"/>
       <c r="C19" s="62" t="s">
@@ -18193,7 +18117,7 @@
     </row>
     <row r="20">
       <c r="A20" s="20" t="s">
-        <v>1328</v>
+        <v>1324</v>
       </c>
       <c r="B20" s="16"/>
       <c r="C20" s="14" t="s">
@@ -18210,7 +18134,7 @@
     </row>
     <row r="21">
       <c r="A21" s="20" t="s">
-        <v>1329</v>
+        <v>1325</v>
       </c>
       <c r="B21" s="16"/>
       <c r="C21" s="14" t="s">
@@ -18227,7 +18151,7 @@
     </row>
     <row r="22">
       <c r="A22" s="20" t="s">
-        <v>1330</v>
+        <v>1326</v>
       </c>
       <c r="B22" s="16"/>
       <c r="C22" s="14" t="s">
@@ -18244,7 +18168,7 @@
     </row>
     <row r="23">
       <c r="A23" s="20" t="s">
-        <v>1331</v>
+        <v>1327</v>
       </c>
       <c r="B23" s="16"/>
       <c r="C23" s="14" t="s">
@@ -18261,7 +18185,7 @@
     </row>
     <row r="24">
       <c r="A24" s="20" t="s">
-        <v>1332</v>
+        <v>1328</v>
       </c>
       <c r="B24" s="16"/>
       <c r="C24" s="14" t="s">
@@ -18278,7 +18202,7 @@
     </row>
     <row r="25">
       <c r="A25" s="20" t="s">
-        <v>1333</v>
+        <v>1329</v>
       </c>
       <c r="B25" s="16"/>
       <c r="C25" s="14" t="s">
@@ -18295,7 +18219,7 @@
     </row>
     <row r="26">
       <c r="A26" s="20" t="s">
-        <v>1334</v>
+        <v>1330</v>
       </c>
       <c r="B26" s="16"/>
       <c r="C26" s="14" t="s">
@@ -18312,7 +18236,7 @@
     </row>
     <row r="27">
       <c r="A27" s="20" t="s">
-        <v>1335</v>
+        <v>1331</v>
       </c>
       <c r="B27" s="16"/>
       <c r="C27" s="14" t="s">
@@ -18329,7 +18253,7 @@
     </row>
     <row r="28">
       <c r="A28" s="20" t="s">
-        <v>1336</v>
+        <v>1332</v>
       </c>
       <c r="B28" s="16"/>
       <c r="C28" s="14" t="s">
@@ -18346,7 +18270,7 @@
     </row>
     <row r="29">
       <c r="A29" s="20" t="s">
-        <v>1337</v>
+        <v>1333</v>
       </c>
       <c r="B29" s="16"/>
       <c r="C29" s="14" t="s">
@@ -18363,7 +18287,7 @@
     </row>
     <row r="30">
       <c r="A30" s="20" t="s">
-        <v>1338</v>
+        <v>1334</v>
       </c>
       <c r="B30" s="16"/>
       <c r="C30" s="14" t="s">
@@ -18380,7 +18304,7 @@
     </row>
     <row r="31">
       <c r="A31" s="20" t="s">
-        <v>1339</v>
+        <v>1335</v>
       </c>
       <c r="B31" s="16"/>
       <c r="C31" s="14" t="s">
@@ -18397,7 +18321,7 @@
     </row>
     <row r="32">
       <c r="A32" s="20" t="s">
-        <v>1340</v>
+        <v>1336</v>
       </c>
       <c r="B32" s="16"/>
       <c r="C32" s="14" t="s">
@@ -18414,14 +18338,14 @@
     </row>
     <row r="33">
       <c r="A33" s="20" t="s">
-        <v>1341</v>
+        <v>1337</v>
       </c>
       <c r="B33" s="16"/>
       <c r="C33" s="14" t="s">
+        <v>1008</v>
+      </c>
+      <c r="D33" s="14" t="s">
         <v>1012</v>
-      </c>
-      <c r="D33" s="14" t="s">
-        <v>1016</v>
       </c>
       <c r="E33" s="20" t="s">
         <v>441</v>
@@ -18431,14 +18355,14 @@
     </row>
     <row r="34">
       <c r="A34" s="20" t="s">
-        <v>1342</v>
+        <v>1338</v>
       </c>
       <c r="B34" s="16"/>
       <c r="C34" s="14" t="s">
-        <v>1020</v>
+        <v>1016</v>
       </c>
       <c r="D34" s="14" t="s">
-        <v>1023</v>
+        <v>1019</v>
       </c>
       <c r="E34" s="20" t="s">
         <v>444</v>
@@ -18448,14 +18372,14 @@
     </row>
     <row r="35">
       <c r="A35" s="20" t="s">
-        <v>1343</v>
+        <v>1339</v>
       </c>
       <c r="B35" s="16"/>
       <c r="C35" s="14" t="s">
-        <v>1035</v>
+        <v>1031</v>
       </c>
       <c r="D35" s="14" t="s">
-        <v>1040</v>
+        <v>1036</v>
       </c>
       <c r="E35" s="20" t="s">
         <v>94</v>
@@ -18465,14 +18389,14 @@
     </row>
     <row r="36">
       <c r="A36" s="20" t="s">
-        <v>1344</v>
+        <v>1340</v>
       </c>
       <c r="B36" s="16"/>
       <c r="C36" s="14" t="s">
+        <v>1042</v>
+      </c>
+      <c r="D36" s="14" t="s">
         <v>1046</v>
-      </c>
-      <c r="D36" s="14" t="s">
-        <v>1050</v>
       </c>
       <c r="E36" s="20" t="s">
         <v>99</v>
@@ -18482,14 +18406,14 @@
     </row>
     <row r="37">
       <c r="A37" s="20" t="s">
-        <v>1345</v>
+        <v>1341</v>
       </c>
       <c r="B37" s="16"/>
       <c r="C37" s="14" t="s">
+        <v>1052</v>
+      </c>
+      <c r="D37" s="14" t="s">
         <v>1056</v>
-      </c>
-      <c r="D37" s="14" t="s">
-        <v>1060</v>
       </c>
       <c r="E37" s="20" t="s">
         <v>103</v>
@@ -18499,14 +18423,14 @@
     </row>
     <row r="38">
       <c r="A38" s="20" t="s">
-        <v>1346</v>
+        <v>1342</v>
       </c>
       <c r="B38" s="16"/>
       <c r="C38" s="14" t="s">
+        <v>1061</v>
+      </c>
+      <c r="D38" s="14" t="s">
         <v>1065</v>
-      </c>
-      <c r="D38" s="14" t="s">
-        <v>1069</v>
       </c>
       <c r="E38" s="20" t="s">
         <v>107</v>
@@ -18516,14 +18440,14 @@
     </row>
     <row r="39">
       <c r="A39" s="20" t="s">
-        <v>1347</v>
+        <v>1343</v>
       </c>
       <c r="B39" s="16"/>
       <c r="C39" s="14" t="s">
+        <v>1070</v>
+      </c>
+      <c r="D39" s="14" t="s">
         <v>1074</v>
-      </c>
-      <c r="D39" s="14" t="s">
-        <v>1078</v>
       </c>
       <c r="E39" s="20" t="s">
         <v>111</v>
@@ -18533,14 +18457,14 @@
     </row>
     <row r="40">
       <c r="A40" s="20" t="s">
-        <v>1348</v>
+        <v>1344</v>
       </c>
       <c r="B40" s="16"/>
       <c r="C40" s="14" t="s">
+        <v>1079</v>
+      </c>
+      <c r="D40" s="14" t="s">
         <v>1083</v>
-      </c>
-      <c r="D40" s="14" t="s">
-        <v>1087</v>
       </c>
       <c r="E40" s="20" t="s">
         <v>115</v>
@@ -18550,14 +18474,14 @@
     </row>
     <row r="41">
       <c r="A41" s="20" t="s">
-        <v>1349</v>
+        <v>1345</v>
       </c>
       <c r="B41" s="16"/>
       <c r="C41" s="14" t="s">
+        <v>1088</v>
+      </c>
+      <c r="D41" s="14" t="s">
         <v>1092</v>
-      </c>
-      <c r="D41" s="14" t="s">
-        <v>1096</v>
       </c>
       <c r="E41" s="20" t="s">
         <v>119</v>
@@ -18567,14 +18491,14 @@
     </row>
     <row r="42">
       <c r="A42" s="20" t="s">
-        <v>1350</v>
+        <v>1346</v>
       </c>
       <c r="B42" s="16"/>
       <c r="C42" s="14" t="s">
+        <v>1097</v>
+      </c>
+      <c r="D42" s="14" t="s">
         <v>1101</v>
-      </c>
-      <c r="D42" s="14" t="s">
-        <v>1105</v>
       </c>
       <c r="E42" s="20" t="s">
         <v>123</v>
@@ -18584,14 +18508,14 @@
     </row>
     <row r="43">
       <c r="A43" s="20" t="s">
-        <v>1351</v>
+        <v>1347</v>
       </c>
       <c r="B43" s="16"/>
       <c r="C43" s="14" t="s">
+        <v>1106</v>
+      </c>
+      <c r="D43" s="14" t="s">
         <v>1110</v>
-      </c>
-      <c r="D43" s="14" t="s">
-        <v>1114</v>
       </c>
       <c r="E43" s="20" t="s">
         <v>127</v>
@@ -18601,14 +18525,14 @@
     </row>
     <row r="44">
       <c r="A44" s="20" t="s">
-        <v>1352</v>
+        <v>1348</v>
       </c>
       <c r="B44" s="16"/>
       <c r="C44" s="14" t="s">
+        <v>1125</v>
+      </c>
+      <c r="D44" s="14" t="s">
         <v>1129</v>
-      </c>
-      <c r="D44" s="14" t="s">
-        <v>1133</v>
       </c>
       <c r="E44" s="20" t="s">
         <v>477</v>
@@ -18618,14 +18542,14 @@
     </row>
     <row r="45">
       <c r="A45" s="20" t="s">
-        <v>1353</v>
+        <v>1349</v>
       </c>
       <c r="B45" s="16"/>
       <c r="C45" s="14" t="s">
+        <v>1138</v>
+      </c>
+      <c r="D45" s="14" t="s">
         <v>1142</v>
-      </c>
-      <c r="D45" s="14" t="s">
-        <v>1146</v>
       </c>
       <c r="E45" s="20" t="s">
         <v>480</v>
@@ -18665,10 +18589,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>1354</v>
+        <v>1350</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>1355</v>
+        <v>1351</v>
       </c>
     </row>
     <row r="2">
@@ -18678,7 +18602,7 @@
       <c r="B2" s="16"/>
       <c r="C2" s="16"/>
       <c r="D2" s="16" t="s">
-        <v>1356</v>
+        <v>1352</v>
       </c>
       <c r="E2" s="16"/>
       <c r="F2" s="16"/>
@@ -18690,7 +18614,7 @@
       <c r="B3" s="16"/>
       <c r="C3" s="16"/>
       <c r="D3" s="16" t="s">
-        <v>1357</v>
+        <v>1353</v>
       </c>
       <c r="E3" s="16"/>
       <c r="F3" s="16"/>
@@ -18737,22 +18661,22 @@
         <v>491</v>
       </c>
       <c r="E1" s="274" t="s">
-        <v>1358</v>
+        <v>1354</v>
       </c>
       <c r="F1" s="274" t="s">
-        <v>1359</v>
+        <v>1355</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>1360</v>
+        <v>1356</v>
       </c>
       <c r="H1" s="275" t="s">
         <v>500</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>1361</v>
+        <v>1357</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>1362</v>
+        <v>1358</v>
       </c>
     </row>
     <row r="2">
@@ -18760,16 +18684,16 @@
         <v>384</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>1363</v>
+        <v>1359</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>1364</v>
+        <v>1360</v>
       </c>
       <c r="D2" s="276"/>
       <c r="F2" s="275"/>
       <c r="H2" s="277"/>
       <c r="J2" s="5" t="s">
-        <v>1365</v>
+        <v>1361</v>
       </c>
     </row>
     <row r="3">
@@ -18777,17 +18701,17 @@
         <v>387</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>1366</v>
+        <v>1362</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>1367</v>
+        <v>1363</v>
       </c>
       <c r="D3" s="277"/>
       <c r="E3" s="275"/>
       <c r="F3" s="275"/>
       <c r="H3" s="275"/>
       <c r="J3" s="5" t="s">
-        <v>1368</v>
+        <v>1364</v>
       </c>
     </row>
     <row r="4">
@@ -18795,17 +18719,17 @@
         <v>390</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>1369</v>
+        <v>1365</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>1370</v>
+        <v>1366</v>
       </c>
       <c r="D4" s="277"/>
       <c r="E4" s="275"/>
       <c r="F4" s="275"/>
       <c r="H4" s="275"/>
       <c r="J4" s="5" t="s">
-        <v>1368</v>
+        <v>1364</v>
       </c>
     </row>
     <row r="5">
@@ -18813,17 +18737,17 @@
         <v>392</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>1371</v>
+        <v>1367</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>1372</v>
+        <v>1368</v>
       </c>
       <c r="D5" s="275"/>
       <c r="E5" s="275"/>
       <c r="F5" s="275"/>
       <c r="H5" s="277"/>
       <c r="J5" s="5" t="s">
-        <v>1373</v>
+        <v>1369</v>
       </c>
     </row>
     <row r="6">
@@ -18831,10 +18755,10 @@
         <v>396</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>1374</v>
+        <v>1370</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>1375</v>
+        <v>1371</v>
       </c>
       <c r="D6" s="275"/>
       <c r="E6" s="123"/>
@@ -18843,7 +18767,7 @@
         <v>487</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>1376</v>
+        <v>1372</v>
       </c>
     </row>
     <row r="7">
@@ -18851,17 +18775,17 @@
         <v>403</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>1377</v>
+        <v>1373</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>1378</v>
+        <v>1374</v>
       </c>
       <c r="D7" s="275"/>
       <c r="E7" s="275"/>
       <c r="F7" s="275"/>
       <c r="H7" s="275"/>
       <c r="J7" s="5" t="s">
-        <v>1379</v>
+        <v>1375</v>
       </c>
     </row>
     <row r="8">
@@ -18869,10 +18793,10 @@
         <v>417</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>1380</v>
+        <v>1376</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>1381</v>
+        <v>1377</v>
       </c>
       <c r="D8" s="275"/>
       <c r="E8" s="275"/>
@@ -18880,7 +18804,7 @@
       <c r="G8" s="275"/>
       <c r="H8" s="275"/>
       <c r="J8" s="5" t="s">
-        <v>1382</v>
+        <v>1378</v>
       </c>
     </row>
     <row r="9">
@@ -18888,17 +18812,17 @@
         <v>423</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>1383</v>
+        <v>1379</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>1384</v>
+        <v>1380</v>
       </c>
       <c r="D9" s="275"/>
       <c r="E9" s="275"/>
       <c r="F9" s="275"/>
       <c r="H9" s="275"/>
       <c r="J9" s="5" t="s">
-        <v>1379</v>
+        <v>1375</v>
       </c>
     </row>
     <row r="10">
@@ -18906,17 +18830,17 @@
         <v>429</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>1385</v>
+        <v>1381</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>1386</v>
+        <v>1382</v>
       </c>
       <c r="D10" s="275"/>
       <c r="E10" s="275"/>
       <c r="F10" s="275"/>
       <c r="H10" s="277"/>
       <c r="J10" s="5" t="s">
-        <v>1387</v>
+        <v>1383</v>
       </c>
     </row>
     <row r="11">
@@ -18924,10 +18848,10 @@
         <v>435</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>1388</v>
+        <v>1384</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>1389</v>
+        <v>1385</v>
       </c>
       <c r="D11" s="275"/>
       <c r="E11" s="275"/>
@@ -18935,7 +18859,7 @@
       <c r="G11" s="275"/>
       <c r="H11" s="275"/>
       <c r="J11" s="14" t="s">
-        <v>1368</v>
+        <v>1364</v>
       </c>
     </row>
     <row r="12">
@@ -18943,10 +18867,10 @@
         <v>420</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>1390</v>
+        <v>1386</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>1391</v>
+        <v>1387</v>
       </c>
       <c r="D12" s="275"/>
       <c r="E12" s="275"/>
@@ -18954,7 +18878,7 @@
       <c r="G12" s="275"/>
       <c r="H12" s="275"/>
       <c r="J12" s="5" t="s">
-        <v>1382</v>
+        <v>1378</v>
       </c>
     </row>
     <row r="13">
@@ -18962,17 +18886,17 @@
         <v>426</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>1392</v>
+        <v>1388</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>1393</v>
+        <v>1389</v>
       </c>
       <c r="D13" s="275"/>
       <c r="E13" s="275"/>
       <c r="F13" s="275"/>
       <c r="H13" s="275"/>
       <c r="J13" s="5" t="s">
-        <v>1379</v>
+        <v>1375</v>
       </c>
     </row>
     <row r="14">
@@ -18980,17 +18904,17 @@
         <v>432</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>1394</v>
+        <v>1390</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>1395</v>
+        <v>1391</v>
       </c>
       <c r="D14" s="275"/>
       <c r="E14" s="275"/>
       <c r="F14" s="275"/>
       <c r="H14" s="277"/>
       <c r="J14" s="5" t="s">
-        <v>1387</v>
+        <v>1383</v>
       </c>
     </row>
     <row r="15">
@@ -18998,10 +18922,10 @@
         <v>438</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>1396</v>
+        <v>1392</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>1397</v>
+        <v>1393</v>
       </c>
       <c r="D15" s="275"/>
       <c r="E15" s="275"/>
@@ -19009,7 +18933,7 @@
       <c r="G15" s="275"/>
       <c r="H15" s="275"/>
       <c r="J15" s="14" t="s">
-        <v>1368</v>
+        <v>1364</v>
       </c>
     </row>
     <row r="16">
@@ -19017,10 +18941,10 @@
         <v>440</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>1398</v>
+        <v>1394</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>1399</v>
+        <v>1395</v>
       </c>
       <c r="D16" s="277"/>
       <c r="E16" s="275"/>
@@ -19029,7 +18953,7 @@
         <v>487</v>
       </c>
       <c r="J16" s="279" t="s">
-        <v>1387</v>
+        <v>1383</v>
       </c>
     </row>
     <row r="17">
@@ -19037,18 +18961,18 @@
         <v>443</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>1400</v>
+        <v>1396</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>1401</v>
+        <v>1397</v>
       </c>
       <c r="E17" s="275"/>
       <c r="F17" s="280"/>
       <c r="H17" s="5" t="s">
-        <v>1402</v>
+        <v>1398</v>
       </c>
       <c r="J17" s="279" t="s">
-        <v>1387</v>
+        <v>1383</v>
       </c>
     </row>
     <row r="18">
@@ -19056,10 +18980,10 @@
         <v>447</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>1403</v>
+        <v>1399</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>1404</v>
+        <v>1400</v>
       </c>
       <c r="E18" s="275"/>
       <c r="F18" s="280"/>
@@ -19067,7 +18991,7 @@
         <v>487</v>
       </c>
       <c r="J18" s="279" t="s">
-        <v>1387</v>
+        <v>1383</v>
       </c>
     </row>
     <row r="19">
@@ -19075,16 +18999,16 @@
         <v>479</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>1405</v>
+        <v>1401</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>1406</v>
+        <v>1402</v>
       </c>
       <c r="E19" s="275"/>
       <c r="F19" s="280"/>
       <c r="H19" s="5"/>
       <c r="J19" s="279" t="s">
-        <v>1382</v>
+        <v>1378</v>
       </c>
     </row>
     <row r="20">
@@ -19092,16 +19016,16 @@
         <v>482</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>1407</v>
+        <v>1403</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>1408</v>
+        <v>1404</v>
       </c>
       <c r="E20" s="275"/>
       <c r="F20" s="280"/>
       <c r="H20" s="5"/>
       <c r="J20" s="5" t="s">
-        <v>1379</v>
+        <v>1375</v>
       </c>
     </row>
   </sheetData>
@@ -19131,66 +19055,66 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>1409</v>
+        <v>1405</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="281" t="s">
-        <v>1410</v>
+        <v>1406</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>1411</v>
+        <v>1407</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>1412</v>
+        <v>1408</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="281" t="s">
-        <v>1413</v>
+        <v>1409</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>1414</v>
+        <v>1410</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>1412</v>
+        <v>1408</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="281" t="s">
-        <v>1415</v>
+        <v>1411</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>1416</v>
+        <v>1412</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>1412</v>
+        <v>1408</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" s="5" t="s">
-        <v>1417</v>
+        <v>1413</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>1412</v>
+        <v>1408</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="5"/>
       <c r="B6" s="282" t="s">
-        <v>1418</v>
+        <v>1414</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>1419</v>
+        <v>1415</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="5"/>
       <c r="B7" s="282" t="s">
-        <v>1420</v>
+        <v>1416</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>1419</v>
+        <v>1415</v>
       </c>
     </row>
   </sheetData>

</xml_diff>